<commit_message>
Add the precision and unit exchange on Dashboard
</commit_message>
<xml_diff>
--- a/JM4000MODBUS_V1.0_May 31, 2025.xlsx
+++ b/JM4000MODBUS_V1.0_May 31, 2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerryw.wang\Documents\MeteringDisplay\RK3588\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA648060-9B6E-448B-97D9-E69D2A5A0E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C8F7F7-5CDE-4514-9090-7E021B59AC49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{3C7CDEC9-8383-43D7-977D-6ADA3FE6D97E}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{3C7CDEC9-8383-43D7-977D-6ADA3FE6D97E}"/>
   </bookViews>
   <sheets>
     <sheet name="参数列表" sheetId="1" r:id="rId1"/>
@@ -6407,6 +6407,15 @@
     <xf numFmtId="49" fontId="24" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -6445,15 +6454,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6855,41 +6855,41 @@
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="172"/>
-      <c r="C1" s="173"/>
-      <c r="D1" s="174"/>
-      <c r="E1" s="174"/>
-      <c r="F1" s="173"/>
-      <c r="G1" s="173"/>
-      <c r="H1" s="173"/>
-      <c r="I1" s="175"/>
+      <c r="B1" s="175"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
+      <c r="H1" s="176"/>
+      <c r="I1" s="178"/>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="176" t="s">
+      <c r="A2" s="179" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="177"/>
-      <c r="C2" s="177"/>
-      <c r="D2" s="178"/>
-      <c r="E2" s="178"/>
-      <c r="F2" s="177"/>
-      <c r="G2" s="177"/>
-      <c r="H2" s="177"/>
-      <c r="I2" s="177"/>
-      <c r="J2" s="177"/>
-      <c r="K2" s="177"/>
-      <c r="L2" s="177"/>
-      <c r="M2" s="177"/>
+      <c r="B2" s="180"/>
+      <c r="C2" s="180"/>
+      <c r="D2" s="181"/>
+      <c r="E2" s="181"/>
+      <c r="F2" s="180"/>
+      <c r="G2" s="180"/>
+      <c r="H2" s="180"/>
+      <c r="I2" s="180"/>
+      <c r="J2" s="180"/>
+      <c r="K2" s="180"/>
+      <c r="L2" s="180"/>
+      <c r="M2" s="180"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
-      <c r="B3" s="179" t="s">
+      <c r="B3" s="182" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="179"/>
-      <c r="D3" s="179"/>
-      <c r="E3" s="179"/>
-      <c r="F3" s="179"/>
+      <c r="C3" s="182"/>
+      <c r="D3" s="182"/>
+      <c r="E3" s="182"/>
+      <c r="F3" s="182"/>
       <c r="G3" s="77"/>
       <c r="H3"/>
       <c r="I3" s="24"/>
@@ -6938,10 +6938,10 @@
       </c>
     </row>
     <row r="5" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="180" t="s">
+      <c r="A5" s="183" t="s">
         <v>340</v>
       </c>
-      <c r="B5" s="180" t="s">
+      <c r="B5" s="183" t="s">
         <v>339</v>
       </c>
       <c r="C5" s="69" t="s">
@@ -6966,8 +6966,8 @@
       </c>
     </row>
     <row r="6" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="181"/>
-      <c r="B6" s="181"/>
+      <c r="A6" s="184"/>
+      <c r="B6" s="184"/>
       <c r="C6" s="69" t="s">
         <v>348</v>
       </c>
@@ -6986,8 +6986,8 @@
       </c>
     </row>
     <row r="7" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="181"/>
-      <c r="B7" s="181"/>
+      <c r="A7" s="184"/>
+      <c r="B7" s="184"/>
       <c r="C7" s="69" t="s">
         <v>350</v>
       </c>
@@ -7006,8 +7006,8 @@
       </c>
     </row>
     <row r="8" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="181"/>
-      <c r="B8" s="181"/>
+      <c r="A8" s="184"/>
+      <c r="B8" s="184"/>
       <c r="C8" s="69" t="s">
         <v>349</v>
       </c>
@@ -7026,8 +7026,8 @@
       </c>
     </row>
     <row r="9" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="181"/>
-      <c r="B9" s="181"/>
+      <c r="A9" s="184"/>
+      <c r="B9" s="184"/>
       <c r="C9" s="69" t="s">
         <v>352</v>
       </c>
@@ -7046,8 +7046,8 @@
       </c>
     </row>
     <row r="10" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="181"/>
-      <c r="B10" s="181"/>
+      <c r="A10" s="184"/>
+      <c r="B10" s="184"/>
       <c r="C10" s="69" t="s">
         <v>363</v>
       </c>
@@ -7066,8 +7066,8 @@
       </c>
     </row>
     <row r="11" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="181"/>
-      <c r="B11" s="181"/>
+      <c r="A11" s="184"/>
+      <c r="B11" s="184"/>
       <c r="C11" s="69" t="s">
         <v>364</v>
       </c>
@@ -7086,8 +7086,8 @@
       </c>
     </row>
     <row r="12" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="182"/>
-      <c r="B12" s="182"/>
+      <c r="A12" s="185"/>
+      <c r="B12" s="185"/>
       <c r="C12" s="69" t="s">
         <v>365</v>
       </c>
@@ -7115,7 +7115,7 @@
       <c r="C13" s="69" t="s">
         <v>366</v>
       </c>
-      <c r="D13" s="185">
+      <c r="D13" s="172">
         <v>4</v>
       </c>
       <c r="E13" s="7" t="s">
@@ -7149,7 +7149,7 @@
       <c r="C14" s="69" t="s">
         <v>367</v>
       </c>
-      <c r="D14" s="186"/>
+      <c r="D14" s="174"/>
       <c r="F14" s="15"/>
       <c r="H14" s="14"/>
       <c r="I14" s="27"/>
@@ -7168,7 +7168,7 @@
       <c r="C15" s="69" t="s">
         <v>368</v>
       </c>
-      <c r="D15" s="185">
+      <c r="D15" s="172">
         <v>4</v>
       </c>
       <c r="E15" s="7" t="s">
@@ -7202,7 +7202,7 @@
       <c r="C16" s="69" t="s">
         <v>369</v>
       </c>
-      <c r="D16" s="186"/>
+      <c r="D16" s="174"/>
       <c r="F16" s="15"/>
       <c r="H16" s="14"/>
       <c r="I16" s="27"/>
@@ -7221,7 +7221,7 @@
       <c r="C17" s="69" t="s">
         <v>370</v>
       </c>
-      <c r="D17" s="185">
+      <c r="D17" s="172">
         <v>4</v>
       </c>
       <c r="E17" s="7" t="s">
@@ -7251,7 +7251,7 @@
       <c r="C18" s="69" t="s">
         <v>371</v>
       </c>
-      <c r="D18" s="186"/>
+      <c r="D18" s="174"/>
       <c r="F18" s="16"/>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
@@ -7270,7 +7270,7 @@
       <c r="C19" s="69" t="s">
         <v>372</v>
       </c>
-      <c r="D19" s="185">
+      <c r="D19" s="172">
         <v>4</v>
       </c>
       <c r="E19" s="7" t="s">
@@ -7303,7 +7303,7 @@
       <c r="C20" s="69" t="s">
         <v>373</v>
       </c>
-      <c r="D20" s="186"/>
+      <c r="D20" s="174"/>
       <c r="F20" s="16"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
@@ -7322,7 +7322,7 @@
       <c r="C21" s="69" t="s">
         <v>374</v>
       </c>
-      <c r="D21" s="185">
+      <c r="D21" s="172">
         <v>4</v>
       </c>
       <c r="E21" s="7" t="s">
@@ -7352,7 +7352,7 @@
       <c r="C22" s="69" t="s">
         <v>375</v>
       </c>
-      <c r="D22" s="186"/>
+      <c r="D22" s="174"/>
       <c r="F22" s="15"/>
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
@@ -7429,7 +7429,7 @@
       <c r="C25" s="69" t="s">
         <v>378</v>
       </c>
-      <c r="D25" s="185">
+      <c r="D25" s="172">
         <v>4</v>
       </c>
       <c r="E25" s="7" t="s">
@@ -7452,7 +7452,7 @@
       <c r="C26" s="69" t="s">
         <v>379</v>
       </c>
-      <c r="D26" s="187"/>
+      <c r="D26" s="173"/>
       <c r="F26" s="15"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -7465,7 +7465,7 @@
       <c r="C27" s="69" t="s">
         <v>380</v>
       </c>
-      <c r="D27" s="185">
+      <c r="D27" s="172">
         <v>4</v>
       </c>
       <c r="E27" s="7" t="s">
@@ -7489,7 +7489,7 @@
       <c r="C28" s="69" t="s">
         <v>381</v>
       </c>
-      <c r="D28" s="187"/>
+      <c r="D28" s="173"/>
       <c r="F28" s="15"/>
       <c r="H28" s="14"/>
       <c r="I28" s="27"/>
@@ -7508,7 +7508,7 @@
       <c r="C29" s="69" t="s">
         <v>382</v>
       </c>
-      <c r="D29" s="185">
+      <c r="D29" s="172">
         <v>4</v>
       </c>
       <c r="E29" s="7" t="s">
@@ -7532,7 +7532,7 @@
       <c r="C30" s="69" t="s">
         <v>383</v>
       </c>
-      <c r="D30" s="187"/>
+      <c r="D30" s="173"/>
       <c r="F30" s="15"/>
       <c r="H30" s="14"/>
       <c r="I30" s="27"/>
@@ -7542,16 +7542,16 @@
       <c r="M30" s="24"/>
     </row>
     <row r="31" spans="1:13" ht="92.4" x14ac:dyDescent="0.25">
-      <c r="A31" s="183" t="s">
+      <c r="A31" s="186" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="183" t="s">
+      <c r="B31" s="186" t="s">
         <v>40</v>
       </c>
       <c r="C31" s="69" t="s">
         <v>384</v>
       </c>
-      <c r="D31" s="185">
+      <c r="D31" s="172">
         <v>4</v>
       </c>
       <c r="E31" s="7" t="s">
@@ -7576,12 +7576,12 @@
       <c r="M31" s="14"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="184"/>
-      <c r="B32" s="184"/>
+      <c r="A32" s="187"/>
+      <c r="B32" s="187"/>
       <c r="C32" s="69" t="s">
         <v>385</v>
       </c>
-      <c r="D32" s="187"/>
+      <c r="D32" s="173"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
@@ -7622,7 +7622,7 @@
       <c r="C34" s="69" t="s">
         <v>387</v>
       </c>
-      <c r="D34" s="185">
+      <c r="D34" s="172">
         <v>4</v>
       </c>
       <c r="E34" s="7" t="s">
@@ -7659,7 +7659,7 @@
       <c r="C35" s="69" t="s">
         <v>388</v>
       </c>
-      <c r="D35" s="186"/>
+      <c r="D35" s="174"/>
       <c r="F35" s="20"/>
       <c r="H35" s="14"/>
       <c r="I35" s="27"/>
@@ -7678,7 +7678,7 @@
       <c r="C36" s="69" t="s">
         <v>389</v>
       </c>
-      <c r="D36" s="185">
+      <c r="D36" s="172">
         <v>4</v>
       </c>
       <c r="E36" s="7" t="s">
@@ -7712,7 +7712,7 @@
       <c r="C37" s="69" t="s">
         <v>390</v>
       </c>
-      <c r="D37" s="186"/>
+      <c r="D37" s="174"/>
       <c r="F37" s="21"/>
       <c r="H37" s="14"/>
       <c r="I37" s="27"/>
@@ -7731,7 +7731,7 @@
       <c r="C38" s="69" t="s">
         <v>391</v>
       </c>
-      <c r="D38" s="185">
+      <c r="D38" s="172">
         <v>4</v>
       </c>
       <c r="E38" s="7" t="s">
@@ -7764,7 +7764,7 @@
       <c r="C39" s="69" t="s">
         <v>392</v>
       </c>
-      <c r="D39" s="186"/>
+      <c r="D39" s="174"/>
       <c r="F39" s="20"/>
       <c r="H39" s="14"/>
       <c r="I39" s="14"/>
@@ -7783,7 +7783,7 @@
       <c r="C40" s="69" t="s">
         <v>393</v>
       </c>
-      <c r="D40" s="185">
+      <c r="D40" s="172">
         <v>4</v>
       </c>
       <c r="E40" s="7" t="s">
@@ -7816,7 +7816,7 @@
       <c r="C41" s="69" t="s">
         <v>394</v>
       </c>
-      <c r="D41" s="186"/>
+      <c r="D41" s="174"/>
       <c r="F41" s="21"/>
       <c r="H41" s="14"/>
       <c r="I41" s="14"/>
@@ -7835,7 +7835,7 @@
       <c r="C42" s="69" t="s">
         <v>395</v>
       </c>
-      <c r="D42" s="185">
+      <c r="D42" s="172">
         <v>4</v>
       </c>
       <c r="E42" s="7" t="s">
@@ -7865,7 +7865,7 @@
       <c r="C43" s="69" t="s">
         <v>396</v>
       </c>
-      <c r="D43" s="186"/>
+      <c r="D43" s="174"/>
       <c r="F43" s="19"/>
       <c r="H43" s="14"/>
       <c r="I43" s="14"/>
@@ -8017,7 +8017,7 @@
       <c r="C48" s="69" t="s">
         <v>401</v>
       </c>
-      <c r="D48" s="185">
+      <c r="D48" s="172">
         <v>4</v>
       </c>
       <c r="F48" s="15" t="s">
@@ -8046,7 +8046,7 @@
       <c r="C49" s="69" t="s">
         <v>402</v>
       </c>
-      <c r="D49" s="186"/>
+      <c r="D49" s="174"/>
       <c r="F49" s="16"/>
       <c r="H49" s="14"/>
       <c r="I49" s="14"/>
@@ -8065,7 +8065,7 @@
       <c r="C50" s="69" t="s">
         <v>403</v>
       </c>
-      <c r="D50" s="185">
+      <c r="D50" s="172">
         <v>4</v>
       </c>
       <c r="F50" s="19" t="s">
@@ -8094,7 +8094,7 @@
       <c r="C51" s="69" t="s">
         <v>404</v>
       </c>
-      <c r="D51" s="187"/>
+      <c r="D51" s="173"/>
       <c r="F51" s="19"/>
       <c r="H51" s="14"/>
       <c r="I51" s="14"/>
@@ -8113,7 +8113,7 @@
       <c r="C52" s="69" t="s">
         <v>405</v>
       </c>
-      <c r="D52" s="185">
+      <c r="D52" s="172">
         <v>4</v>
       </c>
       <c r="E52" s="7" t="s">
@@ -8145,7 +8145,7 @@
       <c r="C53" s="69" t="s">
         <v>406</v>
       </c>
-      <c r="D53" s="186"/>
+      <c r="D53" s="174"/>
       <c r="F53" s="19"/>
       <c r="H53" s="14"/>
       <c r="I53" s="14"/>
@@ -8164,7 +8164,7 @@
       <c r="C54" s="69" t="s">
         <v>407</v>
       </c>
-      <c r="D54" s="185">
+      <c r="D54" s="172">
         <v>4</v>
       </c>
       <c r="F54" s="19" t="s">
@@ -8193,7 +8193,7 @@
       <c r="C55" s="69" t="s">
         <v>408</v>
       </c>
-      <c r="D55" s="187"/>
+      <c r="D55" s="173"/>
       <c r="F55" s="19"/>
       <c r="H55" s="14"/>
       <c r="I55" s="14"/>
@@ -8212,7 +8212,7 @@
       <c r="C56" s="69" t="s">
         <v>409</v>
       </c>
-      <c r="D56" s="185">
+      <c r="D56" s="172">
         <v>4</v>
       </c>
       <c r="E56" s="7" t="s">
@@ -8244,7 +8244,7 @@
       <c r="C57" s="69" t="s">
         <v>410</v>
       </c>
-      <c r="D57" s="186"/>
+      <c r="D57" s="174"/>
       <c r="F57" s="19"/>
       <c r="H57" s="14"/>
       <c r="I57" s="14"/>
@@ -8263,7 +8263,7 @@
       <c r="C58" s="69" t="s">
         <v>411</v>
       </c>
-      <c r="D58" s="185">
+      <c r="D58" s="172">
         <v>4</v>
       </c>
       <c r="F58" s="19" t="s">
@@ -8292,7 +8292,7 @@
       <c r="C59" s="69" t="s">
         <v>412</v>
       </c>
-      <c r="D59" s="187"/>
+      <c r="D59" s="173"/>
       <c r="F59" s="19"/>
       <c r="H59" s="14"/>
       <c r="I59" s="14"/>
@@ -8311,7 +8311,7 @@
       <c r="C60" s="69" t="s">
         <v>413</v>
       </c>
-      <c r="D60" s="185">
+      <c r="D60" s="172">
         <v>4</v>
       </c>
       <c r="E60" s="7" t="s">
@@ -8343,7 +8343,7 @@
       <c r="C61" s="69" t="s">
         <v>414</v>
       </c>
-      <c r="D61" s="186"/>
+      <c r="D61" s="174"/>
       <c r="F61" s="19"/>
       <c r="H61" s="14"/>
       <c r="I61" s="14"/>
@@ -8362,7 +8362,7 @@
       <c r="C62" s="69" t="s">
         <v>415</v>
       </c>
-      <c r="D62" s="185">
+      <c r="D62" s="172">
         <v>4</v>
       </c>
       <c r="F62" s="19" t="s">
@@ -8391,7 +8391,7 @@
       <c r="C63" s="69" t="s">
         <v>416</v>
       </c>
-      <c r="D63" s="187"/>
+      <c r="D63" s="173"/>
       <c r="F63" s="19"/>
       <c r="H63" s="14"/>
       <c r="I63" s="14"/>
@@ -8410,7 +8410,7 @@
       <c r="C64" s="69" t="s">
         <v>417</v>
       </c>
-      <c r="D64" s="185">
+      <c r="D64" s="172">
         <v>4</v>
       </c>
       <c r="E64" s="7" t="s">
@@ -8442,7 +8442,7 @@
       <c r="C65" s="69" t="s">
         <v>418</v>
       </c>
-      <c r="D65" s="186"/>
+      <c r="D65" s="174"/>
       <c r="F65" s="19"/>
       <c r="H65" s="14"/>
       <c r="I65" s="14"/>
@@ -8461,7 +8461,7 @@
       <c r="C66" s="69" t="s">
         <v>419</v>
       </c>
-      <c r="D66" s="185">
+      <c r="D66" s="172">
         <v>4</v>
       </c>
       <c r="F66" s="19" t="s">
@@ -8490,7 +8490,7 @@
       <c r="C67" s="69" t="s">
         <v>420</v>
       </c>
-      <c r="D67" s="187"/>
+      <c r="D67" s="173"/>
       <c r="F67" s="19"/>
       <c r="H67" s="14"/>
       <c r="I67" s="14"/>
@@ -8509,7 +8509,7 @@
       <c r="C68" s="69" t="s">
         <v>421</v>
       </c>
-      <c r="D68" s="185">
+      <c r="D68" s="172">
         <v>4</v>
       </c>
       <c r="E68" s="7" t="s">
@@ -8541,7 +8541,7 @@
       <c r="C69" s="69" t="s">
         <v>422</v>
       </c>
-      <c r="D69" s="186"/>
+      <c r="D69" s="174"/>
       <c r="F69" s="19"/>
       <c r="H69" s="14"/>
       <c r="I69" s="14"/>
@@ -8615,7 +8615,7 @@
       <c r="C72" s="69" t="s">
         <v>425</v>
       </c>
-      <c r="D72" s="185">
+      <c r="D72" s="172">
         <v>4</v>
       </c>
       <c r="E72" s="7" t="s">
@@ -8647,7 +8647,7 @@
       <c r="C73" s="69" t="s">
         <v>426</v>
       </c>
-      <c r="D73" s="186"/>
+      <c r="D73" s="174"/>
       <c r="F73" s="15"/>
       <c r="H73" s="14"/>
       <c r="I73" s="14"/>
@@ -8666,7 +8666,7 @@
       <c r="C74" s="69" t="s">
         <v>427</v>
       </c>
-      <c r="D74" s="185">
+      <c r="D74" s="172">
         <v>4</v>
       </c>
       <c r="E74" s="7" t="s">
@@ -8698,7 +8698,7 @@
       <c r="C75" s="69" t="s">
         <v>428</v>
       </c>
-      <c r="D75" s="186"/>
+      <c r="D75" s="174"/>
       <c r="F75" s="15"/>
       <c r="H75" s="14"/>
       <c r="I75" s="14"/>
@@ -8957,7 +8957,7 @@
       <c r="C84" s="69" t="s">
         <v>437</v>
       </c>
-      <c r="D84" s="185">
+      <c r="D84" s="172">
         <v>4</v>
       </c>
       <c r="E84" s="7" t="s">
@@ -8987,7 +8987,7 @@
       <c r="C85" s="69" t="s">
         <v>438</v>
       </c>
-      <c r="D85" s="186"/>
+      <c r="D85" s="174"/>
       <c r="F85" s="16"/>
       <c r="H85" s="14"/>
       <c r="I85" s="14"/>
@@ -9152,16 +9152,16 @@
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A93" s="183" t="s">
+      <c r="A93" s="186" t="s">
         <v>99</v>
       </c>
-      <c r="B93" s="180" t="s">
+      <c r="B93" s="183" t="s">
         <v>315</v>
       </c>
       <c r="C93" s="69" t="s">
         <v>446</v>
       </c>
-      <c r="D93" s="185">
+      <c r="D93" s="172">
         <v>4</v>
       </c>
       <c r="E93" s="7" t="s">
@@ -9172,25 +9172,25 @@
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A94" s="184"/>
-      <c r="B94" s="184"/>
+      <c r="A94" s="187"/>
+      <c r="B94" s="187"/>
       <c r="C94" s="69" t="s">
         <v>447</v>
       </c>
-      <c r="D94" s="186"/>
+      <c r="D94" s="174"/>
       <c r="F94" s="7"/>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A95" s="183" t="s">
+      <c r="A95" s="186" t="s">
         <v>99</v>
       </c>
-      <c r="B95" s="180" t="s">
+      <c r="B95" s="183" t="s">
         <v>314</v>
       </c>
       <c r="C95" s="69" t="s">
         <v>448</v>
       </c>
-      <c r="D95" s="185">
+      <c r="D95" s="172">
         <v>4</v>
       </c>
       <c r="E95" s="7" t="s">
@@ -9201,12 +9201,12 @@
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A96" s="184"/>
-      <c r="B96" s="184"/>
+      <c r="A96" s="187"/>
+      <c r="B96" s="187"/>
       <c r="C96" s="69" t="s">
         <v>449</v>
       </c>
-      <c r="D96" s="186"/>
+      <c r="D96" s="174"/>
     </row>
     <row r="97" spans="1:11" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
@@ -9253,7 +9253,7 @@
       <c r="C99" s="69" t="s">
         <v>452</v>
       </c>
-      <c r="D99" s="185">
+      <c r="D99" s="172">
         <v>4</v>
       </c>
       <c r="E99" s="7" t="s">
@@ -9274,7 +9274,7 @@
       <c r="C100" s="69" t="s">
         <v>306</v>
       </c>
-      <c r="D100" s="186"/>
+      <c r="D100" s="174"/>
       <c r="E100" s="7"/>
       <c r="F100" s="16"/>
       <c r="G100" s="79"/>
@@ -9291,7 +9291,7 @@
       <c r="C101" s="69" t="s">
         <v>312</v>
       </c>
-      <c r="D101" s="185">
+      <c r="D101" s="172">
         <v>4</v>
       </c>
       <c r="E101" s="7" t="s">
@@ -9312,7 +9312,7 @@
       <c r="C102" s="69" t="s">
         <v>311</v>
       </c>
-      <c r="D102" s="186"/>
+      <c r="D102" s="174"/>
       <c r="F102" s="16"/>
       <c r="G102" s="79"/>
       <c r="H102" s="32"/>
@@ -10313,7 +10313,6 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="D58:D59"/>
     <mergeCell ref="D104:D105"/>
     <mergeCell ref="D106:D107"/>
     <mergeCell ref="F5:F12"/>
@@ -10329,6 +10328,14 @@
     <mergeCell ref="D66:D67"/>
     <mergeCell ref="D68:D69"/>
     <mergeCell ref="D72:D73"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="A95:A96"/>
+    <mergeCell ref="B5:B12"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B93:B94"/>
+    <mergeCell ref="B95:B96"/>
+    <mergeCell ref="A93:A94"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="D50:D51"/>
     <mergeCell ref="D52:D53"/>
@@ -10336,17 +10343,7 @@
     <mergeCell ref="D56:D57"/>
     <mergeCell ref="D48:D49"/>
     <mergeCell ref="D42:D43"/>
-    <mergeCell ref="A95:A96"/>
-    <mergeCell ref="B5:B12"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B93:B94"/>
-    <mergeCell ref="B95:B96"/>
-    <mergeCell ref="D5:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="D58:D59"/>
     <mergeCell ref="D31:D32"/>
     <mergeCell ref="D34:D35"/>
     <mergeCell ref="D36:D37"/>
@@ -10360,6 +10357,9 @@
     <mergeCell ref="D25:D26"/>
     <mergeCell ref="D27:D28"/>
     <mergeCell ref="D29:D30"/>
+    <mergeCell ref="D5:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D15:D16"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51" footer="0.51"/>
@@ -13566,10 +13566,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76419831-8B11-488C-AE0E-C0CC08014EE6}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:Q63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
@@ -13645,7 +13646,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="140" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="140" customFormat="1" ht="31.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="144">
         <v>1</v>
       </c>
@@ -13678,7 +13679,7 @@
       <c r="P2" s="155"/>
       <c r="Q2" s="155"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="144">
         <v>2</v>
       </c>
@@ -13724,7 +13725,7 @@
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="144">
         <v>3</v>
       </c>
@@ -13780,7 +13781,7 @@
         <v>1093.3333333333333</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="144">
         <v>4</v>
       </c>
@@ -13836,7 +13837,7 @@
         <v>1093.3333333333333</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="144">
         <v>5</v>
       </c>
@@ -13884,7 +13885,7 @@
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="144">
         <v>6</v>
       </c>
@@ -13930,7 +13931,7 @@
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="144">
         <v>7</v>
       </c>
@@ -13970,7 +13971,7 @@
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
     </row>
-    <row r="9" spans="1:17" ht="124.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="124.8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="162">
         <v>8</v>
       </c>
@@ -14003,7 +14004,7 @@
       <c r="P9" s="41"/>
       <c r="Q9" s="41"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="144">
         <v>9</v>
       </c>
@@ -14051,7 +14052,7 @@
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="144">
         <v>10</v>
       </c>
@@ -14099,7 +14100,7 @@
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="144">
         <v>11</v>
       </c>
@@ -14147,7 +14148,7 @@
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="144">
         <v>12</v>
       </c>
@@ -14193,7 +14194,7 @@
       <c r="P13" s="6"/>
       <c r="Q13" s="6"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="144">
         <v>13</v>
       </c>
@@ -14287,14 +14288,14 @@
       <c r="N15" s="92" t="s">
         <v>642</v>
       </c>
-      <c r="O15" s="145" t="b">
-        <f>S42=K15*0.004448230531</f>
-        <v>0</v>
+      <c r="O15" s="145">
+        <f>K15*0.004448230531</f>
+        <v>300.00201170223301</v>
       </c>
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="144">
         <v>15</v>
       </c>
@@ -14398,7 +14399,7 @@
       <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="144">
         <v>17</v>
       </c>
@@ -14502,7 +14503,7 @@
       <c r="P19" s="6"/>
       <c r="Q19" s="6"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="144">
         <v>19</v>
       </c>
@@ -14545,7 +14546,7 @@
       <c r="P20" s="6"/>
       <c r="Q20" s="6"/>
     </row>
-    <row r="21" spans="1:17" ht="62.4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" ht="62.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="162">
         <v>20</v>
       </c>
@@ -14578,7 +14579,7 @@
       <c r="P21" s="41"/>
       <c r="Q21" s="41"/>
     </row>
-    <row r="22" spans="1:17" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" ht="46.8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="162">
         <v>21</v>
       </c>
@@ -14609,7 +14610,7 @@
       <c r="P22" s="41"/>
       <c r="Q22" s="41"/>
     </row>
-    <row r="23" spans="1:17" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="31.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="144">
         <v>22</v>
       </c>
@@ -14644,7 +14645,7 @@
       <c r="P23" s="6"/>
       <c r="Q23" s="6"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="144">
         <v>23</v>
       </c>
@@ -14680,7 +14681,7 @@
       <c r="P24" s="6"/>
       <c r="Q24" s="6"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="144">
         <v>24</v>
       </c>
@@ -14762,7 +14763,7 @@
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="144">
         <v>26</v>
       </c>
@@ -14844,7 +14845,7 @@
       <c r="P28" s="6"/>
       <c r="Q28" s="6"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="144">
         <v>28</v>
       </c>
@@ -14926,7 +14927,7 @@
       <c r="P30" s="6"/>
       <c r="Q30" s="6"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="144">
         <v>30</v>
       </c>
@@ -15008,7 +15009,7 @@
       <c r="P32" s="6"/>
       <c r="Q32" s="6"/>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="144">
         <v>32</v>
       </c>
@@ -15090,7 +15091,7 @@
       <c r="P34" s="6"/>
       <c r="Q34" s="6"/>
     </row>
-    <row r="35" spans="1:17" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" ht="46.8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="144">
         <v>34</v>
       </c>
@@ -15123,7 +15124,7 @@
       <c r="P35" s="6"/>
       <c r="Q35" s="6"/>
     </row>
-    <row r="36" spans="1:17" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" ht="46.8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="144">
         <v>35</v>
       </c>
@@ -15156,7 +15157,7 @@
       <c r="P36" s="6"/>
       <c r="Q36" s="6"/>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="144">
         <v>36</v>
       </c>
@@ -15212,7 +15213,7 @@
         <v>109.33333333333333</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="144">
         <v>37</v>
       </c>
@@ -15268,7 +15269,7 @@
         <v>109.33333333333333</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" ht="31.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="144">
         <v>38</v>
       </c>
@@ -15306,7 +15307,7 @@
       <c r="P39" s="6"/>
       <c r="Q39" s="6"/>
     </row>
-    <row r="40" spans="1:17" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" ht="31.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="144">
         <v>39</v>
       </c>
@@ -15344,7 +15345,7 @@
       <c r="P40" s="6"/>
       <c r="Q40" s="6"/>
     </row>
-    <row r="41" spans="1:17" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" ht="31.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="144">
         <v>40</v>
       </c>
@@ -15382,7 +15383,7 @@
       <c r="P41" s="6"/>
       <c r="Q41" s="6"/>
     </row>
-    <row r="42" spans="1:17" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" ht="31.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="144">
         <v>41</v>
       </c>
@@ -15423,7 +15424,7 @@
       <c r="P42" s="6"/>
       <c r="Q42" s="6"/>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="144">
         <v>42</v>
       </c>
@@ -15464,7 +15465,7 @@
       <c r="P43" s="6"/>
       <c r="Q43" s="6"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="144">
         <v>43</v>
       </c>
@@ -15505,7 +15506,7 @@
       <c r="P44" s="6"/>
       <c r="Q44" s="6"/>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="144">
         <v>44</v>
       </c>
@@ -15546,7 +15547,7 @@
       <c r="P45" s="6"/>
       <c r="Q45" s="6"/>
     </row>
-    <row r="46" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="162">
         <v>45</v>
       </c>
@@ -15577,7 +15578,7 @@
       <c r="P46" s="41"/>
       <c r="Q46" s="41"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="144">
         <v>46</v>
       </c>
@@ -15623,7 +15624,7 @@
       <c r="P47" s="6"/>
       <c r="Q47" s="6"/>
     </row>
-    <row r="48" spans="1:17" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" ht="46.8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="162">
         <v>47</v>
       </c>
@@ -15654,7 +15655,7 @@
       <c r="P48" s="41"/>
       <c r="Q48" s="41"/>
     </row>
-    <row r="49" spans="1:17" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" ht="31.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="162">
         <v>48</v>
       </c>
@@ -15685,7 +15686,7 @@
       <c r="P49" s="41"/>
       <c r="Q49" s="41"/>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="144">
         <v>49</v>
       </c>
@@ -15718,7 +15719,7 @@
       <c r="P50" s="6"/>
       <c r="Q50" s="6"/>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="144">
         <v>50</v>
       </c>
@@ -15751,7 +15752,7 @@
       <c r="P51" s="6"/>
       <c r="Q51" s="6"/>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="144">
         <v>51</v>
       </c>
@@ -15784,7 +15785,7 @@
       <c r="P52" s="6"/>
       <c r="Q52" s="6"/>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="144">
         <v>52</v>
       </c>
@@ -15817,7 +15818,7 @@
       <c r="P53" s="6"/>
       <c r="Q53" s="6"/>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="144">
         <v>53</v>
       </c>
@@ -15960,7 +15961,7 @@
       <c r="P56" s="6"/>
       <c r="Q56" s="6"/>
     </row>
-    <row r="57" spans="1:17" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" ht="46.8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="162">
         <v>56</v>
       </c>
@@ -15991,7 +15992,7 @@
       <c r="P57" s="41"/>
       <c r="Q57" s="41"/>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="144">
         <v>57</v>
       </c>
@@ -16032,7 +16033,7 @@
       <c r="P58" s="6"/>
       <c r="Q58" s="6"/>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="144">
         <v>58</v>
       </c>
@@ -16078,7 +16079,7 @@
       <c r="P59" s="6"/>
       <c r="Q59" s="6"/>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="144">
         <v>59</v>
       </c>
@@ -16124,7 +16125,7 @@
       <c r="P60" s="6"/>
       <c r="Q60" s="6"/>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="144">
         <v>60</v>
       </c>
@@ -16165,7 +16166,7 @@
       <c r="P61" s="6"/>
       <c r="Q61" s="6"/>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="144">
         <v>61</v>
       </c>
@@ -16209,7 +16210,7 @@
       <c r="P62" s="6"/>
       <c r="Q62" s="6"/>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="144">
         <v>62</v>
       </c>
@@ -16256,8 +16257,15 @@
       <c r="Q63" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M63" xr:uid="{76419831-8B11-488C-AE0E-C0CC08014EE6}"/>
+  <autoFilter ref="A1:M63" xr:uid="{76419831-8B11-488C-AE0E-C0CC08014EE6}">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="Pound"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
All the screen for modbus has been completed.
</commit_message>
<xml_diff>
--- a/JM4000MODBUS_V1.0_May 31, 2025.xlsx
+++ b/JM4000MODBUS_V1.0_May 31, 2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerryw.wang\Documents\MeteringDisplay\RK3588\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C8F7F7-5CDE-4514-9090-7E021B59AC49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD376564-5623-4B91-BD72-FE8932022308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{3C7CDEC9-8383-43D7-977D-6ADA3FE6D97E}"/>
   </bookViews>
@@ -5319,10 +5319,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>TensionNum</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -5512,6 +5508,10 @@
   </si>
   <si>
     <t>SlopeAngleWellSetting</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TensiometerNumber</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -6407,14 +6407,44 @@
     <xf numFmtId="49" fontId="24" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -6441,21 +6471,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6464,20 +6479,47 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6485,21 +6527,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -6508,51 +6553,6 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6855,41 +6855,41 @@
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="176"/>
-      <c r="D1" s="177"/>
-      <c r="E1" s="177"/>
-      <c r="F1" s="176"/>
-      <c r="G1" s="176"/>
-      <c r="H1" s="176"/>
-      <c r="I1" s="178"/>
+      <c r="B1" s="185"/>
+      <c r="C1" s="186"/>
+      <c r="D1" s="187"/>
+      <c r="E1" s="187"/>
+      <c r="F1" s="186"/>
+      <c r="G1" s="186"/>
+      <c r="H1" s="186"/>
+      <c r="I1" s="188"/>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="179" t="s">
+      <c r="A2" s="189" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="180"/>
-      <c r="C2" s="180"/>
-      <c r="D2" s="181"/>
-      <c r="E2" s="181"/>
-      <c r="F2" s="180"/>
-      <c r="G2" s="180"/>
-      <c r="H2" s="180"/>
-      <c r="I2" s="180"/>
-      <c r="J2" s="180"/>
-      <c r="K2" s="180"/>
-      <c r="L2" s="180"/>
-      <c r="M2" s="180"/>
+      <c r="B2" s="190"/>
+      <c r="C2" s="190"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
+      <c r="F2" s="190"/>
+      <c r="G2" s="190"/>
+      <c r="H2" s="190"/>
+      <c r="I2" s="190"/>
+      <c r="J2" s="190"/>
+      <c r="K2" s="190"/>
+      <c r="L2" s="190"/>
+      <c r="M2" s="190"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
-      <c r="B3" s="182" t="s">
+      <c r="B3" s="192" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="182"/>
-      <c r="D3" s="182"/>
-      <c r="E3" s="182"/>
-      <c r="F3" s="182"/>
+      <c r="C3" s="192"/>
+      <c r="D3" s="192"/>
+      <c r="E3" s="192"/>
+      <c r="F3" s="192"/>
       <c r="G3" s="77"/>
       <c r="H3"/>
       <c r="I3" s="24"/>
@@ -6938,20 +6938,20 @@
       </c>
     </row>
     <row r="5" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="183" t="s">
+      <c r="A5" s="182" t="s">
         <v>340</v>
       </c>
-      <c r="B5" s="183" t="s">
+      <c r="B5" s="182" t="s">
         <v>339</v>
       </c>
       <c r="C5" s="69" t="s">
         <v>351</v>
       </c>
-      <c r="D5" s="188">
+      <c r="D5" s="193">
         <v>16</v>
       </c>
       <c r="E5" s="13"/>
-      <c r="F5" s="193" t="s">
+      <c r="F5" s="174" t="s">
         <v>289</v>
       </c>
       <c r="G5" s="78"/>
@@ -6966,14 +6966,14 @@
       </c>
     </row>
     <row r="6" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="184"/>
-      <c r="B6" s="184"/>
+      <c r="A6" s="183"/>
+      <c r="B6" s="183"/>
       <c r="C6" s="69" t="s">
         <v>348</v>
       </c>
-      <c r="D6" s="189"/>
+      <c r="D6" s="194"/>
       <c r="E6" s="13"/>
-      <c r="F6" s="194"/>
+      <c r="F6" s="175"/>
       <c r="G6" s="78"/>
       <c r="H6" s="14" t="s">
         <v>14</v>
@@ -6986,14 +6986,14 @@
       </c>
     </row>
     <row r="7" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="184"/>
-      <c r="B7" s="184"/>
+      <c r="A7" s="183"/>
+      <c r="B7" s="183"/>
       <c r="C7" s="69" t="s">
         <v>350</v>
       </c>
-      <c r="D7" s="189"/>
+      <c r="D7" s="194"/>
       <c r="E7" s="13"/>
-      <c r="F7" s="194"/>
+      <c r="F7" s="175"/>
       <c r="G7" s="78"/>
       <c r="H7" s="14" t="s">
         <v>14</v>
@@ -7006,14 +7006,14 @@
       </c>
     </row>
     <row r="8" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="184"/>
-      <c r="B8" s="184"/>
+      <c r="A8" s="183"/>
+      <c r="B8" s="183"/>
       <c r="C8" s="69" t="s">
         <v>349</v>
       </c>
-      <c r="D8" s="189"/>
+      <c r="D8" s="194"/>
       <c r="E8" s="13"/>
-      <c r="F8" s="194"/>
+      <c r="F8" s="175"/>
       <c r="G8" s="78"/>
       <c r="H8" s="14" t="s">
         <v>14</v>
@@ -7026,14 +7026,14 @@
       </c>
     </row>
     <row r="9" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="184"/>
-      <c r="B9" s="184"/>
+      <c r="A9" s="183"/>
+      <c r="B9" s="183"/>
       <c r="C9" s="69" t="s">
         <v>352</v>
       </c>
-      <c r="D9" s="189"/>
+      <c r="D9" s="194"/>
       <c r="E9" s="13"/>
-      <c r="F9" s="194"/>
+      <c r="F9" s="175"/>
       <c r="G9" s="78"/>
       <c r="H9" s="14" t="s">
         <v>14</v>
@@ -7046,14 +7046,14 @@
       </c>
     </row>
     <row r="10" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="184"/>
-      <c r="B10" s="184"/>
+      <c r="A10" s="183"/>
+      <c r="B10" s="183"/>
       <c r="C10" s="69" t="s">
         <v>363</v>
       </c>
-      <c r="D10" s="189"/>
+      <c r="D10" s="194"/>
       <c r="E10" s="13"/>
-      <c r="F10" s="194"/>
+      <c r="F10" s="175"/>
       <c r="G10" s="78"/>
       <c r="H10" s="14" t="s">
         <v>14</v>
@@ -7066,14 +7066,14 @@
       </c>
     </row>
     <row r="11" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="184"/>
-      <c r="B11" s="184"/>
+      <c r="A11" s="183"/>
+      <c r="B11" s="183"/>
       <c r="C11" s="69" t="s">
         <v>364</v>
       </c>
-      <c r="D11" s="189"/>
+      <c r="D11" s="194"/>
       <c r="E11" s="13"/>
-      <c r="F11" s="194"/>
+      <c r="F11" s="175"/>
       <c r="G11" s="78"/>
       <c r="H11" s="14" t="s">
         <v>14</v>
@@ -7086,14 +7086,14 @@
       </c>
     </row>
     <row r="12" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="185"/>
-      <c r="B12" s="185"/>
+      <c r="A12" s="184"/>
+      <c r="B12" s="184"/>
       <c r="C12" s="69" t="s">
         <v>365</v>
       </c>
-      <c r="D12" s="190"/>
+      <c r="D12" s="195"/>
       <c r="E12" s="13"/>
-      <c r="F12" s="195"/>
+      <c r="F12" s="176"/>
       <c r="G12" s="78"/>
       <c r="H12" s="14" t="s">
         <v>14</v>
@@ -7115,7 +7115,7 @@
       <c r="C13" s="69" t="s">
         <v>366</v>
       </c>
-      <c r="D13" s="172">
+      <c r="D13" s="177">
         <v>4</v>
       </c>
       <c r="E13" s="7" t="s">
@@ -7149,7 +7149,7 @@
       <c r="C14" s="69" t="s">
         <v>367</v>
       </c>
-      <c r="D14" s="174"/>
+      <c r="D14" s="178"/>
       <c r="F14" s="15"/>
       <c r="H14" s="14"/>
       <c r="I14" s="27"/>
@@ -7168,7 +7168,7 @@
       <c r="C15" s="69" t="s">
         <v>368</v>
       </c>
-      <c r="D15" s="172">
+      <c r="D15" s="177">
         <v>4</v>
       </c>
       <c r="E15" s="7" t="s">
@@ -7202,7 +7202,7 @@
       <c r="C16" s="69" t="s">
         <v>369</v>
       </c>
-      <c r="D16" s="174"/>
+      <c r="D16" s="178"/>
       <c r="F16" s="15"/>
       <c r="H16" s="14"/>
       <c r="I16" s="27"/>
@@ -7221,7 +7221,7 @@
       <c r="C17" s="69" t="s">
         <v>370</v>
       </c>
-      <c r="D17" s="172">
+      <c r="D17" s="177">
         <v>4</v>
       </c>
       <c r="E17" s="7" t="s">
@@ -7251,7 +7251,7 @@
       <c r="C18" s="69" t="s">
         <v>371</v>
       </c>
-      <c r="D18" s="174"/>
+      <c r="D18" s="178"/>
       <c r="F18" s="16"/>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
@@ -7270,7 +7270,7 @@
       <c r="C19" s="69" t="s">
         <v>372</v>
       </c>
-      <c r="D19" s="172">
+      <c r="D19" s="177">
         <v>4</v>
       </c>
       <c r="E19" s="7" t="s">
@@ -7303,7 +7303,7 @@
       <c r="C20" s="69" t="s">
         <v>373</v>
       </c>
-      <c r="D20" s="174"/>
+      <c r="D20" s="178"/>
       <c r="F20" s="16"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
@@ -7322,7 +7322,7 @@
       <c r="C21" s="69" t="s">
         <v>374</v>
       </c>
-      <c r="D21" s="172">
+      <c r="D21" s="177">
         <v>4</v>
       </c>
       <c r="E21" s="7" t="s">
@@ -7352,7 +7352,7 @@
       <c r="C22" s="69" t="s">
         <v>375</v>
       </c>
-      <c r="D22" s="174"/>
+      <c r="D22" s="178"/>
       <c r="F22" s="15"/>
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
@@ -7429,7 +7429,7 @@
       <c r="C25" s="69" t="s">
         <v>378</v>
       </c>
-      <c r="D25" s="172">
+      <c r="D25" s="177">
         <v>4</v>
       </c>
       <c r="E25" s="7" t="s">
@@ -7452,7 +7452,7 @@
       <c r="C26" s="69" t="s">
         <v>379</v>
       </c>
-      <c r="D26" s="173"/>
+      <c r="D26" s="179"/>
       <c r="F26" s="15"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -7465,7 +7465,7 @@
       <c r="C27" s="69" t="s">
         <v>380</v>
       </c>
-      <c r="D27" s="172">
+      <c r="D27" s="177">
         <v>4</v>
       </c>
       <c r="E27" s="7" t="s">
@@ -7489,7 +7489,7 @@
       <c r="C28" s="69" t="s">
         <v>381</v>
       </c>
-      <c r="D28" s="173"/>
+      <c r="D28" s="179"/>
       <c r="F28" s="15"/>
       <c r="H28" s="14"/>
       <c r="I28" s="27"/>
@@ -7508,7 +7508,7 @@
       <c r="C29" s="69" t="s">
         <v>382</v>
       </c>
-      <c r="D29" s="172">
+      <c r="D29" s="177">
         <v>4</v>
       </c>
       <c r="E29" s="7" t="s">
@@ -7532,7 +7532,7 @@
       <c r="C30" s="69" t="s">
         <v>383</v>
       </c>
-      <c r="D30" s="173"/>
+      <c r="D30" s="179"/>
       <c r="F30" s="15"/>
       <c r="H30" s="14"/>
       <c r="I30" s="27"/>
@@ -7542,16 +7542,16 @@
       <c r="M30" s="24"/>
     </row>
     <row r="31" spans="1:13" ht="92.4" x14ac:dyDescent="0.25">
-      <c r="A31" s="186" t="s">
+      <c r="A31" s="180" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="186" t="s">
+      <c r="B31" s="180" t="s">
         <v>40</v>
       </c>
       <c r="C31" s="69" t="s">
         <v>384</v>
       </c>
-      <c r="D31" s="172">
+      <c r="D31" s="177">
         <v>4</v>
       </c>
       <c r="E31" s="7" t="s">
@@ -7576,12 +7576,12 @@
       <c r="M31" s="14"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="187"/>
-      <c r="B32" s="187"/>
+      <c r="A32" s="181"/>
+      <c r="B32" s="181"/>
       <c r="C32" s="69" t="s">
         <v>385</v>
       </c>
-      <c r="D32" s="173"/>
+      <c r="D32" s="179"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
@@ -7622,7 +7622,7 @@
       <c r="C34" s="69" t="s">
         <v>387</v>
       </c>
-      <c r="D34" s="172">
+      <c r="D34" s="177">
         <v>4</v>
       </c>
       <c r="E34" s="7" t="s">
@@ -7659,7 +7659,7 @@
       <c r="C35" s="69" t="s">
         <v>388</v>
       </c>
-      <c r="D35" s="174"/>
+      <c r="D35" s="178"/>
       <c r="F35" s="20"/>
       <c r="H35" s="14"/>
       <c r="I35" s="27"/>
@@ -7678,7 +7678,7 @@
       <c r="C36" s="69" t="s">
         <v>389</v>
       </c>
-      <c r="D36" s="172">
+      <c r="D36" s="177">
         <v>4</v>
       </c>
       <c r="E36" s="7" t="s">
@@ -7712,7 +7712,7 @@
       <c r="C37" s="69" t="s">
         <v>390</v>
       </c>
-      <c r="D37" s="174"/>
+      <c r="D37" s="178"/>
       <c r="F37" s="21"/>
       <c r="H37" s="14"/>
       <c r="I37" s="27"/>
@@ -7731,7 +7731,7 @@
       <c r="C38" s="69" t="s">
         <v>391</v>
       </c>
-      <c r="D38" s="172">
+      <c r="D38" s="177">
         <v>4</v>
       </c>
       <c r="E38" s="7" t="s">
@@ -7764,7 +7764,7 @@
       <c r="C39" s="69" t="s">
         <v>392</v>
       </c>
-      <c r="D39" s="174"/>
+      <c r="D39" s="178"/>
       <c r="F39" s="20"/>
       <c r="H39" s="14"/>
       <c r="I39" s="14"/>
@@ -7783,7 +7783,7 @@
       <c r="C40" s="69" t="s">
         <v>393</v>
       </c>
-      <c r="D40" s="172">
+      <c r="D40" s="177">
         <v>4</v>
       </c>
       <c r="E40" s="7" t="s">
@@ -7816,7 +7816,7 @@
       <c r="C41" s="69" t="s">
         <v>394</v>
       </c>
-      <c r="D41" s="174"/>
+      <c r="D41" s="178"/>
       <c r="F41" s="21"/>
       <c r="H41" s="14"/>
       <c r="I41" s="14"/>
@@ -7835,7 +7835,7 @@
       <c r="C42" s="69" t="s">
         <v>395</v>
       </c>
-      <c r="D42" s="172">
+      <c r="D42" s="177">
         <v>4</v>
       </c>
       <c r="E42" s="7" t="s">
@@ -7865,7 +7865,7 @@
       <c r="C43" s="69" t="s">
         <v>396</v>
       </c>
-      <c r="D43" s="174"/>
+      <c r="D43" s="178"/>
       <c r="F43" s="19"/>
       <c r="H43" s="14"/>
       <c r="I43" s="14"/>
@@ -8017,7 +8017,7 @@
       <c r="C48" s="69" t="s">
         <v>401</v>
       </c>
-      <c r="D48" s="172">
+      <c r="D48" s="177">
         <v>4</v>
       </c>
       <c r="F48" s="15" t="s">
@@ -8046,7 +8046,7 @@
       <c r="C49" s="69" t="s">
         <v>402</v>
       </c>
-      <c r="D49" s="174"/>
+      <c r="D49" s="178"/>
       <c r="F49" s="16"/>
       <c r="H49" s="14"/>
       <c r="I49" s="14"/>
@@ -8065,7 +8065,7 @@
       <c r="C50" s="69" t="s">
         <v>403</v>
       </c>
-      <c r="D50" s="172">
+      <c r="D50" s="177">
         <v>4</v>
       </c>
       <c r="F50" s="19" t="s">
@@ -8094,7 +8094,7 @@
       <c r="C51" s="69" t="s">
         <v>404</v>
       </c>
-      <c r="D51" s="173"/>
+      <c r="D51" s="179"/>
       <c r="F51" s="19"/>
       <c r="H51" s="14"/>
       <c r="I51" s="14"/>
@@ -8113,7 +8113,7 @@
       <c r="C52" s="69" t="s">
         <v>405</v>
       </c>
-      <c r="D52" s="172">
+      <c r="D52" s="177">
         <v>4</v>
       </c>
       <c r="E52" s="7" t="s">
@@ -8145,7 +8145,7 @@
       <c r="C53" s="69" t="s">
         <v>406</v>
       </c>
-      <c r="D53" s="174"/>
+      <c r="D53" s="178"/>
       <c r="F53" s="19"/>
       <c r="H53" s="14"/>
       <c r="I53" s="14"/>
@@ -8164,7 +8164,7 @@
       <c r="C54" s="69" t="s">
         <v>407</v>
       </c>
-      <c r="D54" s="172">
+      <c r="D54" s="177">
         <v>4</v>
       </c>
       <c r="F54" s="19" t="s">
@@ -8193,7 +8193,7 @@
       <c r="C55" s="69" t="s">
         <v>408</v>
       </c>
-      <c r="D55" s="173"/>
+      <c r="D55" s="179"/>
       <c r="F55" s="19"/>
       <c r="H55" s="14"/>
       <c r="I55" s="14"/>
@@ -8212,7 +8212,7 @@
       <c r="C56" s="69" t="s">
         <v>409</v>
       </c>
-      <c r="D56" s="172">
+      <c r="D56" s="177">
         <v>4</v>
       </c>
       <c r="E56" s="7" t="s">
@@ -8244,7 +8244,7 @@
       <c r="C57" s="69" t="s">
         <v>410</v>
       </c>
-      <c r="D57" s="174"/>
+      <c r="D57" s="178"/>
       <c r="F57" s="19"/>
       <c r="H57" s="14"/>
       <c r="I57" s="14"/>
@@ -8263,7 +8263,7 @@
       <c r="C58" s="69" t="s">
         <v>411</v>
       </c>
-      <c r="D58" s="172">
+      <c r="D58" s="177">
         <v>4</v>
       </c>
       <c r="F58" s="19" t="s">
@@ -8292,7 +8292,7 @@
       <c r="C59" s="69" t="s">
         <v>412</v>
       </c>
-      <c r="D59" s="173"/>
+      <c r="D59" s="179"/>
       <c r="F59" s="19"/>
       <c r="H59" s="14"/>
       <c r="I59" s="14"/>
@@ -8311,7 +8311,7 @@
       <c r="C60" s="69" t="s">
         <v>413</v>
       </c>
-      <c r="D60" s="172">
+      <c r="D60" s="177">
         <v>4</v>
       </c>
       <c r="E60" s="7" t="s">
@@ -8343,7 +8343,7 @@
       <c r="C61" s="69" t="s">
         <v>414</v>
       </c>
-      <c r="D61" s="174"/>
+      <c r="D61" s="178"/>
       <c r="F61" s="19"/>
       <c r="H61" s="14"/>
       <c r="I61" s="14"/>
@@ -8362,7 +8362,7 @@
       <c r="C62" s="69" t="s">
         <v>415</v>
       </c>
-      <c r="D62" s="172">
+      <c r="D62" s="177">
         <v>4</v>
       </c>
       <c r="F62" s="19" t="s">
@@ -8391,7 +8391,7 @@
       <c r="C63" s="69" t="s">
         <v>416</v>
       </c>
-      <c r="D63" s="173"/>
+      <c r="D63" s="179"/>
       <c r="F63" s="19"/>
       <c r="H63" s="14"/>
       <c r="I63" s="14"/>
@@ -8410,7 +8410,7 @@
       <c r="C64" s="69" t="s">
         <v>417</v>
       </c>
-      <c r="D64" s="172">
+      <c r="D64" s="177">
         <v>4</v>
       </c>
       <c r="E64" s="7" t="s">
@@ -8442,7 +8442,7 @@
       <c r="C65" s="69" t="s">
         <v>418</v>
       </c>
-      <c r="D65" s="174"/>
+      <c r="D65" s="178"/>
       <c r="F65" s="19"/>
       <c r="H65" s="14"/>
       <c r="I65" s="14"/>
@@ -8461,7 +8461,7 @@
       <c r="C66" s="69" t="s">
         <v>419</v>
       </c>
-      <c r="D66" s="172">
+      <c r="D66" s="177">
         <v>4</v>
       </c>
       <c r="F66" s="19" t="s">
@@ -8490,7 +8490,7 @@
       <c r="C67" s="69" t="s">
         <v>420</v>
       </c>
-      <c r="D67" s="173"/>
+      <c r="D67" s="179"/>
       <c r="F67" s="19"/>
       <c r="H67" s="14"/>
       <c r="I67" s="14"/>
@@ -8509,7 +8509,7 @@
       <c r="C68" s="69" t="s">
         <v>421</v>
       </c>
-      <c r="D68" s="172">
+      <c r="D68" s="177">
         <v>4</v>
       </c>
       <c r="E68" s="7" t="s">
@@ -8541,7 +8541,7 @@
       <c r="C69" s="69" t="s">
         <v>422</v>
       </c>
-      <c r="D69" s="174"/>
+      <c r="D69" s="178"/>
       <c r="F69" s="19"/>
       <c r="H69" s="14"/>
       <c r="I69" s="14"/>
@@ -8615,7 +8615,7 @@
       <c r="C72" s="69" t="s">
         <v>425</v>
       </c>
-      <c r="D72" s="172">
+      <c r="D72" s="177">
         <v>4</v>
       </c>
       <c r="E72" s="7" t="s">
@@ -8647,7 +8647,7 @@
       <c r="C73" s="69" t="s">
         <v>426</v>
       </c>
-      <c r="D73" s="174"/>
+      <c r="D73" s="178"/>
       <c r="F73" s="15"/>
       <c r="H73" s="14"/>
       <c r="I73" s="14"/>
@@ -8666,7 +8666,7 @@
       <c r="C74" s="69" t="s">
         <v>427</v>
       </c>
-      <c r="D74" s="172">
+      <c r="D74" s="177">
         <v>4</v>
       </c>
       <c r="E74" s="7" t="s">
@@ -8698,7 +8698,7 @@
       <c r="C75" s="69" t="s">
         <v>428</v>
       </c>
-      <c r="D75" s="174"/>
+      <c r="D75" s="178"/>
       <c r="F75" s="15"/>
       <c r="H75" s="14"/>
       <c r="I75" s="14"/>
@@ -8957,7 +8957,7 @@
       <c r="C84" s="69" t="s">
         <v>437</v>
       </c>
-      <c r="D84" s="172">
+      <c r="D84" s="177">
         <v>4</v>
       </c>
       <c r="E84" s="7" t="s">
@@ -8987,7 +8987,7 @@
       <c r="C85" s="69" t="s">
         <v>438</v>
       </c>
-      <c r="D85" s="174"/>
+      <c r="D85" s="178"/>
       <c r="F85" s="16"/>
       <c r="H85" s="14"/>
       <c r="I85" s="14"/>
@@ -9152,16 +9152,16 @@
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A93" s="186" t="s">
+      <c r="A93" s="180" t="s">
         <v>99</v>
       </c>
-      <c r="B93" s="183" t="s">
+      <c r="B93" s="182" t="s">
         <v>315</v>
       </c>
       <c r="C93" s="69" t="s">
         <v>446</v>
       </c>
-      <c r="D93" s="172">
+      <c r="D93" s="177">
         <v>4</v>
       </c>
       <c r="E93" s="7" t="s">
@@ -9172,25 +9172,25 @@
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A94" s="187"/>
-      <c r="B94" s="187"/>
+      <c r="A94" s="181"/>
+      <c r="B94" s="181"/>
       <c r="C94" s="69" t="s">
         <v>447</v>
       </c>
-      <c r="D94" s="174"/>
+      <c r="D94" s="178"/>
       <c r="F94" s="7"/>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A95" s="186" t="s">
+      <c r="A95" s="180" t="s">
         <v>99</v>
       </c>
-      <c r="B95" s="183" t="s">
+      <c r="B95" s="182" t="s">
         <v>314</v>
       </c>
       <c r="C95" s="69" t="s">
         <v>448</v>
       </c>
-      <c r="D95" s="172">
+      <c r="D95" s="177">
         <v>4</v>
       </c>
       <c r="E95" s="7" t="s">
@@ -9201,12 +9201,12 @@
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A96" s="187"/>
-      <c r="B96" s="187"/>
+      <c r="A96" s="181"/>
+      <c r="B96" s="181"/>
       <c r="C96" s="69" t="s">
         <v>449</v>
       </c>
-      <c r="D96" s="174"/>
+      <c r="D96" s="178"/>
     </row>
     <row r="97" spans="1:11" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
@@ -9253,7 +9253,7 @@
       <c r="C99" s="69" t="s">
         <v>452</v>
       </c>
-      <c r="D99" s="172">
+      <c r="D99" s="177">
         <v>4</v>
       </c>
       <c r="E99" s="7" t="s">
@@ -9274,7 +9274,7 @@
       <c r="C100" s="69" t="s">
         <v>306</v>
       </c>
-      <c r="D100" s="174"/>
+      <c r="D100" s="178"/>
       <c r="E100" s="7"/>
       <c r="F100" s="16"/>
       <c r="G100" s="79"/>
@@ -9291,7 +9291,7 @@
       <c r="C101" s="69" t="s">
         <v>312</v>
       </c>
-      <c r="D101" s="172">
+      <c r="D101" s="177">
         <v>4</v>
       </c>
       <c r="E101" s="7" t="s">
@@ -9312,7 +9312,7 @@
       <c r="C102" s="69" t="s">
         <v>311</v>
       </c>
-      <c r="D102" s="174"/>
+      <c r="D102" s="178"/>
       <c r="F102" s="16"/>
       <c r="G102" s="79"/>
       <c r="H102" s="32"/>
@@ -9346,7 +9346,7 @@
       <c r="C104" s="70" t="s">
         <v>302</v>
       </c>
-      <c r="D104" s="191">
+      <c r="D104" s="172">
         <v>4</v>
       </c>
       <c r="E104" s="35" t="s">
@@ -9371,7 +9371,7 @@
       <c r="C105" s="70" t="s">
         <v>303</v>
       </c>
-      <c r="D105" s="192"/>
+      <c r="D105" s="173"/>
       <c r="E105" s="35"/>
       <c r="F105" s="36"/>
       <c r="G105" s="80"/>
@@ -9388,7 +9388,7 @@
       <c r="C106" s="70" t="s">
         <v>304</v>
       </c>
-      <c r="D106" s="191">
+      <c r="D106" s="172">
         <v>4</v>
       </c>
       <c r="E106" s="35" t="s">
@@ -9413,7 +9413,7 @@
       <c r="C107" s="70" t="s">
         <v>305</v>
       </c>
-      <c r="D107" s="192"/>
+      <c r="D107" s="173"/>
       <c r="E107" s="35"/>
       <c r="F107" s="36"/>
       <c r="G107" s="80"/>
@@ -10313,6 +10313,37 @@
     </row>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="A5:A12"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="D5:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="A95:A96"/>
+    <mergeCell ref="B5:B12"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B93:B94"/>
+    <mergeCell ref="B95:B96"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="D31:D32"/>
     <mergeCell ref="D104:D105"/>
     <mergeCell ref="D106:D107"/>
     <mergeCell ref="F5:F12"/>
@@ -10329,37 +10360,6 @@
     <mergeCell ref="D68:D69"/>
     <mergeCell ref="D72:D73"/>
     <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="A95:A96"/>
-    <mergeCell ref="B5:B12"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B93:B94"/>
-    <mergeCell ref="B95:B96"/>
-    <mergeCell ref="A93:A94"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="A5:A12"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="D5:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D15:D16"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51" footer="0.51"/>
@@ -10393,13 +10393,13 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="89"/>
-      <c r="B1" s="198" t="s">
+      <c r="B1" s="215" t="s">
         <v>479</v>
       </c>
-      <c r="C1" s="198"/>
-      <c r="D1" s="198"/>
-      <c r="E1" s="198"/>
-      <c r="F1" s="198"/>
+      <c r="C1" s="215"/>
+      <c r="D1" s="215"/>
+      <c r="E1" s="215"/>
+      <c r="F1" s="215"/>
       <c r="G1" s="90"/>
       <c r="H1" s="91"/>
       <c r="I1" s="90"/>
@@ -10444,159 +10444,159 @@
       </c>
     </row>
     <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="199" t="s">
+      <c r="A3" s="198" t="s">
         <v>487</v>
       </c>
-      <c r="B3" s="199" t="s">
+      <c r="B3" s="198" t="s">
         <v>488</v>
       </c>
       <c r="C3" s="92" t="s">
         <v>351</v>
       </c>
-      <c r="D3" s="196">
+      <c r="D3" s="210">
         <v>16</v>
       </c>
       <c r="E3" s="93"/>
-      <c r="F3" s="203" t="s">
+      <c r="F3" s="218" t="s">
         <v>489</v>
       </c>
       <c r="G3" s="94"/>
       <c r="H3" s="27" t="s">
         <v>490</v>
       </c>
-      <c r="I3" s="199" t="s">
+      <c r="I3" s="198" t="s">
         <v>475</v>
       </c>
-      <c r="J3" s="212" t="s">
+      <c r="J3" s="207" t="s">
         <v>476</v>
       </c>
-      <c r="K3" s="199"/>
+      <c r="K3" s="198"/>
       <c r="L3" s="125"/>
     </row>
     <row r="4" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="200"/>
-      <c r="B4" s="200"/>
+      <c r="A4" s="216"/>
+      <c r="B4" s="216"/>
       <c r="C4" s="92" t="s">
         <v>348</v>
       </c>
-      <c r="D4" s="197"/>
+      <c r="D4" s="211"/>
       <c r="E4" s="93"/>
-      <c r="F4" s="204"/>
+      <c r="F4" s="219"/>
       <c r="G4" s="94"/>
       <c r="H4" s="27" t="s">
         <v>490</v>
       </c>
-      <c r="I4" s="211"/>
-      <c r="J4" s="213"/>
-      <c r="K4" s="211"/>
+      <c r="I4" s="206"/>
+      <c r="J4" s="208"/>
+      <c r="K4" s="206"/>
       <c r="L4" s="126"/>
     </row>
     <row r="5" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="200"/>
-      <c r="B5" s="200"/>
+      <c r="A5" s="216"/>
+      <c r="B5" s="216"/>
       <c r="C5" s="92" t="s">
         <v>350</v>
       </c>
-      <c r="D5" s="197"/>
+      <c r="D5" s="211"/>
       <c r="E5" s="93"/>
-      <c r="F5" s="204"/>
+      <c r="F5" s="219"/>
       <c r="G5" s="94"/>
       <c r="H5" s="27" t="s">
         <v>490</v>
       </c>
-      <c r="I5" s="211"/>
-      <c r="J5" s="213"/>
-      <c r="K5" s="211"/>
+      <c r="I5" s="206"/>
+      <c r="J5" s="208"/>
+      <c r="K5" s="206"/>
       <c r="L5" s="126"/>
     </row>
     <row r="6" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="200"/>
-      <c r="B6" s="200"/>
+      <c r="A6" s="216"/>
+      <c r="B6" s="216"/>
       <c r="C6" s="92" t="s">
         <v>349</v>
       </c>
-      <c r="D6" s="197"/>
+      <c r="D6" s="211"/>
       <c r="E6" s="93"/>
-      <c r="F6" s="204"/>
+      <c r="F6" s="219"/>
       <c r="G6" s="94"/>
       <c r="H6" s="27" t="s">
         <v>490</v>
       </c>
-      <c r="I6" s="211"/>
-      <c r="J6" s="213"/>
-      <c r="K6" s="211"/>
+      <c r="I6" s="206"/>
+      <c r="J6" s="208"/>
+      <c r="K6" s="206"/>
       <c r="L6" s="126"/>
     </row>
     <row r="7" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="200"/>
-      <c r="B7" s="200"/>
+      <c r="A7" s="216"/>
+      <c r="B7" s="216"/>
       <c r="C7" s="92" t="s">
         <v>352</v>
       </c>
-      <c r="D7" s="197"/>
+      <c r="D7" s="211"/>
       <c r="E7" s="93"/>
-      <c r="F7" s="204"/>
+      <c r="F7" s="219"/>
       <c r="G7" s="94"/>
       <c r="H7" s="27" t="s">
         <v>490</v>
       </c>
-      <c r="I7" s="211"/>
-      <c r="J7" s="213"/>
-      <c r="K7" s="211"/>
+      <c r="I7" s="206"/>
+      <c r="J7" s="208"/>
+      <c r="K7" s="206"/>
       <c r="L7" s="126"/>
     </row>
     <row r="8" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="200"/>
-      <c r="B8" s="200"/>
+      <c r="A8" s="216"/>
+      <c r="B8" s="216"/>
       <c r="C8" s="92" t="s">
         <v>363</v>
       </c>
-      <c r="D8" s="197"/>
+      <c r="D8" s="211"/>
       <c r="E8" s="93"/>
-      <c r="F8" s="204"/>
+      <c r="F8" s="219"/>
       <c r="G8" s="94"/>
       <c r="H8" s="27" t="s">
         <v>490</v>
       </c>
-      <c r="I8" s="211"/>
-      <c r="J8" s="213"/>
-      <c r="K8" s="211"/>
+      <c r="I8" s="206"/>
+      <c r="J8" s="208"/>
+      <c r="K8" s="206"/>
       <c r="L8" s="126"/>
     </row>
     <row r="9" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="200"/>
-      <c r="B9" s="200"/>
+      <c r="A9" s="216"/>
+      <c r="B9" s="216"/>
       <c r="C9" s="92" t="s">
         <v>364</v>
       </c>
-      <c r="D9" s="197"/>
+      <c r="D9" s="211"/>
       <c r="E9" s="93"/>
-      <c r="F9" s="204"/>
+      <c r="F9" s="219"/>
       <c r="G9" s="94"/>
       <c r="H9" s="27" t="s">
         <v>490</v>
       </c>
-      <c r="I9" s="211"/>
-      <c r="J9" s="213"/>
-      <c r="K9" s="211"/>
+      <c r="I9" s="206"/>
+      <c r="J9" s="208"/>
+      <c r="K9" s="206"/>
       <c r="L9" s="126"/>
     </row>
     <row r="10" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="201"/>
-      <c r="B10" s="201"/>
+      <c r="A10" s="217"/>
+      <c r="B10" s="217"/>
       <c r="C10" s="92" t="s">
         <v>365</v>
       </c>
-      <c r="D10" s="202"/>
+      <c r="D10" s="212"/>
       <c r="E10" s="93"/>
-      <c r="F10" s="205"/>
+      <c r="F10" s="220"/>
       <c r="G10" s="94"/>
       <c r="H10" s="27" t="s">
         <v>490</v>
       </c>
-      <c r="I10" s="208"/>
-      <c r="J10" s="214"/>
-      <c r="K10" s="208"/>
+      <c r="I10" s="199"/>
+      <c r="J10" s="209"/>
+      <c r="K10" s="199"/>
       <c r="L10" s="127"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -10609,7 +10609,7 @@
       <c r="C11" s="92" t="s">
         <v>366</v>
       </c>
-      <c r="D11" s="196">
+      <c r="D11" s="210">
         <v>4</v>
       </c>
       <c r="E11" s="85" t="s">
@@ -10625,7 +10625,7 @@
       <c r="I11" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="212" t="s">
+      <c r="J11" s="207" t="s">
         <v>604</v>
       </c>
       <c r="K11" s="27">
@@ -10646,13 +10646,13 @@
       <c r="C12" s="92" t="s">
         <v>367</v>
       </c>
-      <c r="D12" s="202"/>
+      <c r="D12" s="212"/>
       <c r="E12" s="85"/>
       <c r="F12" s="96"/>
       <c r="G12" s="97"/>
       <c r="H12" s="27"/>
       <c r="I12" s="27"/>
-      <c r="J12" s="214"/>
+      <c r="J12" s="209"/>
       <c r="K12" s="88">
         <v>-9999999</v>
       </c>
@@ -10671,7 +10671,7 @@
       <c r="C13" s="92" t="s">
         <v>368</v>
       </c>
-      <c r="D13" s="196">
+      <c r="D13" s="210">
         <v>4</v>
       </c>
       <c r="E13" s="85" t="s">
@@ -10687,7 +10687,7 @@
       <c r="I13" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="J13" s="215" t="s">
+      <c r="J13" s="202" t="s">
         <v>607</v>
       </c>
       <c r="K13" s="27">
@@ -10708,13 +10708,13 @@
       <c r="C14" s="92" t="s">
         <v>369</v>
       </c>
-      <c r="D14" s="202"/>
+      <c r="D14" s="212"/>
       <c r="E14" s="85"/>
       <c r="F14" s="96"/>
       <c r="G14" s="97"/>
       <c r="H14" s="27"/>
       <c r="I14" s="27"/>
-      <c r="J14" s="216"/>
+      <c r="J14" s="203"/>
       <c r="K14" s="27">
         <v>-2000000</v>
       </c>
@@ -10733,7 +10733,7 @@
       <c r="C15" s="92" t="s">
         <v>370</v>
       </c>
-      <c r="D15" s="196">
+      <c r="D15" s="210">
         <v>4</v>
       </c>
       <c r="E15" s="85" t="s">
@@ -10749,7 +10749,7 @@
       <c r="I15" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="215" t="s">
+      <c r="J15" s="202" t="s">
         <v>607</v>
       </c>
       <c r="K15" s="27">
@@ -10770,13 +10770,13 @@
       <c r="C16" s="92" t="s">
         <v>371</v>
       </c>
-      <c r="D16" s="202"/>
+      <c r="D16" s="212"/>
       <c r="E16" s="85"/>
       <c r="F16" s="98"/>
       <c r="G16" s="97"/>
       <c r="H16" s="27"/>
       <c r="I16" s="27"/>
-      <c r="J16" s="216"/>
+      <c r="J16" s="203"/>
       <c r="K16" s="27">
         <v>-2000000</v>
       </c>
@@ -10795,7 +10795,7 @@
       <c r="C17" s="92" t="s">
         <v>372</v>
       </c>
-      <c r="D17" s="196">
+      <c r="D17" s="210">
         <v>4</v>
       </c>
       <c r="E17" s="85" t="s">
@@ -10813,7 +10813,7 @@
       <c r="I17" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="215" t="s">
+      <c r="J17" s="202" t="s">
         <v>604</v>
       </c>
       <c r="K17" s="27">
@@ -10834,13 +10834,13 @@
       <c r="C18" s="92" t="s">
         <v>373</v>
       </c>
-      <c r="D18" s="202"/>
+      <c r="D18" s="212"/>
       <c r="E18" s="85"/>
       <c r="F18" s="98"/>
       <c r="G18" s="97"/>
       <c r="H18" s="27"/>
       <c r="I18" s="27"/>
-      <c r="J18" s="216"/>
+      <c r="J18" s="203"/>
       <c r="K18" s="27">
         <v>0</v>
       </c>
@@ -10859,7 +10859,7 @@
       <c r="C19" s="92" t="s">
         <v>374</v>
       </c>
-      <c r="D19" s="196">
+      <c r="D19" s="210">
         <v>4</v>
       </c>
       <c r="E19" s="85" t="s">
@@ -10875,7 +10875,7 @@
       <c r="I19" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="215" t="s">
+      <c r="J19" s="202" t="s">
         <v>604</v>
       </c>
       <c r="K19" s="27">
@@ -10896,13 +10896,13 @@
       <c r="C20" s="92" t="s">
         <v>375</v>
       </c>
-      <c r="D20" s="202"/>
+      <c r="D20" s="212"/>
       <c r="E20" s="85"/>
       <c r="F20" s="96"/>
       <c r="G20" s="97"/>
       <c r="H20" s="27"/>
       <c r="I20" s="27"/>
-      <c r="J20" s="216"/>
+      <c r="J20" s="203"/>
       <c r="K20" s="27">
         <v>0</v>
       </c>
@@ -10990,7 +10990,7 @@
       <c r="C23" s="92" t="s">
         <v>378</v>
       </c>
-      <c r="D23" s="196">
+      <c r="D23" s="210">
         <v>4</v>
       </c>
       <c r="E23" s="85" t="s">
@@ -11006,7 +11006,7 @@
         <v>493</v>
       </c>
       <c r="I23" s="92"/>
-      <c r="J23" s="215" t="s">
+      <c r="J23" s="202" t="s">
         <v>604</v>
       </c>
       <c r="K23" s="27">
@@ -11025,13 +11025,13 @@
       <c r="C24" s="92" t="s">
         <v>379</v>
       </c>
-      <c r="D24" s="197"/>
+      <c r="D24" s="211"/>
       <c r="E24" s="85"/>
       <c r="F24" s="96"/>
       <c r="G24" s="97"/>
       <c r="H24" s="92"/>
       <c r="I24" s="92"/>
-      <c r="J24" s="216"/>
+      <c r="J24" s="203"/>
       <c r="K24" s="27">
         <v>-9999999</v>
       </c>
@@ -11050,7 +11050,7 @@
       <c r="C25" s="92" t="s">
         <v>380</v>
       </c>
-      <c r="D25" s="196">
+      <c r="D25" s="210">
         <v>4</v>
       </c>
       <c r="E25" s="85" t="s">
@@ -11066,7 +11066,7 @@
         <v>493</v>
       </c>
       <c r="I25" s="92"/>
-      <c r="J25" s="215" t="s">
+      <c r="J25" s="202" t="s">
         <v>604</v>
       </c>
       <c r="K25" s="27">
@@ -11085,13 +11085,13 @@
       <c r="C26" s="92" t="s">
         <v>381</v>
       </c>
-      <c r="D26" s="197"/>
+      <c r="D26" s="211"/>
       <c r="E26" s="85"/>
       <c r="F26" s="96"/>
       <c r="G26" s="97"/>
       <c r="H26" s="27"/>
       <c r="I26" s="27"/>
-      <c r="J26" s="216"/>
+      <c r="J26" s="203"/>
       <c r="K26" s="27">
         <v>-9999999</v>
       </c>
@@ -11110,7 +11110,7 @@
       <c r="C27" s="92" t="s">
         <v>382</v>
       </c>
-      <c r="D27" s="196">
+      <c r="D27" s="210">
         <v>4</v>
       </c>
       <c r="E27" s="85" t="s">
@@ -11126,7 +11126,7 @@
         <v>493</v>
       </c>
       <c r="I27" s="92"/>
-      <c r="J27" s="215" t="s">
+      <c r="J27" s="202" t="s">
         <v>604</v>
       </c>
       <c r="K27" s="27">
@@ -11145,13 +11145,13 @@
       <c r="C28" s="92" t="s">
         <v>383</v>
       </c>
-      <c r="D28" s="197"/>
+      <c r="D28" s="211"/>
       <c r="E28" s="85"/>
       <c r="F28" s="96"/>
       <c r="G28" s="97"/>
       <c r="H28" s="27"/>
       <c r="I28" s="27"/>
-      <c r="J28" s="216"/>
+      <c r="J28" s="203"/>
       <c r="K28" s="27">
         <v>-9999999</v>
       </c>
@@ -11161,16 +11161,16 @@
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="199" t="s">
+      <c r="A29" s="198" t="s">
         <v>491</v>
       </c>
-      <c r="B29" s="199" t="s">
+      <c r="B29" s="198" t="s">
         <v>513</v>
       </c>
       <c r="C29" s="92" t="s">
         <v>384</v>
       </c>
-      <c r="D29" s="196">
+      <c r="D29" s="210">
         <v>4</v>
       </c>
       <c r="E29" s="85" t="s">
@@ -11186,7 +11186,7 @@
       <c r="I29" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="J29" s="215" t="s">
+      <c r="J29" s="202" t="s">
         <v>604</v>
       </c>
       <c r="K29" s="27">
@@ -11198,18 +11198,18 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="208"/>
-      <c r="B30" s="208"/>
+      <c r="A30" s="199"/>
+      <c r="B30" s="199"/>
       <c r="C30" s="92" t="s">
         <v>385</v>
       </c>
-      <c r="D30" s="197"/>
+      <c r="D30" s="211"/>
       <c r="E30" s="85"/>
       <c r="F30" s="99"/>
       <c r="G30" s="97"/>
       <c r="H30" s="92"/>
       <c r="I30" s="92"/>
-      <c r="J30" s="216"/>
+      <c r="J30" s="203"/>
       <c r="K30" s="27">
         <v>0</v>
       </c>
@@ -11265,7 +11265,7 @@
       <c r="C32" s="92" t="s">
         <v>387</v>
       </c>
-      <c r="D32" s="196">
+      <c r="D32" s="210">
         <v>4</v>
       </c>
       <c r="E32" s="85" t="s">
@@ -11283,7 +11283,7 @@
       <c r="I32" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J32" s="215" t="s">
+      <c r="J32" s="202" t="s">
         <v>609</v>
       </c>
       <c r="K32" s="27">
@@ -11304,13 +11304,13 @@
       <c r="C33" s="92" t="s">
         <v>388</v>
       </c>
-      <c r="D33" s="202"/>
+      <c r="D33" s="212"/>
       <c r="E33" s="85"/>
       <c r="F33" s="102"/>
       <c r="G33" s="97"/>
       <c r="H33" s="27"/>
       <c r="I33" s="27"/>
-      <c r="J33" s="216"/>
+      <c r="J33" s="203"/>
       <c r="K33" s="27">
         <v>0</v>
       </c>
@@ -11329,7 +11329,7 @@
       <c r="C34" s="92" t="s">
         <v>389</v>
       </c>
-      <c r="D34" s="196">
+      <c r="D34" s="210">
         <v>4</v>
       </c>
       <c r="E34" s="85" t="s">
@@ -11345,7 +11345,7 @@
       <c r="I34" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="J34" s="215" t="s">
+      <c r="J34" s="202" t="s">
         <v>610</v>
       </c>
       <c r="K34" s="27">
@@ -11366,13 +11366,13 @@
       <c r="C35" s="92" t="s">
         <v>390</v>
       </c>
-      <c r="D35" s="202"/>
+      <c r="D35" s="212"/>
       <c r="E35" s="85"/>
       <c r="F35" s="128"/>
       <c r="G35" s="97"/>
       <c r="H35" s="27"/>
       <c r="I35" s="27"/>
-      <c r="J35" s="216"/>
+      <c r="J35" s="203"/>
       <c r="K35" s="27">
         <v>0</v>
       </c>
@@ -11391,7 +11391,7 @@
       <c r="C36" s="92" t="s">
         <v>391</v>
       </c>
-      <c r="D36" s="196">
+      <c r="D36" s="210">
         <v>4</v>
       </c>
       <c r="E36" s="85" t="s">
@@ -11409,7 +11409,7 @@
       <c r="I36" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J36" s="215" t="s">
+      <c r="J36" s="202" t="s">
         <v>609</v>
       </c>
       <c r="K36" s="27">
@@ -11430,13 +11430,13 @@
       <c r="C37" s="92" t="s">
         <v>392</v>
       </c>
-      <c r="D37" s="202"/>
+      <c r="D37" s="212"/>
       <c r="E37" s="85"/>
       <c r="F37" s="102"/>
       <c r="G37" s="97"/>
       <c r="H37" s="27"/>
       <c r="I37" s="27"/>
-      <c r="J37" s="216"/>
+      <c r="J37" s="203"/>
       <c r="K37" s="27">
         <v>0</v>
       </c>
@@ -11455,7 +11455,7 @@
       <c r="C38" s="92" t="s">
         <v>393</v>
       </c>
-      <c r="D38" s="196">
+      <c r="D38" s="210">
         <v>4</v>
       </c>
       <c r="E38" s="85" t="s">
@@ -11473,7 +11473,7 @@
       <c r="I38" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J38" s="215" t="s">
+      <c r="J38" s="202" t="s">
         <v>610</v>
       </c>
       <c r="K38" s="27">
@@ -11494,13 +11494,13 @@
       <c r="C39" s="92" t="s">
         <v>394</v>
       </c>
-      <c r="D39" s="202"/>
+      <c r="D39" s="212"/>
       <c r="E39" s="85"/>
       <c r="F39" s="103"/>
       <c r="G39" s="97"/>
       <c r="H39" s="27"/>
       <c r="I39" s="27"/>
-      <c r="J39" s="216"/>
+      <c r="J39" s="203"/>
       <c r="K39" s="27">
         <v>0</v>
       </c>
@@ -11519,7 +11519,7 @@
       <c r="C40" s="92" t="s">
         <v>395</v>
       </c>
-      <c r="D40" s="196">
+      <c r="D40" s="210">
         <v>4</v>
       </c>
       <c r="E40" s="85" t="s">
@@ -11535,7 +11535,7 @@
       <c r="I40" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="J40" s="215" t="s">
+      <c r="J40" s="202" t="s">
         <v>610</v>
       </c>
       <c r="K40" s="27">
@@ -11556,13 +11556,13 @@
       <c r="C41" s="92" t="s">
         <v>396</v>
       </c>
-      <c r="D41" s="202"/>
+      <c r="D41" s="212"/>
       <c r="E41" s="85"/>
       <c r="F41" s="101"/>
       <c r="G41" s="97"/>
       <c r="H41" s="27"/>
       <c r="I41" s="27"/>
-      <c r="J41" s="216"/>
+      <c r="J41" s="203"/>
       <c r="K41" s="27">
         <v>0</v>
       </c>
@@ -11716,7 +11716,7 @@
       <c r="C46" s="92" t="s">
         <v>401</v>
       </c>
-      <c r="D46" s="196">
+      <c r="D46" s="210">
         <v>4</v>
       </c>
       <c r="E46" s="85"/>
@@ -11730,7 +11730,7 @@
       <c r="I46" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J46" s="215" t="s">
+      <c r="J46" s="202" t="s">
         <v>630</v>
       </c>
       <c r="K46" s="27">
@@ -11751,13 +11751,13 @@
       <c r="C47" s="92" t="s">
         <v>402</v>
       </c>
-      <c r="D47" s="202"/>
+      <c r="D47" s="212"/>
       <c r="E47" s="85"/>
       <c r="F47" s="98"/>
       <c r="G47" s="97"/>
       <c r="H47" s="27"/>
       <c r="I47" s="27"/>
-      <c r="J47" s="216"/>
+      <c r="J47" s="203"/>
       <c r="K47" s="27">
         <v>1</v>
       </c>
@@ -11776,7 +11776,7 @@
       <c r="C48" s="130" t="s">
         <v>403</v>
       </c>
-      <c r="D48" s="206">
+      <c r="D48" s="213">
         <v>4</v>
       </c>
       <c r="E48" s="131"/>
@@ -11790,7 +11790,7 @@
       <c r="I48" s="129" t="s">
         <v>78</v>
       </c>
-      <c r="J48" s="217" t="s">
+      <c r="J48" s="200" t="s">
         <v>630</v>
       </c>
       <c r="K48" s="129"/>
@@ -11806,13 +11806,13 @@
       <c r="C49" s="130" t="s">
         <v>404</v>
       </c>
-      <c r="D49" s="207"/>
+      <c r="D49" s="214"/>
       <c r="E49" s="131"/>
       <c r="F49" s="132"/>
       <c r="G49" s="133"/>
       <c r="H49" s="129"/>
       <c r="I49" s="129"/>
-      <c r="J49" s="218"/>
+      <c r="J49" s="201"/>
       <c r="K49" s="129"/>
       <c r="L49" s="134"/>
     </row>
@@ -11826,7 +11826,7 @@
       <c r="C50" s="92" t="s">
         <v>405</v>
       </c>
-      <c r="D50" s="196">
+      <c r="D50" s="210">
         <v>4</v>
       </c>
       <c r="E50" s="85" t="s">
@@ -11842,7 +11842,7 @@
       <c r="I50" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="J50" s="215" t="s">
+      <c r="J50" s="202" t="s">
         <v>609</v>
       </c>
       <c r="K50" s="27">
@@ -11863,13 +11863,13 @@
       <c r="C51" s="92" t="s">
         <v>406</v>
       </c>
-      <c r="D51" s="202"/>
+      <c r="D51" s="212"/>
       <c r="E51" s="85"/>
       <c r="F51" s="101"/>
       <c r="G51" s="97"/>
       <c r="H51" s="27"/>
       <c r="I51" s="27"/>
-      <c r="J51" s="216"/>
+      <c r="J51" s="203"/>
       <c r="K51" s="27">
         <v>0</v>
       </c>
@@ -11888,7 +11888,7 @@
       <c r="C52" s="92" t="s">
         <v>407</v>
       </c>
-      <c r="D52" s="196">
+      <c r="D52" s="210">
         <v>4</v>
       </c>
       <c r="E52" s="85"/>
@@ -11902,7 +11902,7 @@
       <c r="I52" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="J52" s="215" t="s">
+      <c r="J52" s="202" t="s">
         <v>630</v>
       </c>
       <c r="K52" s="27"/>
@@ -11918,13 +11918,13 @@
       <c r="C53" s="92" t="s">
         <v>408</v>
       </c>
-      <c r="D53" s="197"/>
+      <c r="D53" s="211"/>
       <c r="E53" s="85"/>
       <c r="F53" s="101"/>
       <c r="G53" s="97"/>
       <c r="H53" s="27"/>
       <c r="I53" s="27"/>
-      <c r="J53" s="216"/>
+      <c r="J53" s="203"/>
       <c r="K53" s="27"/>
       <c r="L53" s="118"/>
     </row>
@@ -11938,7 +11938,7 @@
       <c r="C54" s="92" t="s">
         <v>409</v>
       </c>
-      <c r="D54" s="196">
+      <c r="D54" s="210">
         <v>4</v>
       </c>
       <c r="E54" s="85" t="s">
@@ -11954,7 +11954,7 @@
       <c r="I54" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="J54" s="199" t="s">
+      <c r="J54" s="198" t="s">
         <v>609</v>
       </c>
       <c r="K54" s="27">
@@ -11975,13 +11975,13 @@
       <c r="C55" s="92" t="s">
         <v>410</v>
       </c>
-      <c r="D55" s="202"/>
+      <c r="D55" s="212"/>
       <c r="E55" s="85"/>
       <c r="F55" s="101"/>
       <c r="G55" s="97"/>
       <c r="H55" s="27"/>
       <c r="I55" s="27"/>
-      <c r="J55" s="208"/>
+      <c r="J55" s="199"/>
       <c r="K55" s="27">
         <v>0</v>
       </c>
@@ -11999,7 +11999,7 @@
       <c r="C56" s="92" t="s">
         <v>411</v>
       </c>
-      <c r="D56" s="196">
+      <c r="D56" s="210">
         <v>4</v>
       </c>
       <c r="E56" s="85"/>
@@ -12013,7 +12013,7 @@
       <c r="I56" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="J56" s="199" t="s">
+      <c r="J56" s="198" t="s">
         <v>630</v>
       </c>
       <c r="K56" s="27"/>
@@ -12029,13 +12029,13 @@
       <c r="C57" s="92" t="s">
         <v>412</v>
       </c>
-      <c r="D57" s="197"/>
+      <c r="D57" s="211"/>
       <c r="E57" s="85"/>
       <c r="F57" s="101"/>
       <c r="G57" s="97"/>
       <c r="H57" s="27"/>
       <c r="I57" s="27"/>
-      <c r="J57" s="208"/>
+      <c r="J57" s="199"/>
       <c r="K57" s="27"/>
       <c r="L57" s="118"/>
     </row>
@@ -12049,7 +12049,7 @@
       <c r="C58" s="92" t="s">
         <v>413</v>
       </c>
-      <c r="D58" s="196">
+      <c r="D58" s="210">
         <v>4</v>
       </c>
       <c r="E58" s="85" t="s">
@@ -12065,7 +12065,7 @@
       <c r="I58" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="J58" s="199" t="s">
+      <c r="J58" s="198" t="s">
         <v>609</v>
       </c>
       <c r="K58" s="27"/>
@@ -12081,13 +12081,13 @@
       <c r="C59" s="92" t="s">
         <v>414</v>
       </c>
-      <c r="D59" s="202"/>
+      <c r="D59" s="212"/>
       <c r="E59" s="85"/>
       <c r="F59" s="101"/>
       <c r="G59" s="97"/>
       <c r="H59" s="27"/>
       <c r="I59" s="27"/>
-      <c r="J59" s="208"/>
+      <c r="J59" s="199"/>
       <c r="K59" s="27"/>
       <c r="L59" s="118"/>
     </row>
@@ -12101,7 +12101,7 @@
       <c r="C60" s="92" t="s">
         <v>415</v>
       </c>
-      <c r="D60" s="196">
+      <c r="D60" s="210">
         <v>4</v>
       </c>
       <c r="E60" s="85"/>
@@ -12115,7 +12115,7 @@
       <c r="I60" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="J60" s="199" t="s">
+      <c r="J60" s="198" t="s">
         <v>630</v>
       </c>
       <c r="K60" s="27"/>
@@ -12131,13 +12131,13 @@
       <c r="C61" s="92" t="s">
         <v>416</v>
       </c>
-      <c r="D61" s="197"/>
+      <c r="D61" s="211"/>
       <c r="E61" s="85"/>
       <c r="F61" s="101"/>
       <c r="G61" s="97"/>
       <c r="H61" s="27"/>
       <c r="I61" s="27"/>
-      <c r="J61" s="208"/>
+      <c r="J61" s="199"/>
       <c r="K61" s="27"/>
       <c r="L61" s="118"/>
     </row>
@@ -12151,7 +12151,7 @@
       <c r="C62" s="92" t="s">
         <v>417</v>
       </c>
-      <c r="D62" s="196">
+      <c r="D62" s="210">
         <v>4</v>
       </c>
       <c r="E62" s="85" t="s">
@@ -12167,7 +12167,7 @@
       <c r="I62" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="J62" s="199" t="s">
+      <c r="J62" s="198" t="s">
         <v>609</v>
       </c>
       <c r="K62" s="27">
@@ -12188,13 +12188,13 @@
       <c r="C63" s="92" t="s">
         <v>418</v>
       </c>
-      <c r="D63" s="202"/>
+      <c r="D63" s="212"/>
       <c r="E63" s="85"/>
       <c r="F63" s="101"/>
       <c r="G63" s="97"/>
       <c r="H63" s="27"/>
       <c r="I63" s="27"/>
-      <c r="J63" s="208"/>
+      <c r="J63" s="199"/>
       <c r="K63" s="27">
         <v>0</v>
       </c>
@@ -12213,7 +12213,7 @@
       <c r="C64" s="92" t="s">
         <v>419</v>
       </c>
-      <c r="D64" s="196">
+      <c r="D64" s="210">
         <v>4</v>
       </c>
       <c r="E64" s="85"/>
@@ -12227,7 +12227,7 @@
       <c r="I64" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="J64" s="199" t="s">
+      <c r="J64" s="198" t="s">
         <v>630</v>
       </c>
       <c r="K64" s="27"/>
@@ -12243,13 +12243,13 @@
       <c r="C65" s="92" t="s">
         <v>420</v>
       </c>
-      <c r="D65" s="197"/>
+      <c r="D65" s="211"/>
       <c r="E65" s="85"/>
       <c r="F65" s="101"/>
       <c r="G65" s="97"/>
       <c r="H65" s="27"/>
       <c r="I65" s="27"/>
-      <c r="J65" s="208"/>
+      <c r="J65" s="199"/>
       <c r="K65" s="27"/>
       <c r="L65" s="118"/>
     </row>
@@ -12263,7 +12263,7 @@
       <c r="C66" s="92" t="s">
         <v>421</v>
       </c>
-      <c r="D66" s="196">
+      <c r="D66" s="210">
         <v>4</v>
       </c>
       <c r="E66" s="85" t="s">
@@ -12279,7 +12279,7 @@
       <c r="I66" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="J66" s="199" t="s">
+      <c r="J66" s="198" t="s">
         <v>609</v>
       </c>
       <c r="K66" s="27">
@@ -12300,13 +12300,13 @@
       <c r="C67" s="92" t="s">
         <v>422</v>
       </c>
-      <c r="D67" s="202"/>
+      <c r="D67" s="212"/>
       <c r="E67" s="85"/>
       <c r="F67" s="101"/>
       <c r="G67" s="97"/>
       <c r="H67" s="27"/>
       <c r="I67" s="27"/>
-      <c r="J67" s="208"/>
+      <c r="J67" s="199"/>
       <c r="K67" s="27">
         <v>0</v>
       </c>
@@ -12387,7 +12387,7 @@
       <c r="C70" s="92" t="s">
         <v>425</v>
       </c>
-      <c r="D70" s="196">
+      <c r="D70" s="210">
         <v>4</v>
       </c>
       <c r="E70" s="85" t="s">
@@ -12403,7 +12403,7 @@
       <c r="I70" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J70" s="199" t="s">
+      <c r="J70" s="198" t="s">
         <v>607</v>
       </c>
       <c r="K70" s="27">
@@ -12424,13 +12424,13 @@
       <c r="C71" s="92" t="s">
         <v>426</v>
       </c>
-      <c r="D71" s="202"/>
+      <c r="D71" s="212"/>
       <c r="E71" s="85"/>
       <c r="F71" s="96"/>
       <c r="G71" s="97"/>
       <c r="H71" s="27"/>
       <c r="I71" s="27"/>
-      <c r="J71" s="208"/>
+      <c r="J71" s="199"/>
       <c r="K71" s="27">
         <v>30000</v>
       </c>
@@ -12449,7 +12449,7 @@
       <c r="C72" s="92" t="s">
         <v>427</v>
       </c>
-      <c r="D72" s="196">
+      <c r="D72" s="210">
         <v>4</v>
       </c>
       <c r="E72" s="85" t="s">
@@ -12465,7 +12465,7 @@
       <c r="I72" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J72" s="199" t="s">
+      <c r="J72" s="198" t="s">
         <v>607</v>
       </c>
       <c r="K72" s="27">
@@ -12486,13 +12486,13 @@
       <c r="C73" s="92" t="s">
         <v>428</v>
       </c>
-      <c r="D73" s="202"/>
+      <c r="D73" s="212"/>
       <c r="E73" s="85"/>
       <c r="F73" s="96"/>
       <c r="G73" s="97"/>
       <c r="H73" s="27"/>
       <c r="I73" s="27"/>
-      <c r="J73" s="208"/>
+      <c r="J73" s="199"/>
       <c r="K73" s="27">
         <v>10000</v>
       </c>
@@ -12792,7 +12792,7 @@
       <c r="C82" s="92" t="s">
         <v>437</v>
       </c>
-      <c r="D82" s="196">
+      <c r="D82" s="210">
         <v>4</v>
       </c>
       <c r="E82" s="85" t="s">
@@ -12808,7 +12808,7 @@
       <c r="I82" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J82" s="199" t="s">
+      <c r="J82" s="198" t="s">
         <v>604</v>
       </c>
       <c r="K82" s="27">
@@ -12829,13 +12829,13 @@
       <c r="C83" s="92" t="s">
         <v>438</v>
       </c>
-      <c r="D83" s="202"/>
+      <c r="D83" s="212"/>
       <c r="E83" s="85"/>
       <c r="F83" s="98"/>
       <c r="G83" s="97"/>
       <c r="H83" s="27"/>
       <c r="I83" s="27"/>
-      <c r="J83" s="208"/>
+      <c r="J83" s="199"/>
       <c r="K83" s="27">
         <v>0</v>
       </c>
@@ -13051,16 +13051,16 @@
       <c r="L90" s="118"/>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A91" s="199" t="s">
+      <c r="A91" s="198" t="s">
         <v>558</v>
       </c>
-      <c r="B91" s="199" t="s">
+      <c r="B91" s="198" t="s">
         <v>593</v>
       </c>
       <c r="C91" s="92" t="s">
         <v>446</v>
       </c>
-      <c r="D91" s="196">
+      <c r="D91" s="210">
         <v>4</v>
       </c>
       <c r="E91" s="85" t="s">
@@ -13072,7 +13072,7 @@
       <c r="G91" s="97"/>
       <c r="H91" s="92"/>
       <c r="I91" s="92"/>
-      <c r="J91" s="199" t="s">
+      <c r="J91" s="198" t="s">
         <v>609</v>
       </c>
       <c r="K91" s="27">
@@ -13084,18 +13084,18 @@
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A92" s="208"/>
-      <c r="B92" s="208"/>
+      <c r="A92" s="199"/>
+      <c r="B92" s="199"/>
       <c r="C92" s="92" t="s">
         <v>447</v>
       </c>
-      <c r="D92" s="202"/>
+      <c r="D92" s="212"/>
       <c r="E92" s="85"/>
       <c r="F92" s="85"/>
       <c r="G92" s="97"/>
       <c r="H92" s="92"/>
       <c r="I92" s="92"/>
-      <c r="J92" s="208"/>
+      <c r="J92" s="199"/>
       <c r="K92" s="27">
         <v>0</v>
       </c>
@@ -13105,16 +13105,16 @@
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A93" s="199" t="s">
+      <c r="A93" s="198" t="s">
         <v>558</v>
       </c>
-      <c r="B93" s="199" t="s">
+      <c r="B93" s="198" t="s">
         <v>594</v>
       </c>
       <c r="C93" s="92" t="s">
         <v>448</v>
       </c>
-      <c r="D93" s="196">
+      <c r="D93" s="210">
         <v>4</v>
       </c>
       <c r="E93" s="85" t="s">
@@ -13126,7 +13126,7 @@
       <c r="G93" s="97"/>
       <c r="H93" s="92"/>
       <c r="I93" s="92"/>
-      <c r="J93" s="199" t="s">
+      <c r="J93" s="198" t="s">
         <v>609</v>
       </c>
       <c r="K93" s="27">
@@ -13138,18 +13138,18 @@
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A94" s="208"/>
-      <c r="B94" s="208"/>
+      <c r="A94" s="199"/>
+      <c r="B94" s="199"/>
       <c r="C94" s="92" t="s">
         <v>449</v>
       </c>
-      <c r="D94" s="202"/>
+      <c r="D94" s="212"/>
       <c r="E94" s="85"/>
       <c r="F94" s="99"/>
       <c r="G94" s="97"/>
       <c r="H94" s="92"/>
       <c r="I94" s="92"/>
-      <c r="J94" s="208"/>
+      <c r="J94" s="199"/>
       <c r="K94" s="27">
         <v>0</v>
       </c>
@@ -13225,7 +13225,7 @@
       <c r="C97" s="92" t="s">
         <v>452</v>
       </c>
-      <c r="D97" s="196">
+      <c r="D97" s="210">
         <v>4</v>
       </c>
       <c r="E97" s="85" t="s">
@@ -13239,7 +13239,7 @@
         <v>490</v>
       </c>
       <c r="I97" s="92"/>
-      <c r="J97" s="199" t="s">
+      <c r="J97" s="198" t="s">
         <v>604</v>
       </c>
       <c r="K97" s="27">
@@ -13258,13 +13258,13 @@
       <c r="C98" s="92" t="s">
         <v>306</v>
       </c>
-      <c r="D98" s="202"/>
+      <c r="D98" s="212"/>
       <c r="E98" s="85"/>
       <c r="F98" s="98"/>
       <c r="G98" s="110"/>
       <c r="H98" s="111"/>
       <c r="I98" s="111"/>
-      <c r="J98" s="208"/>
+      <c r="J98" s="199"/>
       <c r="K98" s="123">
         <v>0</v>
       </c>
@@ -13281,7 +13281,7 @@
       <c r="C99" s="92" t="s">
         <v>312</v>
       </c>
-      <c r="D99" s="196">
+      <c r="D99" s="210">
         <v>4</v>
       </c>
       <c r="E99" s="85" t="s">
@@ -13295,7 +13295,7 @@
         <v>490</v>
       </c>
       <c r="I99" s="92"/>
-      <c r="J99" s="199" t="s">
+      <c r="J99" s="198" t="s">
         <v>604</v>
       </c>
       <c r="K99" s="27">
@@ -13314,13 +13314,13 @@
       <c r="C100" s="92" t="s">
         <v>311</v>
       </c>
-      <c r="D100" s="202"/>
+      <c r="D100" s="212"/>
       <c r="E100" s="85"/>
       <c r="F100" s="98"/>
       <c r="G100" s="110"/>
       <c r="H100" s="111"/>
       <c r="I100" s="92"/>
-      <c r="J100" s="208"/>
+      <c r="J100" s="199"/>
       <c r="K100" s="27">
         <v>0</v>
       </c>
@@ -13370,7 +13370,7 @@
       <c r="C102" s="114" t="s">
         <v>302</v>
       </c>
-      <c r="D102" s="209">
+      <c r="D102" s="204">
         <v>4</v>
       </c>
       <c r="E102" s="115" t="s">
@@ -13384,7 +13384,7 @@
         <v>490</v>
       </c>
       <c r="I102" s="114"/>
-      <c r="J102" s="219" t="s">
+      <c r="J102" s="196" t="s">
         <v>604</v>
       </c>
       <c r="K102" s="124">
@@ -13403,13 +13403,13 @@
       <c r="C103" s="114" t="s">
         <v>303</v>
       </c>
-      <c r="D103" s="210"/>
+      <c r="D103" s="205"/>
       <c r="E103" s="115"/>
       <c r="F103" s="116"/>
       <c r="G103" s="117"/>
       <c r="H103" s="114"/>
       <c r="I103" s="114"/>
-      <c r="J103" s="220"/>
+      <c r="J103" s="197"/>
       <c r="K103" s="124">
         <v>0</v>
       </c>
@@ -13426,7 +13426,7 @@
       <c r="C104" s="114" t="s">
         <v>304</v>
       </c>
-      <c r="D104" s="209">
+      <c r="D104" s="204">
         <v>4</v>
       </c>
       <c r="E104" s="115" t="s">
@@ -13440,7 +13440,7 @@
         <v>490</v>
       </c>
       <c r="I104" s="114"/>
-      <c r="J104" s="219" t="s">
+      <c r="J104" s="196" t="s">
         <v>604</v>
       </c>
       <c r="K104" s="124">
@@ -13459,13 +13459,13 @@
       <c r="C105" s="114" t="s">
         <v>305</v>
       </c>
-      <c r="D105" s="210"/>
+      <c r="D105" s="205"/>
       <c r="E105" s="115"/>
       <c r="F105" s="116"/>
       <c r="G105" s="117"/>
       <c r="H105" s="114"/>
       <c r="I105" s="114"/>
-      <c r="J105" s="220"/>
+      <c r="J105" s="197"/>
       <c r="K105" s="124">
         <v>0</v>
       </c>
@@ -13476,37 +13476,41 @@
     </row>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="J104:J105"/>
-    <mergeCell ref="J82:J83"/>
-    <mergeCell ref="J91:J92"/>
-    <mergeCell ref="J93:J94"/>
-    <mergeCell ref="J97:J98"/>
-    <mergeCell ref="J99:J100"/>
-    <mergeCell ref="J102:J103"/>
-    <mergeCell ref="J72:J73"/>
-    <mergeCell ref="J48:J49"/>
-    <mergeCell ref="J50:J51"/>
-    <mergeCell ref="J52:J53"/>
-    <mergeCell ref="J54:J55"/>
-    <mergeCell ref="J56:J57"/>
-    <mergeCell ref="J58:J59"/>
-    <mergeCell ref="J60:J61"/>
-    <mergeCell ref="J62:J63"/>
-    <mergeCell ref="J64:J65"/>
-    <mergeCell ref="J66:J67"/>
-    <mergeCell ref="J70:J71"/>
-    <mergeCell ref="J46:J47"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="J27:J28"/>
-    <mergeCell ref="J29:J30"/>
-    <mergeCell ref="J32:J33"/>
-    <mergeCell ref="J34:J35"/>
-    <mergeCell ref="J36:J37"/>
-    <mergeCell ref="J38:J39"/>
-    <mergeCell ref="J40:J41"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="D3:D10"/>
+    <mergeCell ref="F3:F10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="A91:A92"/>
+    <mergeCell ref="B91:B92"/>
+    <mergeCell ref="D91:D92"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="B93:B94"/>
+    <mergeCell ref="D93:D94"/>
+    <mergeCell ref="D97:D98"/>
+    <mergeCell ref="D99:D100"/>
     <mergeCell ref="D104:D105"/>
     <mergeCell ref="I3:I10"/>
     <mergeCell ref="J3:J10"/>
@@ -13523,41 +13527,37 @@
     <mergeCell ref="D36:D37"/>
     <mergeCell ref="D38:D39"/>
     <mergeCell ref="D40:D41"/>
-    <mergeCell ref="A93:A94"/>
-    <mergeCell ref="B93:B94"/>
-    <mergeCell ref="D93:D94"/>
-    <mergeCell ref="D97:D98"/>
-    <mergeCell ref="D99:D100"/>
-    <mergeCell ref="A91:A92"/>
-    <mergeCell ref="B91:B92"/>
-    <mergeCell ref="D91:D92"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="A3:A10"/>
-    <mergeCell ref="B3:B10"/>
-    <mergeCell ref="D3:D10"/>
-    <mergeCell ref="F3:F10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="J46:J47"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="J27:J28"/>
+    <mergeCell ref="J29:J30"/>
+    <mergeCell ref="J32:J33"/>
+    <mergeCell ref="J34:J35"/>
+    <mergeCell ref="J36:J37"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="J40:J41"/>
+    <mergeCell ref="J72:J73"/>
+    <mergeCell ref="J48:J49"/>
+    <mergeCell ref="J50:J51"/>
+    <mergeCell ref="J52:J53"/>
+    <mergeCell ref="J54:J55"/>
+    <mergeCell ref="J56:J57"/>
+    <mergeCell ref="J58:J59"/>
+    <mergeCell ref="J60:J61"/>
+    <mergeCell ref="J62:J63"/>
+    <mergeCell ref="J64:J65"/>
+    <mergeCell ref="J66:J67"/>
+    <mergeCell ref="J70:J71"/>
+    <mergeCell ref="J104:J105"/>
+    <mergeCell ref="J82:J83"/>
+    <mergeCell ref="J91:J92"/>
+    <mergeCell ref="J93:J94"/>
+    <mergeCell ref="J97:J98"/>
+    <mergeCell ref="J99:J100"/>
+    <mergeCell ref="J102:J103"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13566,11 +13566,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76419831-8B11-488C-AE0E-C0CC08014EE6}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:Q63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" topLeftCell="B21" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
@@ -13646,7 +13645,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="140" customFormat="1" ht="31.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="140" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A2" s="144">
         <v>1</v>
       </c>
@@ -13679,7 +13678,7 @@
       <c r="P2" s="155"/>
       <c r="Q2" s="155"/>
     </row>
-    <row r="3" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="144">
         <v>2</v>
       </c>
@@ -13725,7 +13724,7 @@
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
     </row>
-    <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="144">
         <v>3</v>
       </c>
@@ -13781,7 +13780,7 @@
         <v>1093.3333333333333</v>
       </c>
     </row>
-    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="144">
         <v>4</v>
       </c>
@@ -13837,7 +13836,7 @@
         <v>1093.3333333333333</v>
       </c>
     </row>
-    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="144">
         <v>5</v>
       </c>
@@ -13885,7 +13884,7 @@
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
     </row>
-    <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="144">
         <v>6</v>
       </c>
@@ -13931,7 +13930,7 @@
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
     </row>
-    <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="144">
         <v>7</v>
       </c>
@@ -13971,7 +13970,7 @@
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
     </row>
-    <row r="9" spans="1:17" ht="124.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="124.8" x14ac:dyDescent="0.25">
       <c r="A9" s="162">
         <v>8</v>
       </c>
@@ -14004,7 +14003,7 @@
       <c r="P9" s="41"/>
       <c r="Q9" s="41"/>
     </row>
-    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="144">
         <v>9</v>
       </c>
@@ -14052,7 +14051,7 @@
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
     </row>
-    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="144">
         <v>10</v>
       </c>
@@ -14100,7 +14099,7 @@
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
     </row>
-    <row r="12" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="144">
         <v>11</v>
       </c>
@@ -14148,12 +14147,12 @@
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
     </row>
-    <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="144">
         <v>12</v>
       </c>
       <c r="B13" s="58" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C13" s="27" t="s">
         <v>686</v>
@@ -14194,12 +14193,12 @@
       <c r="P13" s="6"/>
       <c r="Q13" s="6"/>
     </row>
-    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="144">
         <v>13</v>
       </c>
       <c r="B14" s="58" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C14" s="27" t="s">
         <v>685</v>
@@ -14295,7 +14294,7 @@
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
     </row>
-    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="144">
         <v>15</v>
       </c>
@@ -14399,7 +14398,7 @@
       <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
     </row>
-    <row r="18" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="144">
         <v>17</v>
       </c>
@@ -14503,7 +14502,7 @@
       <c r="P19" s="6"/>
       <c r="Q19" s="6"/>
     </row>
-    <row r="20" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="144">
         <v>19</v>
       </c>
@@ -14546,7 +14545,7 @@
       <c r="P20" s="6"/>
       <c r="Q20" s="6"/>
     </row>
-    <row r="21" spans="1:17" ht="62.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" ht="62.4" x14ac:dyDescent="0.25">
       <c r="A21" s="162">
         <v>20</v>
       </c>
@@ -14579,7 +14578,7 @@
       <c r="P21" s="41"/>
       <c r="Q21" s="41"/>
     </row>
-    <row r="22" spans="1:17" ht="46.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A22" s="162">
         <v>21</v>
       </c>
@@ -14610,7 +14609,7 @@
       <c r="P22" s="41"/>
       <c r="Q22" s="41"/>
     </row>
-    <row r="23" spans="1:17" ht="31.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A23" s="144">
         <v>22</v>
       </c>
@@ -14627,7 +14626,7 @@
         <v>0.01</v>
       </c>
       <c r="F23" s="96" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="G23" s="97" t="s">
         <v>533</v>
@@ -14645,7 +14644,7 @@
       <c r="P23" s="6"/>
       <c r="Q23" s="6"/>
     </row>
-    <row r="24" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="144">
         <v>23</v>
       </c>
@@ -14653,7 +14652,7 @@
         <v>657</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>697</v>
+        <v>740</v>
       </c>
       <c r="D24" s="85">
         <v>4</v>
@@ -14681,7 +14680,7 @@
       <c r="P24" s="6"/>
       <c r="Q24" s="6"/>
     </row>
-    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="144">
         <v>24</v>
       </c>
@@ -14689,7 +14688,7 @@
         <v>658</v>
       </c>
       <c r="C25" s="129" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="D25" s="131">
         <v>4</v>
@@ -14720,7 +14719,7 @@
         <v>659</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D26" s="85">
         <v>4</v>
@@ -14763,7 +14762,7 @@
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
     </row>
-    <row r="27" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="144">
         <v>26</v>
       </c>
@@ -14771,7 +14770,7 @@
         <v>661</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="D27" s="85">
         <v>4</v>
@@ -14799,10 +14798,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="151" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="C28" s="27" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D28" s="85">
         <v>4</v>
@@ -14845,7 +14844,7 @@
       <c r="P28" s="6"/>
       <c r="Q28" s="6"/>
     </row>
-    <row r="29" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="144">
         <v>28</v>
       </c>
@@ -14853,7 +14852,7 @@
         <v>662</v>
       </c>
       <c r="C29" s="27" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="D29" s="85">
         <v>4</v>
@@ -14884,7 +14883,7 @@
         <v>663</v>
       </c>
       <c r="C30" s="27" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D30" s="85">
         <v>4</v>
@@ -14927,7 +14926,7 @@
       <c r="P30" s="6"/>
       <c r="Q30" s="6"/>
     </row>
-    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="144">
         <v>30</v>
       </c>
@@ -14935,7 +14934,7 @@
         <v>664</v>
       </c>
       <c r="C31" s="27" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D31" s="85">
         <v>4</v>
@@ -14966,7 +14965,7 @@
         <v>665</v>
       </c>
       <c r="C32" s="27" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D32" s="85">
         <v>4</v>
@@ -15009,7 +15008,7 @@
       <c r="P32" s="6"/>
       <c r="Q32" s="6"/>
     </row>
-    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="144">
         <v>32</v>
       </c>
@@ -15017,7 +15016,7 @@
         <v>666</v>
       </c>
       <c r="C33" s="27" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D33" s="85">
         <v>4</v>
@@ -15048,7 +15047,7 @@
         <v>667</v>
       </c>
       <c r="C34" s="27" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D34" s="85">
         <v>4</v>
@@ -15091,7 +15090,7 @@
       <c r="P34" s="6"/>
       <c r="Q34" s="6"/>
     </row>
-    <row r="35" spans="1:17" ht="46.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A35" s="144">
         <v>34</v>
       </c>
@@ -15099,7 +15098,7 @@
         <v>559</v>
       </c>
       <c r="C35" s="27" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D35" s="85">
         <v>2</v>
@@ -15124,7 +15123,7 @@
       <c r="P35" s="6"/>
       <c r="Q35" s="6"/>
     </row>
-    <row r="36" spans="1:17" ht="46.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A36" s="144">
         <v>35</v>
       </c>
@@ -15132,7 +15131,7 @@
         <v>561</v>
       </c>
       <c r="C36" s="27" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D36" s="85">
         <v>2</v>
@@ -15157,7 +15156,7 @@
       <c r="P36" s="6"/>
       <c r="Q36" s="6"/>
     </row>
-    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="144">
         <v>36</v>
       </c>
@@ -15165,7 +15164,7 @@
         <v>668</v>
       </c>
       <c r="C37" s="27" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D37" s="85">
         <v>4</v>
@@ -15213,7 +15212,7 @@
         <v>109.33333333333333</v>
       </c>
     </row>
-    <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="144">
         <v>37</v>
       </c>
@@ -15221,7 +15220,7 @@
         <v>669</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D38" s="85">
         <v>4</v>
@@ -15269,7 +15268,7 @@
         <v>109.33333333333333</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="31.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A39" s="144">
         <v>38</v>
       </c>
@@ -15277,7 +15276,7 @@
         <v>568</v>
       </c>
       <c r="C39" s="27" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="D39" s="85">
         <v>2</v>
@@ -15307,7 +15306,7 @@
       <c r="P39" s="6"/>
       <c r="Q39" s="6"/>
     </row>
-    <row r="40" spans="1:17" ht="31.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A40" s="144">
         <v>39</v>
       </c>
@@ -15315,7 +15314,7 @@
         <v>570</v>
       </c>
       <c r="C40" s="27" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="D40" s="85">
         <v>2</v>
@@ -15345,7 +15344,7 @@
       <c r="P40" s="6"/>
       <c r="Q40" s="6"/>
     </row>
-    <row r="41" spans="1:17" ht="31.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A41" s="144">
         <v>40</v>
       </c>
@@ -15353,7 +15352,7 @@
         <v>571</v>
       </c>
       <c r="C41" s="27" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="D41" s="85">
         <v>2</v>
@@ -15383,7 +15382,7 @@
       <c r="P41" s="6"/>
       <c r="Q41" s="6"/>
     </row>
-    <row r="42" spans="1:17" ht="31.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A42" s="144">
         <v>41</v>
       </c>
@@ -15391,7 +15390,7 @@
         <v>572</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="D42" s="85">
         <v>2</v>
@@ -15424,7 +15423,7 @@
       <c r="P42" s="6"/>
       <c r="Q42" s="6"/>
     </row>
-    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="144">
         <v>42</v>
       </c>
@@ -15432,7 +15431,7 @@
         <v>573</v>
       </c>
       <c r="C43" s="27" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D43" s="85">
         <v>2</v>
@@ -15465,7 +15464,7 @@
       <c r="P43" s="6"/>
       <c r="Q43" s="6"/>
     </row>
-    <row r="44" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="144">
         <v>43</v>
       </c>
@@ -15473,7 +15472,7 @@
         <v>574</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="D44" s="85">
         <v>2</v>
@@ -15506,7 +15505,7 @@
       <c r="P44" s="6"/>
       <c r="Q44" s="6"/>
     </row>
-    <row r="45" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="144">
         <v>44</v>
       </c>
@@ -15514,7 +15513,7 @@
         <v>575</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="D45" s="85">
         <v>2</v>
@@ -15547,7 +15546,7 @@
       <c r="P45" s="6"/>
       <c r="Q45" s="6"/>
     </row>
-    <row r="46" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="162">
         <v>45</v>
       </c>
@@ -15555,7 +15554,7 @@
         <v>576</v>
       </c>
       <c r="C46" s="164" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="D46" s="165">
         <v>2</v>
@@ -15578,7 +15577,7 @@
       <c r="P46" s="41"/>
       <c r="Q46" s="41"/>
     </row>
-    <row r="47" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="144">
         <v>46</v>
       </c>
@@ -15586,7 +15585,7 @@
         <v>670</v>
       </c>
       <c r="C47" s="27" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="D47" s="85">
         <v>4</v>
@@ -15624,7 +15623,7 @@
       <c r="P47" s="6"/>
       <c r="Q47" s="6"/>
     </row>
-    <row r="48" spans="1:17" ht="46.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A48" s="162">
         <v>47</v>
       </c>
@@ -15632,7 +15631,7 @@
         <v>579</v>
       </c>
       <c r="C48" s="164" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="D48" s="165">
         <v>2</v>
@@ -15655,7 +15654,7 @@
       <c r="P48" s="41"/>
       <c r="Q48" s="41"/>
     </row>
-    <row r="49" spans="1:17" ht="31.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A49" s="162">
         <v>48</v>
       </c>
@@ -15663,7 +15662,7 @@
         <v>581</v>
       </c>
       <c r="C49" s="164" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="D49" s="165">
         <v>2</v>
@@ -15686,7 +15685,7 @@
       <c r="P49" s="41"/>
       <c r="Q49" s="41"/>
     </row>
-    <row r="50" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="144">
         <v>49</v>
       </c>
@@ -15694,7 +15693,7 @@
         <v>583</v>
       </c>
       <c r="C50" s="27" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="D50" s="85">
         <v>2</v>
@@ -15719,15 +15718,15 @@
       <c r="P50" s="6"/>
       <c r="Q50" s="6"/>
     </row>
-    <row r="51" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="144">
         <v>50</v>
       </c>
       <c r="B51" s="59" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C51" s="27" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D51" s="85">
         <v>2</v>
@@ -15752,7 +15751,7 @@
       <c r="P51" s="6"/>
       <c r="Q51" s="6"/>
     </row>
-    <row r="52" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="144">
         <v>51</v>
       </c>
@@ -15760,7 +15759,7 @@
         <v>587</v>
       </c>
       <c r="C52" s="27" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="D52" s="85">
         <v>2</v>
@@ -15785,7 +15784,7 @@
       <c r="P52" s="6"/>
       <c r="Q52" s="6"/>
     </row>
-    <row r="53" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="144">
         <v>52</v>
       </c>
@@ -15793,7 +15792,7 @@
         <v>317</v>
       </c>
       <c r="C53" s="27" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="D53" s="85">
         <v>2</v>
@@ -15818,7 +15817,7 @@
       <c r="P53" s="6"/>
       <c r="Q53" s="6"/>
     </row>
-    <row r="54" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="144">
         <v>53</v>
       </c>
@@ -15826,7 +15825,7 @@
         <v>316</v>
       </c>
       <c r="C54" s="27" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="D54" s="85">
         <v>2</v>
@@ -15867,7 +15866,7 @@
         <v>593</v>
       </c>
       <c r="C55" s="27" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="D55" s="85">
         <v>4</v>
@@ -15918,7 +15917,7 @@
         <v>594</v>
       </c>
       <c r="C56" s="27" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="D56" s="85">
         <v>4</v>
@@ -15961,7 +15960,7 @@
       <c r="P56" s="6"/>
       <c r="Q56" s="6"/>
     </row>
-    <row r="57" spans="1:17" ht="46.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A57" s="162">
         <v>56</v>
       </c>
@@ -15969,7 +15968,7 @@
         <v>595</v>
       </c>
       <c r="C57" s="164" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="D57" s="165">
         <v>2</v>
@@ -15992,7 +15991,7 @@
       <c r="P57" s="41"/>
       <c r="Q57" s="41"/>
     </row>
-    <row r="58" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="144">
         <v>57</v>
       </c>
@@ -16000,7 +15999,7 @@
         <v>597</v>
       </c>
       <c r="C58" s="27" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="D58" s="85">
         <v>2</v>
@@ -16033,7 +16032,7 @@
       <c r="P58" s="6"/>
       <c r="Q58" s="6"/>
     </row>
-    <row r="59" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="144">
         <v>58</v>
       </c>
@@ -16041,7 +16040,7 @@
         <v>671</v>
       </c>
       <c r="C59" s="27" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="D59" s="85">
         <v>4</v>
@@ -16079,7 +16078,7 @@
       <c r="P59" s="6"/>
       <c r="Q59" s="6"/>
     </row>
-    <row r="60" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="144">
         <v>59</v>
       </c>
@@ -16087,7 +16086,7 @@
         <v>672</v>
       </c>
       <c r="C60" s="27" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="D60" s="85">
         <v>4</v>
@@ -16125,7 +16124,7 @@
       <c r="P60" s="6"/>
       <c r="Q60" s="6"/>
     </row>
-    <row r="61" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="144">
         <v>60</v>
       </c>
@@ -16133,7 +16132,7 @@
         <v>602</v>
       </c>
       <c r="C61" s="27" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="D61" s="136">
         <v>2</v>
@@ -16166,7 +16165,7 @@
       <c r="P61" s="6"/>
       <c r="Q61" s="6"/>
     </row>
-    <row r="62" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="144">
         <v>61</v>
       </c>
@@ -16210,7 +16209,7 @@
       <c r="P62" s="6"/>
       <c r="Q62" s="6"/>
     </row>
-    <row r="63" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="144">
         <v>62</v>
       </c>
@@ -16218,7 +16217,7 @@
         <v>673</v>
       </c>
       <c r="C63" s="160" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D63" s="158">
         <v>4</v>
@@ -16257,13 +16256,7 @@
       <c r="Q63" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M63" xr:uid="{76419831-8B11-488C-AE0E-C0CC08014EE6}">
-    <filterColumn colId="7">
-      <filters>
-        <filter val="Pound"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:M63" xr:uid="{76419831-8B11-488C-AE0E-C0CC08014EE6}"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add control velocity and down count features
</commit_message>
<xml_diff>
--- a/JM4000MODBUS_V1.0_May 31, 2025.xlsx
+++ b/JM4000MODBUS_V1.0_May 31, 2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerryw.wang\Documents\MeteringDisplay\RK3588\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4648A023-26C5-4E5B-9052-59C70228FCF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF2B2A1-CE73-4702-B24F-19D7BEA664C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3C7CDEC9-8383-43D7-977D-6ADA3FE6D97E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3C7CDEC9-8383-43D7-977D-6ADA3FE6D97E}"/>
   </bookViews>
   <sheets>
     <sheet name="参数列表" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1985" uniqueCount="924">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1986" uniqueCount="925">
   <si>
     <t>修改说明</t>
   </si>
@@ -5385,9 +5385,6 @@
     <t>Tension#5</t>
   </si>
   <si>
-    <t>Scale#井</t>
-  </si>
-  <si>
     <t>QuantityOfCalibration</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -8530,6 +8527,14 @@
   <si>
     <t>OrientationDepth</t>
     <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>DepthStartSetting</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>DepthFinishSetting</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -9486,6 +9491,45 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -9511,30 +9555,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -9543,20 +9563,47 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -9564,21 +9611,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -9587,51 +9637,6 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9910,8 +9915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48F8D282-0EA3-4F42-AB54-7D424EF2399B}">
   <dimension ref="A1:M162"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A113" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
@@ -9934,41 +9939,41 @@
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="184"/>
-      <c r="C1" s="185"/>
-      <c r="D1" s="186"/>
-      <c r="E1" s="186"/>
-      <c r="F1" s="185"/>
-      <c r="G1" s="185"/>
-      <c r="H1" s="185"/>
-      <c r="I1" s="187"/>
+      <c r="B1" s="197"/>
+      <c r="C1" s="198"/>
+      <c r="D1" s="199"/>
+      <c r="E1" s="199"/>
+      <c r="F1" s="198"/>
+      <c r="G1" s="198"/>
+      <c r="H1" s="198"/>
+      <c r="I1" s="200"/>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="188" t="s">
+      <c r="A2" s="201" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="189"/>
-      <c r="C2" s="189"/>
-      <c r="D2" s="190"/>
-      <c r="E2" s="190"/>
-      <c r="F2" s="189"/>
-      <c r="G2" s="189"/>
-      <c r="H2" s="189"/>
-      <c r="I2" s="189"/>
-      <c r="J2" s="189"/>
-      <c r="K2" s="189"/>
-      <c r="L2" s="189"/>
-      <c r="M2" s="189"/>
+      <c r="B2" s="202"/>
+      <c r="C2" s="202"/>
+      <c r="D2" s="203"/>
+      <c r="E2" s="203"/>
+      <c r="F2" s="202"/>
+      <c r="G2" s="202"/>
+      <c r="H2" s="202"/>
+      <c r="I2" s="202"/>
+      <c r="J2" s="202"/>
+      <c r="K2" s="202"/>
+      <c r="L2" s="202"/>
+      <c r="M2" s="202"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
-      <c r="B3" s="191" t="s">
+      <c r="B3" s="204" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="191"/>
-      <c r="D3" s="191"/>
-      <c r="E3" s="191"/>
-      <c r="F3" s="191"/>
+      <c r="C3" s="204"/>
+      <c r="D3" s="204"/>
+      <c r="E3" s="204"/>
+      <c r="F3" s="204"/>
       <c r="G3" s="77"/>
       <c r="H3"/>
       <c r="I3" s="24"/>
@@ -10017,20 +10022,20 @@
       </c>
     </row>
     <row r="5" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="192" t="s">
+      <c r="A5" s="194" t="s">
         <v>340</v>
       </c>
-      <c r="B5" s="192" t="s">
+      <c r="B5" s="194" t="s">
         <v>339</v>
       </c>
       <c r="C5" s="69" t="s">
         <v>351</v>
       </c>
-      <c r="D5" s="200">
+      <c r="D5" s="205">
         <v>16</v>
       </c>
       <c r="E5" s="13"/>
-      <c r="F5" s="205" t="s">
+      <c r="F5" s="189" t="s">
         <v>289</v>
       </c>
       <c r="G5" s="78"/>
@@ -10045,14 +10050,14 @@
       </c>
     </row>
     <row r="6" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="193"/>
-      <c r="B6" s="193"/>
+      <c r="A6" s="195"/>
+      <c r="B6" s="195"/>
       <c r="C6" s="69" t="s">
         <v>348</v>
       </c>
-      <c r="D6" s="201"/>
+      <c r="D6" s="206"/>
       <c r="E6" s="13"/>
-      <c r="F6" s="206"/>
+      <c r="F6" s="190"/>
       <c r="G6" s="78"/>
       <c r="H6" s="14" t="s">
         <v>14</v>
@@ -10065,14 +10070,14 @@
       </c>
     </row>
     <row r="7" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="193"/>
-      <c r="B7" s="193"/>
+      <c r="A7" s="195"/>
+      <c r="B7" s="195"/>
       <c r="C7" s="69" t="s">
         <v>350</v>
       </c>
-      <c r="D7" s="201"/>
+      <c r="D7" s="206"/>
       <c r="E7" s="13"/>
-      <c r="F7" s="206"/>
+      <c r="F7" s="190"/>
       <c r="G7" s="78"/>
       <c r="H7" s="14" t="s">
         <v>14</v>
@@ -10085,14 +10090,14 @@
       </c>
     </row>
     <row r="8" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="193"/>
-      <c r="B8" s="193"/>
+      <c r="A8" s="195"/>
+      <c r="B8" s="195"/>
       <c r="C8" s="69" t="s">
         <v>349</v>
       </c>
-      <c r="D8" s="201"/>
+      <c r="D8" s="206"/>
       <c r="E8" s="13"/>
-      <c r="F8" s="206"/>
+      <c r="F8" s="190"/>
       <c r="G8" s="78"/>
       <c r="H8" s="14" t="s">
         <v>14</v>
@@ -10105,14 +10110,14 @@
       </c>
     </row>
     <row r="9" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="193"/>
-      <c r="B9" s="193"/>
+      <c r="A9" s="195"/>
+      <c r="B9" s="195"/>
       <c r="C9" s="69" t="s">
         <v>352</v>
       </c>
-      <c r="D9" s="201"/>
+      <c r="D9" s="206"/>
       <c r="E9" s="13"/>
-      <c r="F9" s="206"/>
+      <c r="F9" s="190"/>
       <c r="G9" s="78"/>
       <c r="H9" s="14" t="s">
         <v>14</v>
@@ -10125,14 +10130,14 @@
       </c>
     </row>
     <row r="10" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="193"/>
-      <c r="B10" s="193"/>
+      <c r="A10" s="195"/>
+      <c r="B10" s="195"/>
       <c r="C10" s="69" t="s">
         <v>363</v>
       </c>
-      <c r="D10" s="201"/>
+      <c r="D10" s="206"/>
       <c r="E10" s="13"/>
-      <c r="F10" s="206"/>
+      <c r="F10" s="190"/>
       <c r="G10" s="78"/>
       <c r="H10" s="14" t="s">
         <v>14</v>
@@ -10145,14 +10150,14 @@
       </c>
     </row>
     <row r="11" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="193"/>
-      <c r="B11" s="193"/>
+      <c r="A11" s="195"/>
+      <c r="B11" s="195"/>
       <c r="C11" s="69" t="s">
         <v>364</v>
       </c>
-      <c r="D11" s="201"/>
+      <c r="D11" s="206"/>
       <c r="E11" s="13"/>
-      <c r="F11" s="206"/>
+      <c r="F11" s="190"/>
       <c r="G11" s="78"/>
       <c r="H11" s="14" t="s">
         <v>14</v>
@@ -10165,14 +10170,14 @@
       </c>
     </row>
     <row r="12" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="194"/>
-      <c r="B12" s="194"/>
+      <c r="A12" s="196"/>
+      <c r="B12" s="196"/>
       <c r="C12" s="69" t="s">
         <v>365</v>
       </c>
-      <c r="D12" s="202"/>
+      <c r="D12" s="207"/>
       <c r="E12" s="13"/>
-      <c r="F12" s="207"/>
+      <c r="F12" s="191"/>
       <c r="G12" s="78"/>
       <c r="H12" s="14" t="s">
         <v>14</v>
@@ -10194,7 +10199,7 @@
       <c r="C13" s="69" t="s">
         <v>366</v>
       </c>
-      <c r="D13" s="197">
+      <c r="D13" s="184">
         <v>4</v>
       </c>
       <c r="E13" s="7" t="s">
@@ -10228,7 +10233,7 @@
       <c r="C14" s="69" t="s">
         <v>367</v>
       </c>
-      <c r="D14" s="198"/>
+      <c r="D14" s="185"/>
       <c r="F14" s="15"/>
       <c r="H14" s="14"/>
       <c r="I14" s="27"/>
@@ -10247,7 +10252,7 @@
       <c r="C15" s="69" t="s">
         <v>368</v>
       </c>
-      <c r="D15" s="197">
+      <c r="D15" s="184">
         <v>4</v>
       </c>
       <c r="E15" s="7" t="s">
@@ -10281,7 +10286,7 @@
       <c r="C16" s="69" t="s">
         <v>369</v>
       </c>
-      <c r="D16" s="198"/>
+      <c r="D16" s="185"/>
       <c r="F16" s="15"/>
       <c r="H16" s="14"/>
       <c r="I16" s="27"/>
@@ -10300,7 +10305,7 @@
       <c r="C17" s="69" t="s">
         <v>370</v>
       </c>
-      <c r="D17" s="197">
+      <c r="D17" s="184">
         <v>4</v>
       </c>
       <c r="E17" s="7" t="s">
@@ -10330,7 +10335,7 @@
       <c r="C18" s="69" t="s">
         <v>371</v>
       </c>
-      <c r="D18" s="198"/>
+      <c r="D18" s="185"/>
       <c r="F18" s="16"/>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
@@ -10349,7 +10354,7 @@
       <c r="C19" s="69" t="s">
         <v>372</v>
       </c>
-      <c r="D19" s="197">
+      <c r="D19" s="184">
         <v>4</v>
       </c>
       <c r="E19" s="7" t="s">
@@ -10382,7 +10387,7 @@
       <c r="C20" s="69" t="s">
         <v>373</v>
       </c>
-      <c r="D20" s="198"/>
+      <c r="D20" s="185"/>
       <c r="F20" s="16"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
@@ -10401,7 +10406,7 @@
       <c r="C21" s="69" t="s">
         <v>374</v>
       </c>
-      <c r="D21" s="197">
+      <c r="D21" s="184">
         <v>4</v>
       </c>
       <c r="E21" s="7" t="s">
@@ -10431,7 +10436,7 @@
       <c r="C22" s="69" t="s">
         <v>375</v>
       </c>
-      <c r="D22" s="198"/>
+      <c r="D22" s="185"/>
       <c r="F22" s="15"/>
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
@@ -10508,7 +10513,7 @@
       <c r="C25" s="69" t="s">
         <v>378</v>
       </c>
-      <c r="D25" s="197">
+      <c r="D25" s="184">
         <v>4</v>
       </c>
       <c r="E25" s="7" t="s">
@@ -10531,7 +10536,7 @@
       <c r="C26" s="69" t="s">
         <v>379</v>
       </c>
-      <c r="D26" s="199"/>
+      <c r="D26" s="186"/>
       <c r="F26" s="15"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -10544,7 +10549,7 @@
       <c r="C27" s="69" t="s">
         <v>380</v>
       </c>
-      <c r="D27" s="197">
+      <c r="D27" s="184">
         <v>4</v>
       </c>
       <c r="E27" s="7" t="s">
@@ -10568,7 +10573,7 @@
       <c r="C28" s="69" t="s">
         <v>381</v>
       </c>
-      <c r="D28" s="199"/>
+      <c r="D28" s="186"/>
       <c r="F28" s="15"/>
       <c r="H28" s="14"/>
       <c r="I28" s="27"/>
@@ -10587,7 +10592,7 @@
       <c r="C29" s="69" t="s">
         <v>382</v>
       </c>
-      <c r="D29" s="197">
+      <c r="D29" s="184">
         <v>4</v>
       </c>
       <c r="E29" s="7" t="s">
@@ -10611,7 +10616,7 @@
       <c r="C30" s="69" t="s">
         <v>383</v>
       </c>
-      <c r="D30" s="199"/>
+      <c r="D30" s="186"/>
       <c r="F30" s="15"/>
       <c r="H30" s="14"/>
       <c r="I30" s="27"/>
@@ -10621,16 +10626,16 @@
       <c r="M30" s="24"/>
     </row>
     <row r="31" spans="1:13" ht="92.4" x14ac:dyDescent="0.25">
-      <c r="A31" s="195" t="s">
+      <c r="A31" s="192" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="195" t="s">
+      <c r="B31" s="192" t="s">
         <v>40</v>
       </c>
       <c r="C31" s="69" t="s">
         <v>384</v>
       </c>
-      <c r="D31" s="197">
+      <c r="D31" s="184">
         <v>4</v>
       </c>
       <c r="E31" s="7" t="s">
@@ -10655,12 +10660,12 @@
       <c r="M31" s="14"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="196"/>
-      <c r="B32" s="196"/>
+      <c r="A32" s="193"/>
+      <c r="B32" s="193"/>
       <c r="C32" s="69" t="s">
         <v>385</v>
       </c>
-      <c r="D32" s="199"/>
+      <c r="D32" s="186"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
@@ -10701,7 +10706,7 @@
       <c r="C34" s="69" t="s">
         <v>387</v>
       </c>
-      <c r="D34" s="197">
+      <c r="D34" s="184">
         <v>4</v>
       </c>
       <c r="E34" s="7" t="s">
@@ -10738,7 +10743,7 @@
       <c r="C35" s="69" t="s">
         <v>388</v>
       </c>
-      <c r="D35" s="198"/>
+      <c r="D35" s="185"/>
       <c r="F35" s="20"/>
       <c r="H35" s="14"/>
       <c r="I35" s="27"/>
@@ -10757,7 +10762,7 @@
       <c r="C36" s="69" t="s">
         <v>389</v>
       </c>
-      <c r="D36" s="197">
+      <c r="D36" s="184">
         <v>4</v>
       </c>
       <c r="E36" s="7" t="s">
@@ -10791,7 +10796,7 @@
       <c r="C37" s="69" t="s">
         <v>390</v>
       </c>
-      <c r="D37" s="198"/>
+      <c r="D37" s="185"/>
       <c r="F37" s="21"/>
       <c r="H37" s="14"/>
       <c r="I37" s="27"/>
@@ -10810,7 +10815,7 @@
       <c r="C38" s="69" t="s">
         <v>391</v>
       </c>
-      <c r="D38" s="197">
+      <c r="D38" s="184">
         <v>4</v>
       </c>
       <c r="E38" s="7" t="s">
@@ -10843,7 +10848,7 @@
       <c r="C39" s="69" t="s">
         <v>392</v>
       </c>
-      <c r="D39" s="198"/>
+      <c r="D39" s="185"/>
       <c r="F39" s="20"/>
       <c r="H39" s="14"/>
       <c r="I39" s="14"/>
@@ -10862,7 +10867,7 @@
       <c r="C40" s="69" t="s">
         <v>393</v>
       </c>
-      <c r="D40" s="197">
+      <c r="D40" s="184">
         <v>4</v>
       </c>
       <c r="E40" s="7" t="s">
@@ -10895,7 +10900,7 @@
       <c r="C41" s="69" t="s">
         <v>394</v>
       </c>
-      <c r="D41" s="198"/>
+      <c r="D41" s="185"/>
       <c r="F41" s="21"/>
       <c r="H41" s="14"/>
       <c r="I41" s="14"/>
@@ -10914,7 +10919,7 @@
       <c r="C42" s="69" t="s">
         <v>395</v>
       </c>
-      <c r="D42" s="197">
+      <c r="D42" s="184">
         <v>4</v>
       </c>
       <c r="E42" s="7" t="s">
@@ -10944,7 +10949,7 @@
       <c r="C43" s="69" t="s">
         <v>396</v>
       </c>
-      <c r="D43" s="198"/>
+      <c r="D43" s="185"/>
       <c r="F43" s="19"/>
       <c r="H43" s="14"/>
       <c r="I43" s="14"/>
@@ -11096,7 +11101,7 @@
       <c r="C48" s="69" t="s">
         <v>401</v>
       </c>
-      <c r="D48" s="197">
+      <c r="D48" s="184">
         <v>4</v>
       </c>
       <c r="F48" s="15" t="s">
@@ -11125,7 +11130,7 @@
       <c r="C49" s="69" t="s">
         <v>402</v>
       </c>
-      <c r="D49" s="198"/>
+      <c r="D49" s="185"/>
       <c r="F49" s="16"/>
       <c r="H49" s="14"/>
       <c r="I49" s="14"/>
@@ -11144,7 +11149,7 @@
       <c r="C50" s="69" t="s">
         <v>403</v>
       </c>
-      <c r="D50" s="197">
+      <c r="D50" s="184">
         <v>4</v>
       </c>
       <c r="F50" s="19" t="s">
@@ -11173,7 +11178,7 @@
       <c r="C51" s="69" t="s">
         <v>404</v>
       </c>
-      <c r="D51" s="199"/>
+      <c r="D51" s="186"/>
       <c r="F51" s="19"/>
       <c r="H51" s="14"/>
       <c r="I51" s="14"/>
@@ -11192,7 +11197,7 @@
       <c r="C52" s="69" t="s">
         <v>405</v>
       </c>
-      <c r="D52" s="197">
+      <c r="D52" s="184">
         <v>4</v>
       </c>
       <c r="E52" s="7" t="s">
@@ -11224,7 +11229,7 @@
       <c r="C53" s="69" t="s">
         <v>406</v>
       </c>
-      <c r="D53" s="198"/>
+      <c r="D53" s="185"/>
       <c r="F53" s="19"/>
       <c r="H53" s="14"/>
       <c r="I53" s="14"/>
@@ -11243,7 +11248,7 @@
       <c r="C54" s="69" t="s">
         <v>407</v>
       </c>
-      <c r="D54" s="197">
+      <c r="D54" s="184">
         <v>4</v>
       </c>
       <c r="F54" s="19" t="s">
@@ -11272,7 +11277,7 @@
       <c r="C55" s="69" t="s">
         <v>408</v>
       </c>
-      <c r="D55" s="199"/>
+      <c r="D55" s="186"/>
       <c r="F55" s="19"/>
       <c r="H55" s="14"/>
       <c r="I55" s="14"/>
@@ -11291,7 +11296,7 @@
       <c r="C56" s="69" t="s">
         <v>409</v>
       </c>
-      <c r="D56" s="197">
+      <c r="D56" s="184">
         <v>4</v>
       </c>
       <c r="E56" s="7" t="s">
@@ -11323,7 +11328,7 @@
       <c r="C57" s="69" t="s">
         <v>410</v>
       </c>
-      <c r="D57" s="198"/>
+      <c r="D57" s="185"/>
       <c r="F57" s="19"/>
       <c r="H57" s="14"/>
       <c r="I57" s="14"/>
@@ -11342,7 +11347,7 @@
       <c r="C58" s="69" t="s">
         <v>411</v>
       </c>
-      <c r="D58" s="197">
+      <c r="D58" s="184">
         <v>4</v>
       </c>
       <c r="F58" s="19" t="s">
@@ -11371,7 +11376,7 @@
       <c r="C59" s="69" t="s">
         <v>412</v>
       </c>
-      <c r="D59" s="199"/>
+      <c r="D59" s="186"/>
       <c r="F59" s="19"/>
       <c r="H59" s="14"/>
       <c r="I59" s="14"/>
@@ -11390,7 +11395,7 @@
       <c r="C60" s="69" t="s">
         <v>413</v>
       </c>
-      <c r="D60" s="197">
+      <c r="D60" s="184">
         <v>4</v>
       </c>
       <c r="E60" s="7" t="s">
@@ -11422,7 +11427,7 @@
       <c r="C61" s="69" t="s">
         <v>414</v>
       </c>
-      <c r="D61" s="198"/>
+      <c r="D61" s="185"/>
       <c r="F61" s="19"/>
       <c r="H61" s="14"/>
       <c r="I61" s="14"/>
@@ -11441,7 +11446,7 @@
       <c r="C62" s="69" t="s">
         <v>415</v>
       </c>
-      <c r="D62" s="197">
+      <c r="D62" s="184">
         <v>4</v>
       </c>
       <c r="F62" s="19" t="s">
@@ -11470,7 +11475,7 @@
       <c r="C63" s="69" t="s">
         <v>416</v>
       </c>
-      <c r="D63" s="199"/>
+      <c r="D63" s="186"/>
       <c r="F63" s="19"/>
       <c r="H63" s="14"/>
       <c r="I63" s="14"/>
@@ -11489,7 +11494,7 @@
       <c r="C64" s="69" t="s">
         <v>417</v>
       </c>
-      <c r="D64" s="197">
+      <c r="D64" s="184">
         <v>4</v>
       </c>
       <c r="E64" s="7" t="s">
@@ -11521,7 +11526,7 @@
       <c r="C65" s="69" t="s">
         <v>418</v>
       </c>
-      <c r="D65" s="198"/>
+      <c r="D65" s="185"/>
       <c r="F65" s="19"/>
       <c r="H65" s="14"/>
       <c r="I65" s="14"/>
@@ -11540,7 +11545,7 @@
       <c r="C66" s="69" t="s">
         <v>419</v>
       </c>
-      <c r="D66" s="197">
+      <c r="D66" s="184">
         <v>4</v>
       </c>
       <c r="F66" s="19" t="s">
@@ -11569,7 +11574,7 @@
       <c r="C67" s="69" t="s">
         <v>420</v>
       </c>
-      <c r="D67" s="199"/>
+      <c r="D67" s="186"/>
       <c r="F67" s="19"/>
       <c r="H67" s="14"/>
       <c r="I67" s="14"/>
@@ -11588,7 +11593,7 @@
       <c r="C68" s="69" t="s">
         <v>421</v>
       </c>
-      <c r="D68" s="197">
+      <c r="D68" s="184">
         <v>4</v>
       </c>
       <c r="E68" s="7" t="s">
@@ -11620,7 +11625,7 @@
       <c r="C69" s="69" t="s">
         <v>422</v>
       </c>
-      <c r="D69" s="198"/>
+      <c r="D69" s="185"/>
       <c r="F69" s="19"/>
       <c r="H69" s="14"/>
       <c r="I69" s="14"/>
@@ -11694,7 +11699,7 @@
       <c r="C72" s="69" t="s">
         <v>425</v>
       </c>
-      <c r="D72" s="197">
+      <c r="D72" s="184">
         <v>4</v>
       </c>
       <c r="E72" s="7" t="s">
@@ -11726,7 +11731,7 @@
       <c r="C73" s="69" t="s">
         <v>426</v>
       </c>
-      <c r="D73" s="198"/>
+      <c r="D73" s="185"/>
       <c r="F73" s="15"/>
       <c r="H73" s="14"/>
       <c r="I73" s="14"/>
@@ -11745,7 +11750,7 @@
       <c r="C74" s="69" t="s">
         <v>427</v>
       </c>
-      <c r="D74" s="197">
+      <c r="D74" s="184">
         <v>4</v>
       </c>
       <c r="E74" s="7" t="s">
@@ -11777,7 +11782,7 @@
       <c r="C75" s="69" t="s">
         <v>428</v>
       </c>
-      <c r="D75" s="198"/>
+      <c r="D75" s="185"/>
       <c r="F75" s="15"/>
       <c r="H75" s="14"/>
       <c r="I75" s="14"/>
@@ -12036,7 +12041,7 @@
       <c r="C84" s="69" t="s">
         <v>437</v>
       </c>
-      <c r="D84" s="197">
+      <c r="D84" s="184">
         <v>4</v>
       </c>
       <c r="E84" s="7" t="s">
@@ -12066,7 +12071,7 @@
       <c r="C85" s="69" t="s">
         <v>438</v>
       </c>
-      <c r="D85" s="198"/>
+      <c r="D85" s="185"/>
       <c r="F85" s="16"/>
       <c r="H85" s="14"/>
       <c r="I85" s="14"/>
@@ -12231,16 +12236,16 @@
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A93" s="195" t="s">
+      <c r="A93" s="192" t="s">
         <v>99</v>
       </c>
-      <c r="B93" s="192" t="s">
+      <c r="B93" s="194" t="s">
         <v>315</v>
       </c>
       <c r="C93" s="69" t="s">
         <v>446</v>
       </c>
-      <c r="D93" s="197">
+      <c r="D93" s="184">
         <v>4</v>
       </c>
       <c r="E93" s="7" t="s">
@@ -12251,25 +12256,25 @@
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A94" s="196"/>
-      <c r="B94" s="196"/>
+      <c r="A94" s="193"/>
+      <c r="B94" s="193"/>
       <c r="C94" s="69" t="s">
         <v>447</v>
       </c>
-      <c r="D94" s="198"/>
+      <c r="D94" s="185"/>
       <c r="F94" s="7"/>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A95" s="195" t="s">
+      <c r="A95" s="192" t="s">
         <v>99</v>
       </c>
-      <c r="B95" s="192" t="s">
+      <c r="B95" s="194" t="s">
         <v>314</v>
       </c>
       <c r="C95" s="69" t="s">
         <v>448</v>
       </c>
-      <c r="D95" s="197">
+      <c r="D95" s="184">
         <v>4</v>
       </c>
       <c r="E95" s="7" t="s">
@@ -12280,12 +12285,12 @@
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A96" s="196"/>
-      <c r="B96" s="196"/>
+      <c r="A96" s="193"/>
+      <c r="B96" s="193"/>
       <c r="C96" s="69" t="s">
         <v>449</v>
       </c>
-      <c r="D96" s="198"/>
+      <c r="D96" s="185"/>
     </row>
     <row r="97" spans="1:11" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
@@ -12332,7 +12337,7 @@
       <c r="C99" s="69" t="s">
         <v>452</v>
       </c>
-      <c r="D99" s="197">
+      <c r="D99" s="184">
         <v>4</v>
       </c>
       <c r="E99" s="7" t="s">
@@ -12353,7 +12358,7 @@
       <c r="C100" s="69" t="s">
         <v>306</v>
       </c>
-      <c r="D100" s="198"/>
+      <c r="D100" s="185"/>
       <c r="E100" s="7"/>
       <c r="F100" s="16"/>
       <c r="G100" s="79"/>
@@ -12370,7 +12375,7 @@
       <c r="C101" s="69" t="s">
         <v>312</v>
       </c>
-      <c r="D101" s="197">
+      <c r="D101" s="184">
         <v>4</v>
       </c>
       <c r="E101" s="7" t="s">
@@ -12391,7 +12396,7 @@
       <c r="C102" s="69" t="s">
         <v>311</v>
       </c>
-      <c r="D102" s="198"/>
+      <c r="D102" s="185"/>
       <c r="F102" s="16"/>
       <c r="G102" s="79"/>
       <c r="H102" s="32"/>
@@ -12425,7 +12430,7 @@
       <c r="C104" s="70" t="s">
         <v>302</v>
       </c>
-      <c r="D104" s="203">
+      <c r="D104" s="187">
         <v>4</v>
       </c>
       <c r="E104" s="35" t="s">
@@ -12450,7 +12455,7 @@
       <c r="C105" s="70" t="s">
         <v>303</v>
       </c>
-      <c r="D105" s="204"/>
+      <c r="D105" s="188"/>
       <c r="E105" s="35"/>
       <c r="F105" s="36"/>
       <c r="G105" s="80"/>
@@ -12467,7 +12472,7 @@
       <c r="C106" s="70" t="s">
         <v>304</v>
       </c>
-      <c r="D106" s="203">
+      <c r="D106" s="187">
         <v>4</v>
       </c>
       <c r="E106" s="35" t="s">
@@ -12492,7 +12497,7 @@
       <c r="C107" s="70" t="s">
         <v>305</v>
       </c>
-      <c r="D107" s="204"/>
+      <c r="D107" s="188"/>
       <c r="E107" s="35"/>
       <c r="F107" s="36"/>
       <c r="G107" s="80"/>
@@ -13392,18 +13397,25 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D104:D105"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="A5:A12"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="D5:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="A95:A96"/>
+    <mergeCell ref="B5:B12"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B93:B94"/>
+    <mergeCell ref="B95:B96"/>
+    <mergeCell ref="A93:A94"/>
     <mergeCell ref="D106:D107"/>
     <mergeCell ref="F5:F12"/>
     <mergeCell ref="D74:D75"/>
@@ -13420,25 +13432,18 @@
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="D50:D51"/>
     <mergeCell ref="D52:D53"/>
-    <mergeCell ref="A95:A96"/>
-    <mergeCell ref="B5:B12"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B93:B94"/>
-    <mergeCell ref="B95:B96"/>
-    <mergeCell ref="A93:A94"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="A5:A12"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="D5:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D104:D105"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="D38:D39"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51" footer="0.51"/>
@@ -13451,7 +13456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C842772-46F4-4927-B032-D056DFDFA6B1}">
   <dimension ref="A1:L105"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B77" workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
@@ -13472,13 +13477,13 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="89"/>
-      <c r="B1" s="210" t="s">
+      <c r="B1" s="227" t="s">
         <v>479</v>
       </c>
-      <c r="C1" s="210"/>
-      <c r="D1" s="210"/>
-      <c r="E1" s="210"/>
-      <c r="F1" s="210"/>
+      <c r="C1" s="227"/>
+      <c r="D1" s="227"/>
+      <c r="E1" s="227"/>
+      <c r="F1" s="227"/>
       <c r="G1" s="90"/>
       <c r="H1" s="91"/>
       <c r="I1" s="90"/>
@@ -13523,159 +13528,159 @@
       </c>
     </row>
     <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="211" t="s">
+      <c r="A3" s="210" t="s">
         <v>487</v>
       </c>
-      <c r="B3" s="211" t="s">
+      <c r="B3" s="210" t="s">
         <v>488</v>
       </c>
       <c r="C3" s="92" t="s">
         <v>351</v>
       </c>
-      <c r="D3" s="208">
+      <c r="D3" s="222">
         <v>16</v>
       </c>
       <c r="E3" s="93"/>
-      <c r="F3" s="215" t="s">
+      <c r="F3" s="230" t="s">
         <v>489</v>
       </c>
       <c r="G3" s="94"/>
       <c r="H3" s="27" t="s">
         <v>490</v>
       </c>
-      <c r="I3" s="211" t="s">
+      <c r="I3" s="210" t="s">
         <v>475</v>
       </c>
-      <c r="J3" s="224" t="s">
+      <c r="J3" s="219" t="s">
         <v>476</v>
       </c>
-      <c r="K3" s="211"/>
+      <c r="K3" s="210"/>
       <c r="L3" s="125"/>
     </row>
     <row r="4" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="212"/>
-      <c r="B4" s="212"/>
+      <c r="A4" s="228"/>
+      <c r="B4" s="228"/>
       <c r="C4" s="92" t="s">
         <v>348</v>
       </c>
-      <c r="D4" s="209"/>
+      <c r="D4" s="223"/>
       <c r="E4" s="93"/>
-      <c r="F4" s="216"/>
+      <c r="F4" s="231"/>
       <c r="G4" s="94"/>
       <c r="H4" s="27" t="s">
         <v>490</v>
       </c>
-      <c r="I4" s="223"/>
-      <c r="J4" s="225"/>
-      <c r="K4" s="223"/>
+      <c r="I4" s="218"/>
+      <c r="J4" s="220"/>
+      <c r="K4" s="218"/>
       <c r="L4" s="126"/>
     </row>
     <row r="5" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="212"/>
-      <c r="B5" s="212"/>
+      <c r="A5" s="228"/>
+      <c r="B5" s="228"/>
       <c r="C5" s="92" t="s">
         <v>350</v>
       </c>
-      <c r="D5" s="209"/>
+      <c r="D5" s="223"/>
       <c r="E5" s="93"/>
-      <c r="F5" s="216"/>
+      <c r="F5" s="231"/>
       <c r="G5" s="94"/>
       <c r="H5" s="27" t="s">
         <v>490</v>
       </c>
-      <c r="I5" s="223"/>
-      <c r="J5" s="225"/>
-      <c r="K5" s="223"/>
+      <c r="I5" s="218"/>
+      <c r="J5" s="220"/>
+      <c r="K5" s="218"/>
       <c r="L5" s="126"/>
     </row>
     <row r="6" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="212"/>
-      <c r="B6" s="212"/>
+      <c r="A6" s="228"/>
+      <c r="B6" s="228"/>
       <c r="C6" s="92" t="s">
         <v>349</v>
       </c>
-      <c r="D6" s="209"/>
+      <c r="D6" s="223"/>
       <c r="E6" s="93"/>
-      <c r="F6" s="216"/>
+      <c r="F6" s="231"/>
       <c r="G6" s="94"/>
       <c r="H6" s="27" t="s">
         <v>490</v>
       </c>
-      <c r="I6" s="223"/>
-      <c r="J6" s="225"/>
-      <c r="K6" s="223"/>
+      <c r="I6" s="218"/>
+      <c r="J6" s="220"/>
+      <c r="K6" s="218"/>
       <c r="L6" s="126"/>
     </row>
     <row r="7" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="212"/>
-      <c r="B7" s="212"/>
+      <c r="A7" s="228"/>
+      <c r="B7" s="228"/>
       <c r="C7" s="92" t="s">
         <v>352</v>
       </c>
-      <c r="D7" s="209"/>
+      <c r="D7" s="223"/>
       <c r="E7" s="93"/>
-      <c r="F7" s="216"/>
+      <c r="F7" s="231"/>
       <c r="G7" s="94"/>
       <c r="H7" s="27" t="s">
         <v>490</v>
       </c>
-      <c r="I7" s="223"/>
-      <c r="J7" s="225"/>
-      <c r="K7" s="223"/>
+      <c r="I7" s="218"/>
+      <c r="J7" s="220"/>
+      <c r="K7" s="218"/>
       <c r="L7" s="126"/>
     </row>
     <row r="8" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="212"/>
-      <c r="B8" s="212"/>
+      <c r="A8" s="228"/>
+      <c r="B8" s="228"/>
       <c r="C8" s="92" t="s">
         <v>363</v>
       </c>
-      <c r="D8" s="209"/>
+      <c r="D8" s="223"/>
       <c r="E8" s="93"/>
-      <c r="F8" s="216"/>
+      <c r="F8" s="231"/>
       <c r="G8" s="94"/>
       <c r="H8" s="27" t="s">
         <v>490</v>
       </c>
-      <c r="I8" s="223"/>
-      <c r="J8" s="225"/>
-      <c r="K8" s="223"/>
+      <c r="I8" s="218"/>
+      <c r="J8" s="220"/>
+      <c r="K8" s="218"/>
       <c r="L8" s="126"/>
     </row>
     <row r="9" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="212"/>
-      <c r="B9" s="212"/>
+      <c r="A9" s="228"/>
+      <c r="B9" s="228"/>
       <c r="C9" s="92" t="s">
         <v>364</v>
       </c>
-      <c r="D9" s="209"/>
+      <c r="D9" s="223"/>
       <c r="E9" s="93"/>
-      <c r="F9" s="216"/>
+      <c r="F9" s="231"/>
       <c r="G9" s="94"/>
       <c r="H9" s="27" t="s">
         <v>490</v>
       </c>
-      <c r="I9" s="223"/>
-      <c r="J9" s="225"/>
-      <c r="K9" s="223"/>
+      <c r="I9" s="218"/>
+      <c r="J9" s="220"/>
+      <c r="K9" s="218"/>
       <c r="L9" s="126"/>
     </row>
     <row r="10" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="213"/>
-      <c r="B10" s="213"/>
+      <c r="A10" s="229"/>
+      <c r="B10" s="229"/>
       <c r="C10" s="92" t="s">
         <v>365</v>
       </c>
-      <c r="D10" s="214"/>
+      <c r="D10" s="224"/>
       <c r="E10" s="93"/>
-      <c r="F10" s="217"/>
+      <c r="F10" s="232"/>
       <c r="G10" s="94"/>
       <c r="H10" s="27" t="s">
         <v>490</v>
       </c>
-      <c r="I10" s="220"/>
-      <c r="J10" s="226"/>
-      <c r="K10" s="220"/>
+      <c r="I10" s="211"/>
+      <c r="J10" s="221"/>
+      <c r="K10" s="211"/>
       <c r="L10" s="127"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -13688,7 +13693,7 @@
       <c r="C11" s="92" t="s">
         <v>366</v>
       </c>
-      <c r="D11" s="208">
+      <c r="D11" s="222">
         <v>4</v>
       </c>
       <c r="E11" s="85" t="s">
@@ -13704,7 +13709,7 @@
       <c r="I11" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="224" t="s">
+      <c r="J11" s="219" t="s">
         <v>604</v>
       </c>
       <c r="K11" s="27">
@@ -13725,13 +13730,13 @@
       <c r="C12" s="92" t="s">
         <v>367</v>
       </c>
-      <c r="D12" s="214"/>
+      <c r="D12" s="224"/>
       <c r="E12" s="85"/>
       <c r="F12" s="96"/>
       <c r="G12" s="97"/>
       <c r="H12" s="27"/>
       <c r="I12" s="27"/>
-      <c r="J12" s="226"/>
+      <c r="J12" s="221"/>
       <c r="K12" s="88">
         <v>-9999999</v>
       </c>
@@ -13750,7 +13755,7 @@
       <c r="C13" s="92" t="s">
         <v>368</v>
       </c>
-      <c r="D13" s="208">
+      <c r="D13" s="222">
         <v>4</v>
       </c>
       <c r="E13" s="85" t="s">
@@ -13766,7 +13771,7 @@
       <c r="I13" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="J13" s="227" t="s">
+      <c r="J13" s="214" t="s">
         <v>607</v>
       </c>
       <c r="K13" s="27">
@@ -13787,13 +13792,13 @@
       <c r="C14" s="92" t="s">
         <v>369</v>
       </c>
-      <c r="D14" s="214"/>
+      <c r="D14" s="224"/>
       <c r="E14" s="85"/>
       <c r="F14" s="96"/>
       <c r="G14" s="97"/>
       <c r="H14" s="27"/>
       <c r="I14" s="27"/>
-      <c r="J14" s="228"/>
+      <c r="J14" s="215"/>
       <c r="K14" s="27">
         <v>-2000000</v>
       </c>
@@ -13812,7 +13817,7 @@
       <c r="C15" s="92" t="s">
         <v>370</v>
       </c>
-      <c r="D15" s="208">
+      <c r="D15" s="222">
         <v>4</v>
       </c>
       <c r="E15" s="85" t="s">
@@ -13828,7 +13833,7 @@
       <c r="I15" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="227" t="s">
+      <c r="J15" s="214" t="s">
         <v>607</v>
       </c>
       <c r="K15" s="27">
@@ -13849,13 +13854,13 @@
       <c r="C16" s="92" t="s">
         <v>371</v>
       </c>
-      <c r="D16" s="214"/>
+      <c r="D16" s="224"/>
       <c r="E16" s="85"/>
       <c r="F16" s="98"/>
       <c r="G16" s="97"/>
       <c r="H16" s="27"/>
       <c r="I16" s="27"/>
-      <c r="J16" s="228"/>
+      <c r="J16" s="215"/>
       <c r="K16" s="27">
         <v>-2000000</v>
       </c>
@@ -13874,7 +13879,7 @@
       <c r="C17" s="92" t="s">
         <v>372</v>
       </c>
-      <c r="D17" s="208">
+      <c r="D17" s="222">
         <v>4</v>
       </c>
       <c r="E17" s="85" t="s">
@@ -13892,7 +13897,7 @@
       <c r="I17" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="227" t="s">
+      <c r="J17" s="214" t="s">
         <v>604</v>
       </c>
       <c r="K17" s="27">
@@ -13913,13 +13918,13 @@
       <c r="C18" s="92" t="s">
         <v>373</v>
       </c>
-      <c r="D18" s="214"/>
+      <c r="D18" s="224"/>
       <c r="E18" s="85"/>
       <c r="F18" s="98"/>
       <c r="G18" s="97"/>
       <c r="H18" s="27"/>
       <c r="I18" s="27"/>
-      <c r="J18" s="228"/>
+      <c r="J18" s="215"/>
       <c r="K18" s="27">
         <v>0</v>
       </c>
@@ -13938,7 +13943,7 @@
       <c r="C19" s="92" t="s">
         <v>374</v>
       </c>
-      <c r="D19" s="208">
+      <c r="D19" s="222">
         <v>4</v>
       </c>
       <c r="E19" s="85" t="s">
@@ -13954,7 +13959,7 @@
       <c r="I19" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="227" t="s">
+      <c r="J19" s="214" t="s">
         <v>604</v>
       </c>
       <c r="K19" s="27">
@@ -13975,13 +13980,13 @@
       <c r="C20" s="92" t="s">
         <v>375</v>
       </c>
-      <c r="D20" s="214"/>
+      <c r="D20" s="224"/>
       <c r="E20" s="85"/>
       <c r="F20" s="96"/>
       <c r="G20" s="97"/>
       <c r="H20" s="27"/>
       <c r="I20" s="27"/>
-      <c r="J20" s="228"/>
+      <c r="J20" s="215"/>
       <c r="K20" s="27">
         <v>0</v>
       </c>
@@ -14069,7 +14074,7 @@
       <c r="C23" s="92" t="s">
         <v>378</v>
       </c>
-      <c r="D23" s="208">
+      <c r="D23" s="222">
         <v>4</v>
       </c>
       <c r="E23" s="85" t="s">
@@ -14085,7 +14090,7 @@
         <v>493</v>
       </c>
       <c r="I23" s="92"/>
-      <c r="J23" s="227" t="s">
+      <c r="J23" s="214" t="s">
         <v>604</v>
       </c>
       <c r="K23" s="27">
@@ -14104,13 +14109,13 @@
       <c r="C24" s="92" t="s">
         <v>379</v>
       </c>
-      <c r="D24" s="209"/>
+      <c r="D24" s="223"/>
       <c r="E24" s="85"/>
       <c r="F24" s="96"/>
       <c r="G24" s="97"/>
       <c r="H24" s="92"/>
       <c r="I24" s="92"/>
-      <c r="J24" s="228"/>
+      <c r="J24" s="215"/>
       <c r="K24" s="27">
         <v>-9999999</v>
       </c>
@@ -14129,7 +14134,7 @@
       <c r="C25" s="92" t="s">
         <v>380</v>
       </c>
-      <c r="D25" s="208">
+      <c r="D25" s="222">
         <v>4</v>
       </c>
       <c r="E25" s="85" t="s">
@@ -14145,7 +14150,7 @@
         <v>493</v>
       </c>
       <c r="I25" s="92"/>
-      <c r="J25" s="227" t="s">
+      <c r="J25" s="214" t="s">
         <v>604</v>
       </c>
       <c r="K25" s="27">
@@ -14164,13 +14169,13 @@
       <c r="C26" s="92" t="s">
         <v>381</v>
       </c>
-      <c r="D26" s="209"/>
+      <c r="D26" s="223"/>
       <c r="E26" s="85"/>
       <c r="F26" s="96"/>
       <c r="G26" s="97"/>
       <c r="H26" s="27"/>
       <c r="I26" s="27"/>
-      <c r="J26" s="228"/>
+      <c r="J26" s="215"/>
       <c r="K26" s="27">
         <v>-9999999</v>
       </c>
@@ -14189,7 +14194,7 @@
       <c r="C27" s="92" t="s">
         <v>382</v>
       </c>
-      <c r="D27" s="208">
+      <c r="D27" s="222">
         <v>4</v>
       </c>
       <c r="E27" s="85" t="s">
@@ -14205,7 +14210,7 @@
         <v>493</v>
       </c>
       <c r="I27" s="92"/>
-      <c r="J27" s="227" t="s">
+      <c r="J27" s="214" t="s">
         <v>604</v>
       </c>
       <c r="K27" s="27">
@@ -14224,13 +14229,13 @@
       <c r="C28" s="92" t="s">
         <v>383</v>
       </c>
-      <c r="D28" s="209"/>
+      <c r="D28" s="223"/>
       <c r="E28" s="85"/>
       <c r="F28" s="96"/>
       <c r="G28" s="97"/>
       <c r="H28" s="27"/>
       <c r="I28" s="27"/>
-      <c r="J28" s="228"/>
+      <c r="J28" s="215"/>
       <c r="K28" s="27">
         <v>-9999999</v>
       </c>
@@ -14240,16 +14245,16 @@
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="211" t="s">
+      <c r="A29" s="210" t="s">
         <v>491</v>
       </c>
-      <c r="B29" s="211" t="s">
+      <c r="B29" s="210" t="s">
         <v>513</v>
       </c>
       <c r="C29" s="92" t="s">
         <v>384</v>
       </c>
-      <c r="D29" s="208">
+      <c r="D29" s="222">
         <v>4</v>
       </c>
       <c r="E29" s="85" t="s">
@@ -14265,7 +14270,7 @@
       <c r="I29" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="J29" s="227" t="s">
+      <c r="J29" s="214" t="s">
         <v>604</v>
       </c>
       <c r="K29" s="27">
@@ -14277,18 +14282,18 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="220"/>
-      <c r="B30" s="220"/>
+      <c r="A30" s="211"/>
+      <c r="B30" s="211"/>
       <c r="C30" s="92" t="s">
         <v>385</v>
       </c>
-      <c r="D30" s="209"/>
+      <c r="D30" s="223"/>
       <c r="E30" s="85"/>
       <c r="F30" s="99"/>
       <c r="G30" s="97"/>
       <c r="H30" s="92"/>
       <c r="I30" s="92"/>
-      <c r="J30" s="228"/>
+      <c r="J30" s="215"/>
       <c r="K30" s="27">
         <v>0</v>
       </c>
@@ -14344,7 +14349,7 @@
       <c r="C32" s="92" t="s">
         <v>387</v>
       </c>
-      <c r="D32" s="208">
+      <c r="D32" s="222">
         <v>4</v>
       </c>
       <c r="E32" s="85" t="s">
@@ -14362,7 +14367,7 @@
       <c r="I32" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J32" s="227" t="s">
+      <c r="J32" s="214" t="s">
         <v>609</v>
       </c>
       <c r="K32" s="27">
@@ -14383,13 +14388,13 @@
       <c r="C33" s="92" t="s">
         <v>388</v>
       </c>
-      <c r="D33" s="214"/>
+      <c r="D33" s="224"/>
       <c r="E33" s="85"/>
       <c r="F33" s="102"/>
       <c r="G33" s="97"/>
       <c r="H33" s="27"/>
       <c r="I33" s="27"/>
-      <c r="J33" s="228"/>
+      <c r="J33" s="215"/>
       <c r="K33" s="27">
         <v>0</v>
       </c>
@@ -14408,7 +14413,7 @@
       <c r="C34" s="92" t="s">
         <v>389</v>
       </c>
-      <c r="D34" s="208">
+      <c r="D34" s="222">
         <v>4</v>
       </c>
       <c r="E34" s="85" t="s">
@@ -14424,7 +14429,7 @@
       <c r="I34" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="J34" s="227" t="s">
+      <c r="J34" s="214" t="s">
         <v>610</v>
       </c>
       <c r="K34" s="27">
@@ -14445,13 +14450,13 @@
       <c r="C35" s="92" t="s">
         <v>390</v>
       </c>
-      <c r="D35" s="214"/>
+      <c r="D35" s="224"/>
       <c r="E35" s="85"/>
       <c r="F35" s="128"/>
       <c r="G35" s="97"/>
       <c r="H35" s="27"/>
       <c r="I35" s="27"/>
-      <c r="J35" s="228"/>
+      <c r="J35" s="215"/>
       <c r="K35" s="27">
         <v>0</v>
       </c>
@@ -14470,7 +14475,7 @@
       <c r="C36" s="92" t="s">
         <v>391</v>
       </c>
-      <c r="D36" s="208">
+      <c r="D36" s="222">
         <v>4</v>
       </c>
       <c r="E36" s="85" t="s">
@@ -14488,7 +14493,7 @@
       <c r="I36" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J36" s="227" t="s">
+      <c r="J36" s="214" t="s">
         <v>609</v>
       </c>
       <c r="K36" s="27">
@@ -14509,13 +14514,13 @@
       <c r="C37" s="92" t="s">
         <v>392</v>
       </c>
-      <c r="D37" s="214"/>
+      <c r="D37" s="224"/>
       <c r="E37" s="85"/>
       <c r="F37" s="102"/>
       <c r="G37" s="97"/>
       <c r="H37" s="27"/>
       <c r="I37" s="27"/>
-      <c r="J37" s="228"/>
+      <c r="J37" s="215"/>
       <c r="K37" s="27">
         <v>0</v>
       </c>
@@ -14534,7 +14539,7 @@
       <c r="C38" s="92" t="s">
         <v>393</v>
       </c>
-      <c r="D38" s="208">
+      <c r="D38" s="222">
         <v>4</v>
       </c>
       <c r="E38" s="85" t="s">
@@ -14552,7 +14557,7 @@
       <c r="I38" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J38" s="227" t="s">
+      <c r="J38" s="214" t="s">
         <v>610</v>
       </c>
       <c r="K38" s="27">
@@ -14573,13 +14578,13 @@
       <c r="C39" s="92" t="s">
         <v>394</v>
       </c>
-      <c r="D39" s="214"/>
+      <c r="D39" s="224"/>
       <c r="E39" s="85"/>
       <c r="F39" s="103"/>
       <c r="G39" s="97"/>
       <c r="H39" s="27"/>
       <c r="I39" s="27"/>
-      <c r="J39" s="228"/>
+      <c r="J39" s="215"/>
       <c r="K39" s="27">
         <v>0</v>
       </c>
@@ -14598,7 +14603,7 @@
       <c r="C40" s="92" t="s">
         <v>395</v>
       </c>
-      <c r="D40" s="208">
+      <c r="D40" s="222">
         <v>4</v>
       </c>
       <c r="E40" s="85" t="s">
@@ -14614,7 +14619,7 @@
       <c r="I40" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="J40" s="227" t="s">
+      <c r="J40" s="214" t="s">
         <v>610</v>
       </c>
       <c r="K40" s="27">
@@ -14635,13 +14640,13 @@
       <c r="C41" s="92" t="s">
         <v>396</v>
       </c>
-      <c r="D41" s="214"/>
+      <c r="D41" s="224"/>
       <c r="E41" s="85"/>
       <c r="F41" s="101"/>
       <c r="G41" s="97"/>
       <c r="H41" s="27"/>
       <c r="I41" s="27"/>
-      <c r="J41" s="228"/>
+      <c r="J41" s="215"/>
       <c r="K41" s="27">
         <v>0</v>
       </c>
@@ -14795,7 +14800,7 @@
       <c r="C46" s="92" t="s">
         <v>401</v>
       </c>
-      <c r="D46" s="208">
+      <c r="D46" s="222">
         <v>4</v>
       </c>
       <c r="E46" s="85"/>
@@ -14809,7 +14814,7 @@
       <c r="I46" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J46" s="227" t="s">
+      <c r="J46" s="214" t="s">
         <v>630</v>
       </c>
       <c r="K46" s="27">
@@ -14830,13 +14835,13 @@
       <c r="C47" s="92" t="s">
         <v>402</v>
       </c>
-      <c r="D47" s="214"/>
+      <c r="D47" s="224"/>
       <c r="E47" s="85"/>
       <c r="F47" s="98"/>
       <c r="G47" s="97"/>
       <c r="H47" s="27"/>
       <c r="I47" s="27"/>
-      <c r="J47" s="228"/>
+      <c r="J47" s="215"/>
       <c r="K47" s="27">
         <v>1</v>
       </c>
@@ -14855,7 +14860,7 @@
       <c r="C48" s="130" t="s">
         <v>403</v>
       </c>
-      <c r="D48" s="218">
+      <c r="D48" s="225">
         <v>4</v>
       </c>
       <c r="E48" s="131"/>
@@ -14869,7 +14874,7 @@
       <c r="I48" s="129" t="s">
         <v>78</v>
       </c>
-      <c r="J48" s="229" t="s">
+      <c r="J48" s="212" t="s">
         <v>630</v>
       </c>
       <c r="K48" s="129"/>
@@ -14885,13 +14890,13 @@
       <c r="C49" s="130" t="s">
         <v>404</v>
       </c>
-      <c r="D49" s="219"/>
+      <c r="D49" s="226"/>
       <c r="E49" s="131"/>
       <c r="F49" s="132"/>
       <c r="G49" s="133"/>
       <c r="H49" s="129"/>
       <c r="I49" s="129"/>
-      <c r="J49" s="230"/>
+      <c r="J49" s="213"/>
       <c r="K49" s="129"/>
       <c r="L49" s="134"/>
     </row>
@@ -14905,7 +14910,7 @@
       <c r="C50" s="92" t="s">
         <v>405</v>
       </c>
-      <c r="D50" s="208">
+      <c r="D50" s="222">
         <v>4</v>
       </c>
       <c r="E50" s="85" t="s">
@@ -14921,7 +14926,7 @@
       <c r="I50" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="J50" s="227" t="s">
+      <c r="J50" s="214" t="s">
         <v>609</v>
       </c>
       <c r="K50" s="27">
@@ -14942,13 +14947,13 @@
       <c r="C51" s="92" t="s">
         <v>406</v>
       </c>
-      <c r="D51" s="214"/>
+      <c r="D51" s="224"/>
       <c r="E51" s="85"/>
       <c r="F51" s="101"/>
       <c r="G51" s="97"/>
       <c r="H51" s="27"/>
       <c r="I51" s="27"/>
-      <c r="J51" s="228"/>
+      <c r="J51" s="215"/>
       <c r="K51" s="27">
         <v>0</v>
       </c>
@@ -14967,7 +14972,7 @@
       <c r="C52" s="92" t="s">
         <v>407</v>
       </c>
-      <c r="D52" s="208">
+      <c r="D52" s="222">
         <v>4</v>
       </c>
       <c r="E52" s="85"/>
@@ -14981,7 +14986,7 @@
       <c r="I52" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="J52" s="227" t="s">
+      <c r="J52" s="214" t="s">
         <v>630</v>
       </c>
       <c r="K52" s="27"/>
@@ -14997,13 +15002,13 @@
       <c r="C53" s="92" t="s">
         <v>408</v>
       </c>
-      <c r="D53" s="209"/>
+      <c r="D53" s="223"/>
       <c r="E53" s="85"/>
       <c r="F53" s="101"/>
       <c r="G53" s="97"/>
       <c r="H53" s="27"/>
       <c r="I53" s="27"/>
-      <c r="J53" s="228"/>
+      <c r="J53" s="215"/>
       <c r="K53" s="27"/>
       <c r="L53" s="118"/>
     </row>
@@ -15017,7 +15022,7 @@
       <c r="C54" s="92" t="s">
         <v>409</v>
       </c>
-      <c r="D54" s="208">
+      <c r="D54" s="222">
         <v>4</v>
       </c>
       <c r="E54" s="85" t="s">
@@ -15033,7 +15038,7 @@
       <c r="I54" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="J54" s="211" t="s">
+      <c r="J54" s="210" t="s">
         <v>609</v>
       </c>
       <c r="K54" s="27">
@@ -15054,13 +15059,13 @@
       <c r="C55" s="92" t="s">
         <v>410</v>
       </c>
-      <c r="D55" s="214"/>
+      <c r="D55" s="224"/>
       <c r="E55" s="85"/>
       <c r="F55" s="101"/>
       <c r="G55" s="97"/>
       <c r="H55" s="27"/>
       <c r="I55" s="27"/>
-      <c r="J55" s="220"/>
+      <c r="J55" s="211"/>
       <c r="K55" s="27">
         <v>0</v>
       </c>
@@ -15078,7 +15083,7 @@
       <c r="C56" s="92" t="s">
         <v>411</v>
       </c>
-      <c r="D56" s="208">
+      <c r="D56" s="222">
         <v>4</v>
       </c>
       <c r="E56" s="85"/>
@@ -15092,7 +15097,7 @@
       <c r="I56" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="J56" s="211" t="s">
+      <c r="J56" s="210" t="s">
         <v>630</v>
       </c>
       <c r="K56" s="27"/>
@@ -15108,13 +15113,13 @@
       <c r="C57" s="92" t="s">
         <v>412</v>
       </c>
-      <c r="D57" s="209"/>
+      <c r="D57" s="223"/>
       <c r="E57" s="85"/>
       <c r="F57" s="101"/>
       <c r="G57" s="97"/>
       <c r="H57" s="27"/>
       <c r="I57" s="27"/>
-      <c r="J57" s="220"/>
+      <c r="J57" s="211"/>
       <c r="K57" s="27"/>
       <c r="L57" s="118"/>
     </row>
@@ -15128,7 +15133,7 @@
       <c r="C58" s="92" t="s">
         <v>413</v>
       </c>
-      <c r="D58" s="208">
+      <c r="D58" s="222">
         <v>4</v>
       </c>
       <c r="E58" s="85" t="s">
@@ -15144,7 +15149,7 @@
       <c r="I58" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="J58" s="211" t="s">
+      <c r="J58" s="210" t="s">
         <v>609</v>
       </c>
       <c r="K58" s="27"/>
@@ -15160,13 +15165,13 @@
       <c r="C59" s="92" t="s">
         <v>414</v>
       </c>
-      <c r="D59" s="214"/>
+      <c r="D59" s="224"/>
       <c r="E59" s="85"/>
       <c r="F59" s="101"/>
       <c r="G59" s="97"/>
       <c r="H59" s="27"/>
       <c r="I59" s="27"/>
-      <c r="J59" s="220"/>
+      <c r="J59" s="211"/>
       <c r="K59" s="27"/>
       <c r="L59" s="118"/>
     </row>
@@ -15180,7 +15185,7 @@
       <c r="C60" s="92" t="s">
         <v>415</v>
       </c>
-      <c r="D60" s="208">
+      <c r="D60" s="222">
         <v>4</v>
       </c>
       <c r="E60" s="85"/>
@@ -15194,7 +15199,7 @@
       <c r="I60" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="J60" s="211" t="s">
+      <c r="J60" s="210" t="s">
         <v>630</v>
       </c>
       <c r="K60" s="27"/>
@@ -15210,13 +15215,13 @@
       <c r="C61" s="92" t="s">
         <v>416</v>
       </c>
-      <c r="D61" s="209"/>
+      <c r="D61" s="223"/>
       <c r="E61" s="85"/>
       <c r="F61" s="101"/>
       <c r="G61" s="97"/>
       <c r="H61" s="27"/>
       <c r="I61" s="27"/>
-      <c r="J61" s="220"/>
+      <c r="J61" s="211"/>
       <c r="K61" s="27"/>
       <c r="L61" s="118"/>
     </row>
@@ -15230,7 +15235,7 @@
       <c r="C62" s="92" t="s">
         <v>417</v>
       </c>
-      <c r="D62" s="208">
+      <c r="D62" s="222">
         <v>4</v>
       </c>
       <c r="E62" s="85" t="s">
@@ -15246,7 +15251,7 @@
       <c r="I62" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="J62" s="211" t="s">
+      <c r="J62" s="210" t="s">
         <v>609</v>
       </c>
       <c r="K62" s="27">
@@ -15267,13 +15272,13 @@
       <c r="C63" s="92" t="s">
         <v>418</v>
       </c>
-      <c r="D63" s="214"/>
+      <c r="D63" s="224"/>
       <c r="E63" s="85"/>
       <c r="F63" s="101"/>
       <c r="G63" s="97"/>
       <c r="H63" s="27"/>
       <c r="I63" s="27"/>
-      <c r="J63" s="220"/>
+      <c r="J63" s="211"/>
       <c r="K63" s="27">
         <v>0</v>
       </c>
@@ -15292,7 +15297,7 @@
       <c r="C64" s="92" t="s">
         <v>419</v>
       </c>
-      <c r="D64" s="208">
+      <c r="D64" s="222">
         <v>4</v>
       </c>
       <c r="E64" s="85"/>
@@ -15306,7 +15311,7 @@
       <c r="I64" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="J64" s="211" t="s">
+      <c r="J64" s="210" t="s">
         <v>630</v>
       </c>
       <c r="K64" s="27"/>
@@ -15322,13 +15327,13 @@
       <c r="C65" s="92" t="s">
         <v>420</v>
       </c>
-      <c r="D65" s="209"/>
+      <c r="D65" s="223"/>
       <c r="E65" s="85"/>
       <c r="F65" s="101"/>
       <c r="G65" s="97"/>
       <c r="H65" s="27"/>
       <c r="I65" s="27"/>
-      <c r="J65" s="220"/>
+      <c r="J65" s="211"/>
       <c r="K65" s="27"/>
       <c r="L65" s="118"/>
     </row>
@@ -15342,7 +15347,7 @@
       <c r="C66" s="92" t="s">
         <v>421</v>
       </c>
-      <c r="D66" s="208">
+      <c r="D66" s="222">
         <v>4</v>
       </c>
       <c r="E66" s="85" t="s">
@@ -15358,7 +15363,7 @@
       <c r="I66" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="J66" s="211" t="s">
+      <c r="J66" s="210" t="s">
         <v>609</v>
       </c>
       <c r="K66" s="27">
@@ -15379,13 +15384,13 @@
       <c r="C67" s="92" t="s">
         <v>422</v>
       </c>
-      <c r="D67" s="214"/>
+      <c r="D67" s="224"/>
       <c r="E67" s="85"/>
       <c r="F67" s="101"/>
       <c r="G67" s="97"/>
       <c r="H67" s="27"/>
       <c r="I67" s="27"/>
-      <c r="J67" s="220"/>
+      <c r="J67" s="211"/>
       <c r="K67" s="27">
         <v>0</v>
       </c>
@@ -15466,7 +15471,7 @@
       <c r="C70" s="92" t="s">
         <v>425</v>
       </c>
-      <c r="D70" s="208">
+      <c r="D70" s="222">
         <v>4</v>
       </c>
       <c r="E70" s="85" t="s">
@@ -15482,7 +15487,7 @@
       <c r="I70" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J70" s="211" t="s">
+      <c r="J70" s="210" t="s">
         <v>607</v>
       </c>
       <c r="K70" s="27">
@@ -15503,13 +15508,13 @@
       <c r="C71" s="92" t="s">
         <v>426</v>
       </c>
-      <c r="D71" s="214"/>
+      <c r="D71" s="224"/>
       <c r="E71" s="85"/>
       <c r="F71" s="96"/>
       <c r="G71" s="97"/>
       <c r="H71" s="27"/>
       <c r="I71" s="27"/>
-      <c r="J71" s="220"/>
+      <c r="J71" s="211"/>
       <c r="K71" s="27">
         <v>30000</v>
       </c>
@@ -15528,7 +15533,7 @@
       <c r="C72" s="92" t="s">
         <v>427</v>
       </c>
-      <c r="D72" s="208">
+      <c r="D72" s="222">
         <v>4</v>
       </c>
       <c r="E72" s="85" t="s">
@@ -15544,7 +15549,7 @@
       <c r="I72" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J72" s="211" t="s">
+      <c r="J72" s="210" t="s">
         <v>607</v>
       </c>
       <c r="K72" s="27">
@@ -15565,13 +15570,13 @@
       <c r="C73" s="92" t="s">
         <v>428</v>
       </c>
-      <c r="D73" s="214"/>
+      <c r="D73" s="224"/>
       <c r="E73" s="85"/>
       <c r="F73" s="96"/>
       <c r="G73" s="97"/>
       <c r="H73" s="27"/>
       <c r="I73" s="27"/>
-      <c r="J73" s="220"/>
+      <c r="J73" s="211"/>
       <c r="K73" s="27">
         <v>10000</v>
       </c>
@@ -15871,7 +15876,7 @@
       <c r="C82" s="92" t="s">
         <v>437</v>
       </c>
-      <c r="D82" s="208">
+      <c r="D82" s="222">
         <v>4</v>
       </c>
       <c r="E82" s="85" t="s">
@@ -15887,7 +15892,7 @@
       <c r="I82" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J82" s="211" t="s">
+      <c r="J82" s="210" t="s">
         <v>604</v>
       </c>
       <c r="K82" s="27">
@@ -15908,13 +15913,13 @@
       <c r="C83" s="92" t="s">
         <v>438</v>
       </c>
-      <c r="D83" s="214"/>
+      <c r="D83" s="224"/>
       <c r="E83" s="85"/>
       <c r="F83" s="98"/>
       <c r="G83" s="97"/>
       <c r="H83" s="27"/>
       <c r="I83" s="27"/>
-      <c r="J83" s="220"/>
+      <c r="J83" s="211"/>
       <c r="K83" s="27">
         <v>0</v>
       </c>
@@ -16130,16 +16135,16 @@
       <c r="L90" s="118"/>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A91" s="211" t="s">
+      <c r="A91" s="210" t="s">
         <v>558</v>
       </c>
-      <c r="B91" s="211" t="s">
+      <c r="B91" s="210" t="s">
         <v>593</v>
       </c>
       <c r="C91" s="92" t="s">
         <v>446</v>
       </c>
-      <c r="D91" s="208">
+      <c r="D91" s="222">
         <v>4</v>
       </c>
       <c r="E91" s="85" t="s">
@@ -16151,7 +16156,7 @@
       <c r="G91" s="97"/>
       <c r="H91" s="92"/>
       <c r="I91" s="92"/>
-      <c r="J91" s="211" t="s">
+      <c r="J91" s="210" t="s">
         <v>609</v>
       </c>
       <c r="K91" s="27">
@@ -16163,18 +16168,18 @@
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A92" s="220"/>
-      <c r="B92" s="220"/>
+      <c r="A92" s="211"/>
+      <c r="B92" s="211"/>
       <c r="C92" s="92" t="s">
         <v>447</v>
       </c>
-      <c r="D92" s="214"/>
+      <c r="D92" s="224"/>
       <c r="E92" s="85"/>
       <c r="F92" s="85"/>
       <c r="G92" s="97"/>
       <c r="H92" s="92"/>
       <c r="I92" s="92"/>
-      <c r="J92" s="220"/>
+      <c r="J92" s="211"/>
       <c r="K92" s="27">
         <v>0</v>
       </c>
@@ -16184,16 +16189,16 @@
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A93" s="211" t="s">
+      <c r="A93" s="210" t="s">
         <v>558</v>
       </c>
-      <c r="B93" s="211" t="s">
+      <c r="B93" s="210" t="s">
         <v>594</v>
       </c>
       <c r="C93" s="92" t="s">
         <v>448</v>
       </c>
-      <c r="D93" s="208">
+      <c r="D93" s="222">
         <v>4</v>
       </c>
       <c r="E93" s="85" t="s">
@@ -16205,7 +16210,7 @@
       <c r="G93" s="97"/>
       <c r="H93" s="92"/>
       <c r="I93" s="92"/>
-      <c r="J93" s="211" t="s">
+      <c r="J93" s="210" t="s">
         <v>609</v>
       </c>
       <c r="K93" s="27">
@@ -16217,18 +16222,18 @@
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A94" s="220"/>
-      <c r="B94" s="220"/>
+      <c r="A94" s="211"/>
+      <c r="B94" s="211"/>
       <c r="C94" s="92" t="s">
         <v>449</v>
       </c>
-      <c r="D94" s="214"/>
+      <c r="D94" s="224"/>
       <c r="E94" s="85"/>
       <c r="F94" s="99"/>
       <c r="G94" s="97"/>
       <c r="H94" s="92"/>
       <c r="I94" s="92"/>
-      <c r="J94" s="220"/>
+      <c r="J94" s="211"/>
       <c r="K94" s="27">
         <v>0</v>
       </c>
@@ -16304,7 +16309,7 @@
       <c r="C97" s="92" t="s">
         <v>452</v>
       </c>
-      <c r="D97" s="208">
+      <c r="D97" s="222">
         <v>4</v>
       </c>
       <c r="E97" s="85" t="s">
@@ -16318,7 +16323,7 @@
         <v>490</v>
       </c>
       <c r="I97" s="92"/>
-      <c r="J97" s="211" t="s">
+      <c r="J97" s="210" t="s">
         <v>604</v>
       </c>
       <c r="K97" s="27">
@@ -16337,13 +16342,13 @@
       <c r="C98" s="92" t="s">
         <v>306</v>
       </c>
-      <c r="D98" s="214"/>
+      <c r="D98" s="224"/>
       <c r="E98" s="85"/>
       <c r="F98" s="98"/>
       <c r="G98" s="110"/>
       <c r="H98" s="111"/>
       <c r="I98" s="111"/>
-      <c r="J98" s="220"/>
+      <c r="J98" s="211"/>
       <c r="K98" s="123">
         <v>0</v>
       </c>
@@ -16360,7 +16365,7 @@
       <c r="C99" s="92" t="s">
         <v>312</v>
       </c>
-      <c r="D99" s="208">
+      <c r="D99" s="222">
         <v>4</v>
       </c>
       <c r="E99" s="85" t="s">
@@ -16374,7 +16379,7 @@
         <v>490</v>
       </c>
       <c r="I99" s="92"/>
-      <c r="J99" s="211" t="s">
+      <c r="J99" s="210" t="s">
         <v>604</v>
       </c>
       <c r="K99" s="27">
@@ -16393,13 +16398,13 @@
       <c r="C100" s="92" t="s">
         <v>311</v>
       </c>
-      <c r="D100" s="214"/>
+      <c r="D100" s="224"/>
       <c r="E100" s="85"/>
       <c r="F100" s="98"/>
       <c r="G100" s="110"/>
       <c r="H100" s="111"/>
       <c r="I100" s="92"/>
-      <c r="J100" s="220"/>
+      <c r="J100" s="211"/>
       <c r="K100" s="27">
         <v>0</v>
       </c>
@@ -16449,7 +16454,7 @@
       <c r="C102" s="114" t="s">
         <v>302</v>
       </c>
-      <c r="D102" s="221">
+      <c r="D102" s="216">
         <v>4</v>
       </c>
       <c r="E102" s="115" t="s">
@@ -16463,7 +16468,7 @@
         <v>490</v>
       </c>
       <c r="I102" s="114"/>
-      <c r="J102" s="231" t="s">
+      <c r="J102" s="208" t="s">
         <v>604</v>
       </c>
       <c r="K102" s="124">
@@ -16482,13 +16487,13 @@
       <c r="C103" s="114" t="s">
         <v>303</v>
       </c>
-      <c r="D103" s="222"/>
+      <c r="D103" s="217"/>
       <c r="E103" s="115"/>
       <c r="F103" s="116"/>
       <c r="G103" s="117"/>
       <c r="H103" s="114"/>
       <c r="I103" s="114"/>
-      <c r="J103" s="232"/>
+      <c r="J103" s="209"/>
       <c r="K103" s="124">
         <v>0</v>
       </c>
@@ -16505,7 +16510,7 @@
       <c r="C104" s="114" t="s">
         <v>304</v>
       </c>
-      <c r="D104" s="221">
+      <c r="D104" s="216">
         <v>4</v>
       </c>
       <c r="E104" s="115" t="s">
@@ -16519,7 +16524,7 @@
         <v>490</v>
       </c>
       <c r="I104" s="114"/>
-      <c r="J104" s="231" t="s">
+      <c r="J104" s="208" t="s">
         <v>604</v>
       </c>
       <c r="K104" s="124">
@@ -16538,13 +16543,13 @@
       <c r="C105" s="114" t="s">
         <v>305</v>
       </c>
-      <c r="D105" s="222"/>
+      <c r="D105" s="217"/>
       <c r="E105" s="115"/>
       <c r="F105" s="116"/>
       <c r="G105" s="117"/>
       <c r="H105" s="114"/>
       <c r="I105" s="114"/>
-      <c r="J105" s="232"/>
+      <c r="J105" s="209"/>
       <c r="K105" s="124">
         <v>0</v>
       </c>
@@ -16555,37 +16560,41 @@
     </row>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="J104:J105"/>
-    <mergeCell ref="J82:J83"/>
-    <mergeCell ref="J91:J92"/>
-    <mergeCell ref="J93:J94"/>
-    <mergeCell ref="J97:J98"/>
-    <mergeCell ref="J99:J100"/>
-    <mergeCell ref="J102:J103"/>
-    <mergeCell ref="J72:J73"/>
-    <mergeCell ref="J48:J49"/>
-    <mergeCell ref="J50:J51"/>
-    <mergeCell ref="J52:J53"/>
-    <mergeCell ref="J54:J55"/>
-    <mergeCell ref="J56:J57"/>
-    <mergeCell ref="J58:J59"/>
-    <mergeCell ref="J60:J61"/>
-    <mergeCell ref="J62:J63"/>
-    <mergeCell ref="J64:J65"/>
-    <mergeCell ref="J66:J67"/>
-    <mergeCell ref="J70:J71"/>
-    <mergeCell ref="J46:J47"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="J27:J28"/>
-    <mergeCell ref="J29:J30"/>
-    <mergeCell ref="J32:J33"/>
-    <mergeCell ref="J34:J35"/>
-    <mergeCell ref="J36:J37"/>
-    <mergeCell ref="J38:J39"/>
-    <mergeCell ref="J40:J41"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="D3:D10"/>
+    <mergeCell ref="F3:F10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="A91:A92"/>
+    <mergeCell ref="B91:B92"/>
+    <mergeCell ref="D91:D92"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="B93:B94"/>
+    <mergeCell ref="D93:D94"/>
+    <mergeCell ref="D97:D98"/>
+    <mergeCell ref="D99:D100"/>
     <mergeCell ref="D104:D105"/>
     <mergeCell ref="I3:I10"/>
     <mergeCell ref="J3:J10"/>
@@ -16602,41 +16611,37 @@
     <mergeCell ref="D36:D37"/>
     <mergeCell ref="D38:D39"/>
     <mergeCell ref="D40:D41"/>
-    <mergeCell ref="A93:A94"/>
-    <mergeCell ref="B93:B94"/>
-    <mergeCell ref="D93:D94"/>
-    <mergeCell ref="D97:D98"/>
-    <mergeCell ref="D99:D100"/>
-    <mergeCell ref="A91:A92"/>
-    <mergeCell ref="B91:B92"/>
-    <mergeCell ref="D91:D92"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="A3:A10"/>
-    <mergeCell ref="B3:B10"/>
-    <mergeCell ref="D3:D10"/>
-    <mergeCell ref="F3:F10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="J46:J47"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="J27:J28"/>
+    <mergeCell ref="J29:J30"/>
+    <mergeCell ref="J32:J33"/>
+    <mergeCell ref="J34:J35"/>
+    <mergeCell ref="J36:J37"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="J40:J41"/>
+    <mergeCell ref="J72:J73"/>
+    <mergeCell ref="J48:J49"/>
+    <mergeCell ref="J50:J51"/>
+    <mergeCell ref="J52:J53"/>
+    <mergeCell ref="J54:J55"/>
+    <mergeCell ref="J56:J57"/>
+    <mergeCell ref="J58:J59"/>
+    <mergeCell ref="J60:J61"/>
+    <mergeCell ref="J62:J63"/>
+    <mergeCell ref="J64:J65"/>
+    <mergeCell ref="J66:J67"/>
+    <mergeCell ref="J70:J71"/>
+    <mergeCell ref="J104:J105"/>
+    <mergeCell ref="J82:J83"/>
+    <mergeCell ref="J91:J92"/>
+    <mergeCell ref="J93:J94"/>
+    <mergeCell ref="J97:J98"/>
+    <mergeCell ref="J99:J100"/>
+    <mergeCell ref="J102:J103"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16647,8 +16652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76419831-8B11-488C-AE0E-C0CC08014EE6}">
   <dimension ref="A1:Q63"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
@@ -17231,7 +17236,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="58" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="C13" s="27" t="s">
         <v>686</v>
@@ -17277,7 +17282,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="58" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C14" s="27" t="s">
         <v>685</v>
@@ -17705,7 +17710,7 @@
         <v>0.01</v>
       </c>
       <c r="F23" s="96" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="G23" s="97" t="s">
         <v>533</v>
@@ -17731,7 +17736,7 @@
         <v>657</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="D24" s="85">
         <v>4</v>
@@ -18177,7 +18182,7 @@
         <v>559</v>
       </c>
       <c r="C35" s="27" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D35" s="85">
         <v>2</v>
@@ -18210,7 +18215,7 @@
         <v>561</v>
       </c>
       <c r="C36" s="27" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D36" s="85">
         <v>2</v>
@@ -18243,7 +18248,7 @@
         <v>668</v>
       </c>
       <c r="C37" s="27" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D37" s="85">
         <v>4</v>
@@ -18299,7 +18304,7 @@
         <v>669</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D38" s="85">
         <v>4</v>
@@ -18355,7 +18360,7 @@
         <v>568</v>
       </c>
       <c r="C39" s="27" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="D39" s="85">
         <v>2</v>
@@ -18393,7 +18398,7 @@
         <v>570</v>
       </c>
       <c r="C40" s="27" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="D40" s="85">
         <v>2</v>
@@ -18431,7 +18436,7 @@
         <v>571</v>
       </c>
       <c r="C41" s="27" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D41" s="85">
         <v>2</v>
@@ -18469,7 +18474,7 @@
         <v>572</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="D42" s="85">
         <v>2</v>
@@ -18510,7 +18515,7 @@
         <v>573</v>
       </c>
       <c r="C43" s="27" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="D43" s="85">
         <v>2</v>
@@ -18551,7 +18556,7 @@
         <v>574</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D44" s="85">
         <v>2</v>
@@ -18592,7 +18597,7 @@
         <v>575</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="D45" s="85">
         <v>2</v>
@@ -18633,7 +18638,7 @@
         <v>576</v>
       </c>
       <c r="C46" s="164" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="D46" s="165">
         <v>2</v>
@@ -18664,7 +18669,7 @@
         <v>670</v>
       </c>
       <c r="C47" s="27" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="D47" s="85">
         <v>4</v>
@@ -18710,7 +18715,7 @@
         <v>579</v>
       </c>
       <c r="C48" s="164" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="D48" s="165">
         <v>2</v>
@@ -18741,7 +18746,7 @@
         <v>581</v>
       </c>
       <c r="C49" s="164" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="D49" s="165">
         <v>2</v>
@@ -18772,7 +18777,7 @@
         <v>583</v>
       </c>
       <c r="C50" s="27" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="D50" s="85">
         <v>2</v>
@@ -18802,10 +18807,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="59" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C51" s="27" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="D51" s="85">
         <v>2</v>
@@ -18838,7 +18843,7 @@
         <v>587</v>
       </c>
       <c r="C52" s="27" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D52" s="85">
         <v>2</v>
@@ -18871,7 +18876,7 @@
         <v>317</v>
       </c>
       <c r="C53" s="27" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D53" s="85">
         <v>2</v>
@@ -18904,7 +18909,7 @@
         <v>316</v>
       </c>
       <c r="C54" s="27" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="D54" s="85">
         <v>2</v>
@@ -18945,7 +18950,7 @@
         <v>593</v>
       </c>
       <c r="C55" s="27" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="D55" s="85">
         <v>4</v>
@@ -18996,7 +19001,7 @@
         <v>594</v>
       </c>
       <c r="C56" s="27" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="D56" s="85">
         <v>4</v>
@@ -19047,7 +19052,7 @@
         <v>595</v>
       </c>
       <c r="C57" s="164" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="D57" s="165">
         <v>2</v>
@@ -19078,7 +19083,7 @@
         <v>597</v>
       </c>
       <c r="C58" s="27" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="D58" s="85">
         <v>2</v>
@@ -19119,7 +19124,7 @@
         <v>671</v>
       </c>
       <c r="C59" s="27" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="D59" s="85">
         <v>4</v>
@@ -19165,7 +19170,7 @@
         <v>672</v>
       </c>
       <c r="C60" s="27" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="D60" s="85">
         <v>4</v>
@@ -19211,7 +19216,7 @@
         <v>602</v>
       </c>
       <c r="C61" s="27" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="D61" s="136">
         <v>2</v>
@@ -19251,7 +19256,9 @@
       <c r="B62" s="157" t="s">
         <v>673</v>
       </c>
-      <c r="C62" s="160"/>
+      <c r="C62" s="160" t="s">
+        <v>923</v>
+      </c>
       <c r="D62" s="158">
         <v>4</v>
       </c>
@@ -19296,7 +19303,7 @@
         <v>673</v>
       </c>
       <c r="C63" s="160" t="s">
-        <v>708</v>
+        <v>924</v>
       </c>
       <c r="D63" s="158">
         <v>4</v>
@@ -19347,7 +19354,7 @@
   <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
@@ -19364,7 +19371,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" ht="62.4" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -19380,20 +19387,20 @@
     <row r="2" spans="1:13" s="91" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A2" s="92"/>
       <c r="B2" s="92" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C2" s="172"/>
       <c r="D2" s="173" t="s">
+        <v>862</v>
+      </c>
+      <c r="E2" s="85" t="s">
+        <v>742</v>
+      </c>
+      <c r="F2" s="174" t="s">
+        <v>743</v>
+      </c>
+      <c r="G2" s="95" t="s">
         <v>863</v>
-      </c>
-      <c r="E2" s="85" t="s">
-        <v>743</v>
-      </c>
-      <c r="F2" s="174" t="s">
-        <v>744</v>
-      </c>
-      <c r="G2" s="95" t="s">
-        <v>864</v>
       </c>
       <c r="H2" s="51"/>
       <c r="I2" s="51"/>
@@ -19404,25 +19411,25 @@
     </row>
     <row r="3" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="92" t="s">
+        <v>744</v>
+      </c>
+      <c r="B3" s="92" t="s">
         <v>745</v>
       </c>
-      <c r="B3" s="92" t="s">
-        <v>746</v>
-      </c>
       <c r="C3" s="92" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="D3" s="92" t="s">
         <v>307</v>
       </c>
       <c r="E3" s="85" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="F3" s="99" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="G3" s="96" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="H3" s="92"/>
       <c r="I3" s="92"/>
@@ -19434,22 +19441,22 @@
     <row r="4" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="92"/>
       <c r="B4" s="92" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C4" s="92" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D4" s="92" t="s">
         <v>308</v>
       </c>
       <c r="E4" s="85" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="F4" s="99" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="G4" s="96" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="H4" s="92"/>
       <c r="I4" s="92"/>
@@ -19459,22 +19466,22 @@
     <row r="5" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="92"/>
       <c r="B5" s="92" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C5" s="92" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="D5" s="92" t="s">
         <v>309</v>
       </c>
       <c r="E5" s="85" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="F5" s="99" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="G5" s="96" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="H5" s="92"/>
       <c r="I5" s="92"/>
@@ -19484,22 +19491,22 @@
     <row r="6" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="92"/>
       <c r="B6" s="92" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="C6" s="92" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="D6" s="92" t="s">
         <v>148</v>
       </c>
       <c r="E6" s="85" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F6" s="99" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="G6" s="96" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="H6" s="92"/>
       <c r="I6" s="92"/>
@@ -19509,22 +19516,22 @@
     <row r="7" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="92"/>
       <c r="B7" s="92" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="C7" s="92" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="D7" s="92" t="s">
         <v>151</v>
       </c>
       <c r="E7" s="85" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F7" s="99" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="G7" s="96" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H7" s="92"/>
       <c r="I7" s="92"/>
@@ -19534,22 +19541,22 @@
     <row r="8" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="92"/>
       <c r="B8" s="92" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="C8" s="92" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="D8" s="92" t="s">
         <v>154</v>
       </c>
       <c r="E8" s="85" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F8" s="99" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="G8" s="96" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="H8" s="92"/>
       <c r="I8" s="92"/>
@@ -19559,22 +19566,22 @@
     <row r="9" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="92"/>
       <c r="B9" s="92" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C9" s="92" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D9" s="92" t="s">
         <v>158</v>
       </c>
       <c r="E9" s="85" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F9" s="99" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="G9" s="96" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="H9" s="92"/>
       <c r="I9" s="92"/>
@@ -19584,22 +19591,22 @@
     <row r="10" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="92"/>
       <c r="B10" s="92" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="C10" s="92" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D10" s="92" t="s">
         <v>161</v>
       </c>
       <c r="E10" s="85" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="F10" s="99" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="G10" s="96" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="H10" s="92"/>
       <c r="I10" s="92"/>
@@ -19611,20 +19618,20 @@
     <row r="11" spans="1:13" s="181" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="114"/>
       <c r="B11" s="114" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="C11" s="114" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D11" s="114" t="s">
         <v>165</v>
       </c>
       <c r="E11" s="115" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="F11" s="177"/>
       <c r="G11" s="178" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="H11" s="179"/>
       <c r="I11" s="179"/>
@@ -19636,20 +19643,20 @@
     <row r="12" spans="1:13" s="182" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="114"/>
       <c r="B12" s="114" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="C12" s="114" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="D12" s="114" t="s">
         <v>168</v>
       </c>
       <c r="E12" s="115" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="F12" s="159"/>
       <c r="G12" s="178" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="H12" s="114"/>
       <c r="I12" s="114"/>
@@ -19659,20 +19666,20 @@
     <row r="13" spans="1:13" s="182" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="114"/>
       <c r="B13" s="114" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C13" s="114" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D13" s="114" t="s">
         <v>171</v>
       </c>
       <c r="E13" s="115" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F13" s="159"/>
       <c r="G13" s="178" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="H13" s="114"/>
       <c r="I13" s="114"/>
@@ -19682,14 +19689,14 @@
     <row r="14" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="92"/>
       <c r="B14" s="92" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C14" s="92"/>
       <c r="D14" s="92" t="s">
         <v>173</v>
       </c>
       <c r="E14" s="85" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="F14" s="99"/>
       <c r="G14" s="97"/>
@@ -19701,14 +19708,14 @@
     <row r="15" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="92"/>
       <c r="B15" s="92" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C15" s="92"/>
       <c r="D15" s="92" t="s">
         <v>175</v>
       </c>
       <c r="E15" s="85" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="F15" s="99"/>
       <c r="G15" s="97"/>
@@ -19720,14 +19727,14 @@
     <row r="16" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="92"/>
       <c r="B16" s="92" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C16" s="92"/>
       <c r="D16" s="92" t="s">
         <v>177</v>
       </c>
       <c r="E16" s="85" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="F16" s="99"/>
       <c r="G16" s="97"/>
@@ -19739,14 +19746,14 @@
     <row r="17" spans="1:11" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="92"/>
       <c r="B17" s="92" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C17" s="92"/>
       <c r="D17" s="92" t="s">
         <v>179</v>
       </c>
       <c r="E17" s="85" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="F17" s="99"/>
       <c r="G17" s="97"/>
@@ -19758,14 +19765,14 @@
     <row r="18" spans="1:11" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="92"/>
       <c r="B18" s="92" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C18" s="92"/>
       <c r="D18" s="92" t="s">
         <v>181</v>
       </c>
       <c r="E18" s="85" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F18" s="99"/>
       <c r="G18" s="97"/>
@@ -19776,26 +19783,26 @@
     </row>
     <row r="19" spans="1:11" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="92" t="s">
+        <v>761</v>
+      </c>
+      <c r="B19" s="92" t="s">
         <v>762</v>
       </c>
-      <c r="B19" s="92" t="s">
-        <v>763</v>
-      </c>
       <c r="C19" s="92" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="D19" s="92" t="s">
         <v>185</v>
       </c>
       <c r="E19" s="85" t="s">
+        <v>803</v>
+      </c>
+      <c r="F19" s="99" t="s">
         <v>804</v>
-      </c>
-      <c r="F19" s="99" t="s">
-        <v>805</v>
       </c>
       <c r="G19" s="97"/>
       <c r="H19" s="92" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="I19" s="92"/>
       <c r="J19" s="92"/>
@@ -19804,23 +19811,23 @@
     <row r="20" spans="1:11" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="92"/>
       <c r="B20" s="92" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="C20" s="92" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="D20" s="92" t="s">
         <v>190</v>
       </c>
       <c r="E20" s="85" t="s">
+        <v>806</v>
+      </c>
+      <c r="F20" s="99" t="s">
         <v>807</v>
-      </c>
-      <c r="F20" s="99" t="s">
-        <v>808</v>
       </c>
       <c r="G20" s="97"/>
       <c r="H20" s="92" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="I20" s="92"/>
       <c r="J20" s="92"/>
@@ -19829,23 +19836,23 @@
     <row r="21" spans="1:11" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="92"/>
       <c r="B21" s="92" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C21" s="92" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="D21" s="92" t="s">
         <v>195</v>
       </c>
       <c r="E21" s="85" t="s">
+        <v>809</v>
+      </c>
+      <c r="F21" s="99" t="s">
         <v>810</v>
-      </c>
-      <c r="F21" s="99" t="s">
-        <v>811</v>
       </c>
       <c r="G21" s="97"/>
       <c r="H21" s="92" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="I21" s="92"/>
       <c r="J21" s="92"/>
@@ -19854,23 +19861,23 @@
     <row r="22" spans="1:11" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="92"/>
       <c r="B22" s="92" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C22" s="92" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="D22" s="92" t="s">
         <v>199</v>
       </c>
       <c r="E22" s="85" t="s">
+        <v>812</v>
+      </c>
+      <c r="F22" s="99" t="s">
         <v>813</v>
-      </c>
-      <c r="F22" s="99" t="s">
-        <v>814</v>
       </c>
       <c r="G22" s="97"/>
       <c r="H22" s="92" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="I22" s="92"/>
       <c r="J22" s="92"/>
@@ -19879,25 +19886,25 @@
     <row r="23" spans="1:11" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="92"/>
       <c r="B23" s="92" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="C23" s="92" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="D23" s="92" t="s">
         <v>204</v>
       </c>
       <c r="E23" s="85" t="s">
+        <v>815</v>
+      </c>
+      <c r="F23" s="99" t="s">
         <v>816</v>
-      </c>
-      <c r="F23" s="99" t="s">
-        <v>817</v>
       </c>
       <c r="G23" s="97" t="s">
         <v>207</v>
       </c>
       <c r="H23" s="92" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="I23" s="92"/>
       <c r="J23" s="92"/>
@@ -19906,25 +19913,25 @@
     <row r="24" spans="1:11" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="92"/>
       <c r="B24" s="92" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="C24" s="92" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="D24" s="92" t="s">
         <v>210</v>
       </c>
       <c r="E24" s="85" t="s">
+        <v>818</v>
+      </c>
+      <c r="F24" s="99" t="s">
         <v>819</v>
-      </c>
-      <c r="F24" s="99" t="s">
-        <v>820</v>
       </c>
       <c r="G24" s="97" t="s">
         <v>207</v>
       </c>
       <c r="H24" s="92" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="I24" s="92"/>
       <c r="J24" s="92"/>
@@ -19933,19 +19940,19 @@
     <row r="25" spans="1:11" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="92"/>
       <c r="B25" s="92" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="C25" s="92" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="D25" s="92" t="s">
         <v>214</v>
       </c>
       <c r="E25" s="85" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="F25" s="99" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="G25" s="97"/>
       <c r="H25" s="92"/>
@@ -19956,22 +19963,22 @@
     <row r="26" spans="1:11" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="92"/>
       <c r="B26" s="92" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="C26" s="92" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="D26" s="92" t="s">
         <v>217</v>
       </c>
       <c r="E26" s="85" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="F26" s="99" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="G26" s="27" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="H26" s="92"/>
       <c r="I26" s="92"/>
@@ -19981,22 +19988,22 @@
     <row r="27" spans="1:11" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="92"/>
       <c r="B27" s="92" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="C27" s="92" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="D27" s="92" t="s">
         <v>222</v>
       </c>
       <c r="E27" s="85" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="F27" s="99" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="G27" s="27" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="H27" s="92"/>
       <c r="I27" s="92"/>
@@ -20005,22 +20012,22 @@
     </row>
     <row r="28" spans="1:11" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="92" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C28" s="92" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="D28" s="92" t="s">
         <v>226</v>
       </c>
       <c r="E28" s="85" t="s">
+        <v>825</v>
+      </c>
+      <c r="F28" s="99" t="s">
         <v>826</v>
       </c>
-      <c r="F28" s="99" t="s">
-        <v>827</v>
-      </c>
       <c r="G28" s="27" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="I28" s="92"/>
       <c r="J28" s="92"/>
@@ -20028,22 +20035,22 @@
     </row>
     <row r="29" spans="1:11" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="92" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="C29" s="92" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="D29" s="92" t="s">
         <v>230</v>
       </c>
       <c r="E29" s="85" t="s">
+        <v>828</v>
+      </c>
+      <c r="F29" s="99" t="s">
         <v>829</v>
       </c>
-      <c r="F29" s="99" t="s">
-        <v>830</v>
-      </c>
       <c r="G29" s="27" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="I29" s="92"/>
       <c r="J29" s="92"/>
@@ -20052,22 +20059,22 @@
     <row r="30" spans="1:11" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="92"/>
       <c r="B30" s="92" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="C30" s="92" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="D30" s="92" t="s">
         <v>234</v>
       </c>
       <c r="E30" s="85" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="F30" s="99" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="G30" s="27" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="H30" s="92"/>
       <c r="I30" s="92"/>
@@ -20077,16 +20084,16 @@
     <row r="31" spans="1:11" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="92"/>
       <c r="B31" s="92" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C31" s="92" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="D31" s="92" t="s">
         <v>236</v>
       </c>
       <c r="E31" s="85" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="F31" s="99"/>
       <c r="G31" s="97"/>
@@ -20098,16 +20105,16 @@
     <row r="32" spans="1:11" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="92"/>
       <c r="B32" s="92" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C32" s="92" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="D32" s="92" t="s">
         <v>238</v>
       </c>
       <c r="E32" s="85" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="F32" s="99"/>
       <c r="G32" s="97"/>
@@ -20119,16 +20126,16 @@
     <row r="33" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="92"/>
       <c r="B33" s="92" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C33" s="92" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="D33" s="92" t="s">
         <v>240</v>
       </c>
       <c r="E33" s="85" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="F33" s="99"/>
       <c r="G33" s="97"/>
@@ -20140,16 +20147,16 @@
     <row r="34" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="92"/>
       <c r="B34" s="92" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C34" s="92" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="D34" s="92" t="s">
         <v>242</v>
       </c>
       <c r="E34" s="85" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="F34" s="99"/>
       <c r="G34" s="97"/>
@@ -20160,25 +20167,25 @@
     </row>
     <row r="35" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="92" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="B35" s="92" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="C35" s="92" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="D35" s="92" t="s">
         <v>246</v>
       </c>
       <c r="E35" s="85" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="F35" s="99" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="G35" s="96" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="H35" s="92"/>
       <c r="I35" s="92"/>
@@ -20190,22 +20197,22 @@
     <row r="36" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="92"/>
       <c r="B36" s="92" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="C36" s="92" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="D36" s="92" t="s">
         <v>250</v>
       </c>
       <c r="E36" s="85" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="F36" s="99" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="G36" s="96" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="H36" s="92"/>
       <c r="I36" s="92"/>
@@ -20215,22 +20222,22 @@
     <row r="37" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="92"/>
       <c r="B37" s="183" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="C37" s="183" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="D37" s="92" t="s">
         <v>253</v>
       </c>
       <c r="E37" s="85" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="F37" s="183" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="G37" s="105" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="H37" s="92"/>
       <c r="I37" s="92"/>
@@ -20240,22 +20247,22 @@
     <row r="38" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="92"/>
       <c r="B38" s="183" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="C38" s="183" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="D38" s="92" t="s">
         <v>256</v>
       </c>
       <c r="E38" s="85" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="F38" s="183" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="G38" s="105" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="H38" s="92"/>
       <c r="I38" s="92"/>
@@ -20265,22 +20272,22 @@
     <row r="39" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="92"/>
       <c r="B39" s="183" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="C39" s="183" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="D39" s="92" t="s">
         <v>259</v>
       </c>
       <c r="E39" s="85" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="F39" s="183" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="G39" s="105" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="H39" s="92"/>
       <c r="I39" s="92"/>
@@ -20290,22 +20297,22 @@
     <row r="40" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="92"/>
       <c r="B40" s="183" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="C40" s="183" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="D40" s="92" t="s">
         <v>262</v>
       </c>
       <c r="E40" s="85" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="F40" s="183" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="G40" s="105" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="H40" s="92"/>
       <c r="I40" s="92"/>
@@ -20315,22 +20322,22 @@
     <row r="41" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="92"/>
       <c r="B41" s="183" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="C41" s="183" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D41" s="92" t="s">
         <v>362</v>
       </c>
       <c r="E41" s="85" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="F41" s="183" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="G41" s="105" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="H41" s="92"/>
       <c r="I41" s="92"/>
@@ -20340,22 +20347,22 @@
     <row r="42" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="92"/>
       <c r="B42" s="65" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C42" s="65" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D42" s="92" t="s">
         <v>361</v>
       </c>
       <c r="E42" s="85" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="F42" s="99" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="G42" s="105" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="H42" s="92"/>
       <c r="I42" s="92"/>
@@ -20365,22 +20372,22 @@
     <row r="43" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="92"/>
       <c r="B43" s="65" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="C43" s="65" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="D43" s="92" t="s">
         <v>360</v>
       </c>
       <c r="E43" s="85" t="s">
+        <v>852</v>
+      </c>
+      <c r="F43" s="99" t="s">
         <v>853</v>
       </c>
-      <c r="F43" s="99" t="s">
-        <v>854</v>
-      </c>
       <c r="G43" s="105" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="H43" s="92"/>
       <c r="I43" s="92"/>
@@ -20390,22 +20397,22 @@
     <row r="44" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="92"/>
       <c r="B44" s="176" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="C44" s="176" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="D44" s="92" t="s">
         <v>359</v>
       </c>
       <c r="E44" s="85" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="F44" s="99" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="G44" s="105" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="H44" s="92"/>
       <c r="I44" s="92"/>
@@ -20415,22 +20422,22 @@
     <row r="45" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="92"/>
       <c r="B45" s="176" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="C45" s="176" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="D45" s="92" t="s">
         <v>358</v>
       </c>
       <c r="E45" s="85" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="F45" s="99" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="G45" s="105" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="H45" s="92"/>
       <c r="I45" s="92"/>
@@ -20440,22 +20447,22 @@
     <row r="46" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="92"/>
       <c r="B46" s="176" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="C46" s="176" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="D46" s="92" t="s">
         <v>357</v>
       </c>
       <c r="E46" s="85" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="F46" s="99" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="G46" s="105" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="H46" s="92"/>
       <c r="I46" s="92"/>
@@ -20465,22 +20472,22 @@
     <row r="47" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="92"/>
       <c r="B47" s="176" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="C47" s="176" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="D47" s="92" t="s">
         <v>356</v>
       </c>
       <c r="E47" s="85" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="F47" s="99" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="G47" s="105" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="H47" s="92"/>
       <c r="I47" s="92"/>
@@ -20490,22 +20497,22 @@
     <row r="48" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="92"/>
       <c r="B48" s="176" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="C48" s="176" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D48" s="92" t="s">
         <v>355</v>
       </c>
       <c r="E48" s="85" t="s">
+        <v>858</v>
+      </c>
+      <c r="F48" s="99" t="s">
         <v>859</v>
       </c>
-      <c r="F48" s="99" t="s">
-        <v>860</v>
-      </c>
       <c r="G48" s="105" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="H48" s="92"/>
       <c r="I48" s="92"/>
@@ -20515,14 +20522,14 @@
     <row r="49" spans="1:11" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="92"/>
       <c r="B49" s="92" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="C49" s="92"/>
       <c r="D49" s="92" t="s">
         <v>354</v>
       </c>
       <c r="E49" s="85" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="F49" s="99"/>
       <c r="G49" s="97"/>
@@ -20534,14 +20541,14 @@
     <row r="50" spans="1:11" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="92"/>
       <c r="B50" s="92" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="C50" s="92"/>
       <c r="D50" s="92" t="s">
         <v>353</v>
       </c>
       <c r="E50" s="85" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="F50" s="99"/>
       <c r="G50" s="97"/>

</xml_diff>